<commit_message>
update data as of 17 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FFE655-08F2-C64D-B737-2463CF4441C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA05CB0-2611-0E4E-A940-BF4226604CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="960" windowWidth="27480" windowHeight="17040" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
+    <workbookView xWindow="10020" yWindow="960" windowWidth="27480" windowHeight="17040" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -581,9 +581,6 @@
     <t>NICases</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Deaths</t>
   </si>
   <si>
@@ -612,13 +609,16 @@
   </si>
   <si>
     <t>UKRecovered</t>
+  </si>
+  <si>
+    <t>Nation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -647,17 +647,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="4"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="2">
@@ -687,10 +686,10 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,24 +1010,24 @@
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.83203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="4"/>
     <col min="8" max="8" width="19.83203125" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="5"/>
-    <col min="10" max="10" width="10.83203125" style="7"/>
+    <col min="10" max="10" width="10.83203125" style="6"/>
     <col min="11" max="11" width="20.83203125" style="4" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" style="4"/>
     <col min="16" max="16" width="24.83203125" style="4" customWidth="1"/>
     <col min="17" max="18" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13">
       <c r="E1" s="1" t="s">
         <v>150</v>
       </c>
@@ -1042,764 +1041,764 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>355</v>
-      </c>
-      <c r="D2" s="7" t="str">
+        <v>371</v>
+      </c>
+      <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>355,</v>
+        <v>371,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>355</v>
+        <v>371</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>6499</v>
-      </c>
-      <c r="J2" s="7" t="str">
+        <v>6859</v>
+      </c>
+      <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>6499,</v>
+        <v>6859,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>4611</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1001</v>
-      </c>
-      <c r="D3" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1001,</v>
+        <v>1035</v>
+      </c>
+      <c r="D3" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1035,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1001</v>
+        <v>1035</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>19511</v>
-      </c>
-      <c r="J3" s="7" t="str">
-        <f t="shared" ref="J3:J25" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>19511,</v>
+        <v>20215</v>
+      </c>
+      <c r="J3" s="6" t="str">
+        <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
+        <v>20215,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>6499</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+        <v>6859</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>415</v>
-      </c>
-      <c r="D4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>415,</v>
+        <v>433</v>
+      </c>
+      <c r="D4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>433,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>12956</v>
-      </c>
-      <c r="J4" s="7" t="str">
+        <v>13498</v>
+      </c>
+      <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12956,</v>
+        <v>13498,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>19511</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+        <v>20215</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>139</v>
-      </c>
-      <c r="D5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>139,</v>
+        <v>156</v>
+      </c>
+      <c r="D5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>156,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>10633</v>
-      </c>
-      <c r="J5" s="7" t="str">
+        <v>11211</v>
+      </c>
+      <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10633,</v>
+        <v>11211,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>4694</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+        <v>4957</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>244</v>
-      </c>
-      <c r="D6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>244,</v>
+        <v>268</v>
+      </c>
+      <c r="D6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>268,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>12093</v>
-      </c>
-      <c r="J6" s="7" t="str">
+        <v>12687</v>
+      </c>
+      <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12093,</v>
+        <v>12687,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>12093</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+        <v>12687</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>462</v>
-      </c>
-      <c r="D7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>462,</v>
+        <v>480</v>
+      </c>
+      <c r="D7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>480,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>10919</v>
-      </c>
-      <c r="J7" s="7" t="str">
+        <v>11471</v>
+      </c>
+      <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10919,</v>
+        <v>11471,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>10919</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+        <v>11471</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>1982</v>
-      </c>
-      <c r="D8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1982,</v>
+        <v>2064</v>
+      </c>
+      <c r="D8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2064,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>1982</v>
+        <v>2064</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>3913</v>
-      </c>
-      <c r="J8" s="7" t="str">
+        <v>4222</v>
+      </c>
+      <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>3913,</v>
+        <v>4222,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>3913</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+        <v>4222</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>188</v>
-      </c>
-      <c r="D9" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>188,</v>
+        <v>204</v>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>204,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>2965</v>
-      </c>
-      <c r="J9" s="7" t="str">
+        <v>3311</v>
+      </c>
+      <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>2965,</v>
+        <v>3311,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>8345</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+        <v>8718</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>190</v>
-      </c>
-      <c r="D10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>190,</v>
+        <v>198</v>
+      </c>
+      <c r="D10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>198,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>79489</v>
-      </c>
-      <c r="J10" s="7" t="str">
+        <v>83474</v>
+      </c>
+      <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>79489</v>
+        <v>83474</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>5939</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+        <v>6254</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>447</v>
-      </c>
-      <c r="D11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>447,</v>
+        <v>482</v>
+      </c>
+      <c r="D11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>482,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>259</v>
-      </c>
-      <c r="D12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>259,</v>
+        <v>281</v>
+      </c>
+      <c r="D12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>281,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>139</v>
-      </c>
-      <c r="D13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>139,</v>
+        <v>143</v>
+      </c>
+      <c r="D13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>143,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>151</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>460</v>
-      </c>
-      <c r="D14" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>460,</v>
+        <v>476</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>476,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>460</v>
+        <v>476</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>79489</v>
-      </c>
-      <c r="J14" s="7" t="str">
+        <v>83474</v>
+      </c>
+      <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>79489,</v>
+        <v>83474,</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>79489</v>
+        <v>83474</v>
       </c>
       <c r="M14" s="3">
-        <v>12395</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+        <v>13133</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1086</v>
-      </c>
-      <c r="D15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1086,</v>
+        <v>1126</v>
+      </c>
+      <c r="D15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1126,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1086</v>
+        <v>1126</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>7102</v>
-      </c>
-      <c r="J15" s="7" t="str">
+        <v>7409</v>
+      </c>
+      <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>7102,</v>
+        <v>7409,</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>2201</v>
+        <v>2338</v>
       </c>
       <c r="M15" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>233</v>
-      </c>
-      <c r="D16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>233,</v>
+        <v>268</v>
+      </c>
+      <c r="D16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>268,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>233</v>
+        <v>268</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>6401</v>
-      </c>
-      <c r="J16" s="7" t="str">
+        <v>6645</v>
+      </c>
+      <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6401,</v>
+        <v>6645,</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>7102</v>
+        <v>7409</v>
       </c>
       <c r="M16" s="2">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>374</v>
-      </c>
-      <c r="D17" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>374,</v>
+        <v>413</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>413,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>374</v>
+        <v>413</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>2201</v>
-      </c>
-      <c r="J17" s="7" t="str">
+        <v>2338</v>
+      </c>
+      <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>2201</v>
+        <v>2338</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>6401</v>
+        <v>6645</v>
       </c>
       <c r="M17" s="2">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>815</v>
-      </c>
-      <c r="D18" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>815,</v>
+        <v>842</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>842,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>542</v>
-      </c>
-      <c r="D19" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>542,</v>
+        <v>565</v>
+      </c>
+      <c r="D19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>565,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>262</v>
-      </c>
-      <c r="D20" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>262,</v>
+        <v>272</v>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>272,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="18" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="18">
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>168</v>
-      </c>
-      <c r="D21" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>168,</v>
+        <v>177</v>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>177,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="H21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>327608</v>
-      </c>
-      <c r="J21" s="7" t="str">
+        <v>341551</v>
+      </c>
+      <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>327608,</v>
-      </c>
-      <c r="K21" s="6">
-        <v>327608</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+        <v>341551,</v>
+      </c>
+      <c r="K21" s="9">
+        <v>341551</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>441</v>
-      </c>
-      <c r="D22" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>441,</v>
+        <v>453</v>
+      </c>
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>453,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="H22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I22" s="5">
-        <f>K21-K23</f>
-        <v>224515</v>
-      </c>
-      <c r="J22" s="7" t="str">
+        <f>I21-I23</f>
+        <v>232859</v>
+      </c>
+      <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>224515,</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" ht="18" x14ac:dyDescent="0.2">
+        <v>232859,</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="18">
       <c r="B23" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>455</v>
-      </c>
-      <c r="D23" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>455,</v>
+        <v>474</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>474,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>455</v>
+        <v>474</v>
       </c>
       <c r="H23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>103093</v>
-      </c>
-      <c r="J23" s="7" t="str">
+        <v>108692</v>
+      </c>
+      <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>103093,</v>
-      </c>
-      <c r="K23" s="6">
-        <v>103093</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" ht="18" x14ac:dyDescent="0.2">
+        <v>108692,</v>
+      </c>
+      <c r="K23" s="9">
+        <v>108692</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="18">
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>309</v>
-      </c>
-      <c r="D24" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>309,</v>
+        <v>335</v>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>335,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>309</v>
+        <v>335</v>
       </c>
       <c r="H24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>13729</v>
-      </c>
-      <c r="J24" s="7" t="str">
+        <v>14576</v>
+      </c>
+      <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13729,</v>
-      </c>
-      <c r="K24" s="6">
-        <v>13729</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+        <v>14576,</v>
+      </c>
+      <c r="K24" s="9">
+        <v>14576</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>477</v>
-      </c>
-      <c r="D25" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>477,</v>
+        <v>506</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>506,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>477</v>
+        <v>506</v>
       </c>
       <c r="H25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I25" s="5">
         <f>K25</f>
         <v>135</v>
       </c>
-      <c r="J25" s="7" t="str">
+      <c r="J25" s="6" t="str">
         <f>_xlfn.CONCAT(I25)</f>
         <v>135</v>
       </c>
@@ -1807,36 +1806,36 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13">
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>473</v>
-      </c>
-      <c r="D26" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>473,</v>
+        <v>497</v>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>497,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>349</v>
-      </c>
-      <c r="D27" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>349,</v>
+        <v>360</v>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>360,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1845,502 +1844,502 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13">
       <c r="B28" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>770</v>
-      </c>
-      <c r="D28" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>770,</v>
+        <v>829</v>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>829,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>459</v>
-      </c>
-      <c r="D29" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>459,</v>
+        <v>474</v>
+      </c>
+      <c r="D29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>474,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="2">
-        <v>770</v>
-      </c>
-      <c r="H29" s="8">
+        <v>829</v>
+      </c>
+      <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43937</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+        <v>43938</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
       <c r="B30" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1050</v>
-      </c>
-      <c r="D30" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1050,</v>
+        <v>1082</v>
+      </c>
+      <c r="D30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1082,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>459</v>
-      </c>
-      <c r="H30" s="9" t="str">
+        <v>474</v>
+      </c>
+      <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 16/04/2020,327608,224515,103093,13729,135</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+        <v>9:00 17/04/2020,341551,232859,108692,14576,135</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
       <c r="B31" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1345</v>
-      </c>
-      <c r="D31" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1345,</v>
+        <v>1403</v>
+      </c>
+      <c r="D31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1403,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1050</v>
-      </c>
-      <c r="H31" s="9" t="str">
+        <v>1082</v>
+      </c>
+      <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 16/04/2020,79489,7102,6401,2201</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+        <v>9:00 17/04/2020,83474,7409,6645,2338</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>157</v>
-      </c>
-      <c r="D32" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>157,</v>
+        <v>169</v>
+      </c>
+      <c r="D32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>169,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1345</v>
-      </c>
-      <c r="H32" s="9" t="str">
+        <v>1403</v>
+      </c>
+      <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 16/04/2020,6499,19511,12956,10633,12093,10919,3913,2965,79489</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+        <v>9:00 17/04/2020,6859,20215,13498,11211,12687,11471,4222,3311,83474</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
       <c r="B33" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>379</v>
-      </c>
-      <c r="D33" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>379,</v>
+        <v>384</v>
+      </c>
+      <c r="D33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>384,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>157</v>
-      </c>
-      <c r="H33" s="9" t="str">
+        <v>169</v>
+      </c>
+      <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 16/04/2020,355,1001,415,139,244,462,1982,188,190,447,259,139,460,1086,233,374,815,542,262,168,441,455,309,477,473,349,770,459,1050,1345,157,379,803,460,239,212,490,802,272,383,570,1647,492,768,509,537,227,405,1858,428,696,79,505,127,1609,554,509,55,337,376,1958,175,317,381,339,950,1769,743,427,581,732,531,1010,387,744,428,526,325,331,638,809,786,86,142,127,339,542,784,502,339,755,378,1015,113,176,200,246,548,195,297,278,407,12,379,624,560,1412,287,262,372,248,223,251,301,229,1001,407,1051,549,217,240,527,729,1739,500,200,320,143,207,107,517,402,344,609,586,766,372,742,186,679,510,354,271,163,623,201,501,718,153,2965</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+        <v>9:00 17/04/2020,371,1035,433,156,268,480,2064,204,198,482,281,143,476,1126,268,413,842,565,272,177,453,474,335,506,497,360,829,474,1082,1403,169,384,840,471,247,225,518,831,300,396,616,1721,513,825,533,550,230,417,1941,472,724,79,524,129,1695,571,530,58,352,389,2108,201,330,395,357,970,1842,784,442,609,752,551,1028,428,788,441,543,346,344,670,834,842,89,154,141,356,564,801,530,352,789,395,1070,120,189,217,263,566,202,304,291,429,12,392,660,578,1474,299,270,399,274,247,277,317,239,1026,427,1102,579,225,258,545,761,1771,519,236,338,147,213,110,535,424,371,627,606,786,393,761,188,735,525,375,294,166,688,210,518,762,160,3311</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
       <c r="B34" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>803</v>
-      </c>
-      <c r="D34" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>803,</v>
+        <v>840</v>
+      </c>
+      <c r="D34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>840,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
       <c r="B35" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>460</v>
-      </c>
-      <c r="D35" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>460,</v>
+        <v>471</v>
+      </c>
+      <c r="D35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>471,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="2">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
       <c r="B36" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>239</v>
-      </c>
-      <c r="D36" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>239,</v>
+        <v>247</v>
+      </c>
+      <c r="D36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>247,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>212</v>
-      </c>
-      <c r="D37" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>212,</v>
+        <v>225</v>
+      </c>
+      <c r="D37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>225,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>490</v>
-      </c>
-      <c r="D38" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>490,</v>
+        <v>518</v>
+      </c>
+      <c r="D38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>518,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
       <c r="B39" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>802</v>
-      </c>
-      <c r="D39" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>802,</v>
+        <v>831</v>
+      </c>
+      <c r="D39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>831,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
       <c r="B40" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>272</v>
-      </c>
-      <c r="D40" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>272,</v>
+        <v>300</v>
+      </c>
+      <c r="D40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>300,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
       <c r="B41" t="s">
         <v>39</v>
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>383</v>
-      </c>
-      <c r="D41" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>383,</v>
+        <v>396</v>
+      </c>
+      <c r="D41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>396,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
       <c r="B42" t="s">
         <v>40</v>
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>570</v>
-      </c>
-      <c r="D42" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>570,</v>
+        <v>616</v>
+      </c>
+      <c r="D42" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>616,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
       <c r="B43" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>1647</v>
-      </c>
-      <c r="D43" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1647,</v>
+        <v>1721</v>
+      </c>
+      <c r="D43" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1721,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
       <c r="B44" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>492</v>
-      </c>
-      <c r="D44" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>492,</v>
+        <v>513</v>
+      </c>
+      <c r="D44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>513,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
       <c r="B45" t="s">
         <v>43</v>
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>768</v>
-      </c>
-      <c r="D45" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>768,</v>
+        <v>825</v>
+      </c>
+      <c r="D45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>825,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
       <c r="B46" t="s">
         <v>44</v>
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>509</v>
-      </c>
-      <c r="D46" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>509,</v>
+        <v>533</v>
+      </c>
+      <c r="D46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>533,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="2">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
       <c r="B47" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>537</v>
-      </c>
-      <c r="D47" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>537,</v>
+        <v>550</v>
+      </c>
+      <c r="D47" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>550,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
       <c r="B48" t="s">
         <v>46</v>
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>227</v>
-      </c>
-      <c r="D48" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>227,</v>
+        <v>230</v>
+      </c>
+      <c r="D48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>230,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
       <c r="B49" t="s">
         <v>47</v>
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>405</v>
-      </c>
-      <c r="D49" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>405,</v>
+        <v>417</v>
+      </c>
+      <c r="D49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>417,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
       <c r="B50" t="s">
         <v>48</v>
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>1858</v>
-      </c>
-      <c r="D50" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1858,</v>
+        <v>1941</v>
+      </c>
+      <c r="D50" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1941,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
       <c r="B51" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>428</v>
-      </c>
-      <c r="D51" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>428,</v>
+        <v>472</v>
+      </c>
+      <c r="D51" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>472,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>1858</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
       <c r="B52" t="s">
         <v>50</v>
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>696</v>
-      </c>
-      <c r="D52" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>696,</v>
+        <v>724</v>
+      </c>
+      <c r="D52" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>724,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
       <c r="B53" t="s">
         <v>51</v>
       </c>
@@ -2348,7 +2347,7 @@
         <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="D53" s="7" t="str">
+      <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>79,</v>
       </c>
@@ -2356,20 +2355,20 @@
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
       <c r="B54" t="s">
         <v>52</v>
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>505</v>
-      </c>
-      <c r="D54" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>505,</v>
+        <v>524</v>
+      </c>
+      <c r="D54" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>524,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
@@ -2378,938 +2377,938 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6">
       <c r="B55" t="s">
         <v>53</v>
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>127</v>
-      </c>
-      <c r="D55" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>127,</v>
+        <v>129</v>
+      </c>
+      <c r="D55" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>129,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
       <c r="B56" t="s">
         <v>54</v>
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1609</v>
-      </c>
-      <c r="D56" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1609,</v>
+        <v>1695</v>
+      </c>
+      <c r="D56" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>1695,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
       <c r="B57" t="s">
         <v>55</v>
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>554</v>
-      </c>
-      <c r="D57" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>554,</v>
+        <v>571</v>
+      </c>
+      <c r="D57" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>571,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
       <c r="B58" t="s">
         <v>56</v>
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>509</v>
-      </c>
-      <c r="D58" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>509,</v>
+        <v>530</v>
+      </c>
+      <c r="D58" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>530,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
       <c r="B59" t="s">
         <v>57</v>
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>55</v>
-      </c>
-      <c r="D59" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>55,</v>
+        <v>58</v>
+      </c>
+      <c r="D59" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>58,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
       <c r="B60" t="s">
         <v>58</v>
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>337</v>
-      </c>
-      <c r="D60" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>337,</v>
+        <v>352</v>
+      </c>
+      <c r="D60" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>352,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
       <c r="B61" t="s">
         <v>59</v>
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>376</v>
-      </c>
-      <c r="D61" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>376,</v>
+        <v>389</v>
+      </c>
+      <c r="D61" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>389,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
       <c r="B62" t="s">
         <v>60</v>
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>1958</v>
-      </c>
-      <c r="D62" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>1958,</v>
+        <v>2108</v>
+      </c>
+      <c r="D62" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2108,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
       <c r="B63" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>175</v>
-      </c>
-      <c r="D63" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>175,</v>
+        <v>201</v>
+      </c>
+      <c r="D63" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>201,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>1958</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
       <c r="B64" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>317</v>
-      </c>
-      <c r="D64" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>317,</v>
+        <v>330</v>
+      </c>
+      <c r="D64" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>330,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
       <c r="B65" t="s">
         <v>63</v>
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>381</v>
-      </c>
-      <c r="D65" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>381,</v>
+        <v>395</v>
+      </c>
+      <c r="D65" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>395,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
       <c r="B66" t="s">
         <v>64</v>
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>339</v>
-      </c>
-      <c r="D66" s="7" t="str">
+        <v>357</v>
+      </c>
+      <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>339,</v>
+        <v>357,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
       <c r="B67" t="s">
         <v>65</v>
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>950</v>
-      </c>
-      <c r="D67" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>950,</v>
+        <v>970</v>
+      </c>
+      <c r="D67" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>970,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
       <c r="B68" t="s">
         <v>66</v>
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>1769</v>
-      </c>
-      <c r="D68" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>1769,</v>
+        <v>1842</v>
+      </c>
+      <c r="D68" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1842,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="2">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
       <c r="B69" t="s">
         <v>67</v>
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>743</v>
-      </c>
-      <c r="D69" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>743,</v>
+        <v>784</v>
+      </c>
+      <c r="D69" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>784,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
       <c r="B70" t="s">
         <v>68</v>
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>427</v>
-      </c>
-      <c r="D70" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>427,</v>
+        <v>442</v>
+      </c>
+      <c r="D70" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>442,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="2">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
       <c r="B71" t="s">
         <v>69</v>
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>581</v>
-      </c>
-      <c r="D71" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>581,</v>
+        <v>609</v>
+      </c>
+      <c r="D71" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>609,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
       <c r="B72" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>732</v>
-      </c>
-      <c r="D72" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>732,</v>
+        <v>752</v>
+      </c>
+      <c r="D72" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>752,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
       <c r="B73" t="s">
         <v>71</v>
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>531</v>
-      </c>
-      <c r="D73" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>531,</v>
+        <v>551</v>
+      </c>
+      <c r="D73" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>551,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
       <c r="B74" t="s">
         <v>72</v>
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1010</v>
-      </c>
-      <c r="D74" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>1010,</v>
+        <v>1028</v>
+      </c>
+      <c r="D74" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1028,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
       <c r="B75" t="s">
         <v>73</v>
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>387</v>
-      </c>
-      <c r="D75" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>387,</v>
+        <v>428</v>
+      </c>
+      <c r="D75" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>428,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
       <c r="B76" t="s">
         <v>74</v>
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>744</v>
-      </c>
-      <c r="D76" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>744,</v>
+        <v>788</v>
+      </c>
+      <c r="D76" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>788,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
       <c r="B77" t="s">
         <v>75</v>
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>428</v>
-      </c>
-      <c r="D77" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>428,</v>
+        <v>441</v>
+      </c>
+      <c r="D77" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>441,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
       <c r="B78" t="s">
         <v>76</v>
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>526</v>
-      </c>
-      <c r="D78" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>526,</v>
+        <v>543</v>
+      </c>
+      <c r="D78" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>543,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6">
       <c r="B79" t="s">
         <v>77</v>
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>325</v>
-      </c>
-      <c r="D79" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>325,</v>
+        <v>346</v>
+      </c>
+      <c r="D79" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>346,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6">
       <c r="B80" t="s">
         <v>78</v>
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>331</v>
-      </c>
-      <c r="D80" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>331,</v>
+        <v>344</v>
+      </c>
+      <c r="D80" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>344,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
       <c r="B81" t="s">
         <v>79</v>
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>638</v>
-      </c>
-      <c r="D81" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>638,</v>
+        <v>670</v>
+      </c>
+      <c r="D81" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>670,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
       <c r="B82" t="s">
         <v>80</v>
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>809</v>
-      </c>
-      <c r="D82" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>809,</v>
+        <v>834</v>
+      </c>
+      <c r="D82" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>834,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
       <c r="B83" t="s">
         <v>81</v>
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>786</v>
-      </c>
-      <c r="D83" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>786,</v>
+        <v>842</v>
+      </c>
+      <c r="D83" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>842,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
       <c r="B84" t="s">
         <v>82</v>
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>86</v>
-      </c>
-      <c r="D84" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>86,</v>
+        <v>89</v>
+      </c>
+      <c r="D84" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>89,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="2">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6">
       <c r="B85" t="s">
         <v>83</v>
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>142</v>
-      </c>
-      <c r="D85" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>142,</v>
+        <v>154</v>
+      </c>
+      <c r="D85" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>154,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
       <c r="B86" t="s">
         <v>84</v>
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>127</v>
-      </c>
-      <c r="D86" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>127,</v>
+        <v>141</v>
+      </c>
+      <c r="D86" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>141,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6">
       <c r="B87" t="s">
         <v>85</v>
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>339</v>
-      </c>
-      <c r="D87" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>339,</v>
+        <v>356</v>
+      </c>
+      <c r="D87" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>356,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6">
       <c r="B88" t="s">
         <v>86</v>
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>542</v>
-      </c>
-      <c r="D88" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>542,</v>
+        <v>564</v>
+      </c>
+      <c r="D88" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>564,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6">
       <c r="B89" t="s">
         <v>87</v>
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>784</v>
-      </c>
-      <c r="D89" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>784,</v>
+        <v>801</v>
+      </c>
+      <c r="D89" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>801,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6">
       <c r="B90" t="s">
         <v>88</v>
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>502</v>
-      </c>
-      <c r="D90" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>502,</v>
+        <v>530</v>
+      </c>
+      <c r="D90" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>530,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6">
       <c r="B91" t="s">
         <v>89</v>
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>339</v>
-      </c>
-      <c r="D91" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>339,</v>
+        <v>352</v>
+      </c>
+      <c r="D91" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>352,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6">
       <c r="B92" t="s">
         <v>90</v>
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>755</v>
-      </c>
-      <c r="D92" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>755,</v>
+        <v>789</v>
+      </c>
+      <c r="D92" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>789,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6">
       <c r="B93" t="s">
         <v>91</v>
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>378</v>
-      </c>
-      <c r="D93" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>378,</v>
+        <v>395</v>
+      </c>
+      <c r="D93" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>395,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6">
       <c r="B94" t="s">
         <v>92</v>
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1015</v>
-      </c>
-      <c r="D94" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>1015,</v>
+        <v>1070</v>
+      </c>
+      <c r="D94" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1070,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6">
       <c r="B95" t="s">
         <v>93</v>
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>113</v>
-      </c>
-      <c r="D95" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>113,</v>
+        <v>120</v>
+      </c>
+      <c r="D95" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>120,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6">
       <c r="B96" t="s">
         <v>94</v>
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>176</v>
-      </c>
-      <c r="D96" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>176,</v>
+        <v>189</v>
+      </c>
+      <c r="D96" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>189,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6">
       <c r="B97" t="s">
         <v>95</v>
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>200</v>
-      </c>
-      <c r="D97" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>200,</v>
+        <v>217</v>
+      </c>
+      <c r="D97" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>217,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6">
       <c r="B98" t="s">
         <v>96</v>
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>246</v>
-      </c>
-      <c r="D98" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>246,</v>
+        <v>263</v>
+      </c>
+      <c r="D98" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>263,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6">
       <c r="B99" t="s">
         <v>97</v>
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>548</v>
-      </c>
-      <c r="D99" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>548,</v>
+        <v>566</v>
+      </c>
+      <c r="D99" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>566,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6">
       <c r="B100" t="s">
         <v>98</v>
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>195</v>
-      </c>
-      <c r="D100" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>195,</v>
+        <v>202</v>
+      </c>
+      <c r="D100" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>202,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6">
       <c r="B101" t="s">
         <v>99</v>
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>297</v>
-      </c>
-      <c r="D101" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>297,</v>
+        <v>304</v>
+      </c>
+      <c r="D101" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>304,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6">
       <c r="B102" t="s">
         <v>100</v>
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>278</v>
-      </c>
-      <c r="D102" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>278,</v>
+        <v>291</v>
+      </c>
+      <c r="D102" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>291,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6">
       <c r="B103" t="s">
         <v>101</v>
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>407</v>
-      </c>
-      <c r="D103" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>407,</v>
+        <v>429</v>
+      </c>
+      <c r="D103" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>429,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -3317,7 +3316,7 @@
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="D104" s="7" t="str">
+      <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
         <v>12,</v>
       </c>
@@ -3325,20 +3324,20 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6">
       <c r="B105" t="s">
         <v>103</v>
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>379</v>
-      </c>
-      <c r="D105" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>379,</v>
+        <v>392</v>
+      </c>
+      <c r="D105" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>392,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3347,878 +3346,878 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:6">
       <c r="B106" t="s">
         <v>104</v>
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>624</v>
-      </c>
-      <c r="D106" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>624,</v>
+        <v>660</v>
+      </c>
+      <c r="D106" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>660,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6">
       <c r="B107" t="s">
         <v>105</v>
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>560</v>
-      </c>
-      <c r="D107" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>560,</v>
+        <v>578</v>
+      </c>
+      <c r="D107" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>578,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6">
       <c r="B108" t="s">
         <v>106</v>
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1412</v>
-      </c>
-      <c r="D108" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>1412,</v>
+        <v>1474</v>
+      </c>
+      <c r="D108" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1474,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6">
       <c r="B109" t="s">
         <v>107</v>
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>287</v>
-      </c>
-      <c r="D109" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>287,</v>
+        <v>299</v>
+      </c>
+      <c r="D109" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>299,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6">
       <c r="B110" t="s">
         <v>108</v>
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>262</v>
-      </c>
-      <c r="D110" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>262,</v>
+        <v>270</v>
+      </c>
+      <c r="D110" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>270,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6">
       <c r="B111" t="s">
         <v>109</v>
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>372</v>
-      </c>
-      <c r="D111" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>372,</v>
+        <v>399</v>
+      </c>
+      <c r="D111" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>399,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6">
       <c r="B112" t="s">
         <v>110</v>
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>248</v>
-      </c>
-      <c r="D112" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>248,</v>
+        <v>274</v>
+      </c>
+      <c r="D112" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>274,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6">
       <c r="B113" t="s">
         <v>111</v>
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>223</v>
-      </c>
-      <c r="D113" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>223,</v>
+        <v>247</v>
+      </c>
+      <c r="D113" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>247,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6">
       <c r="B114" t="s">
         <v>112</v>
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>251</v>
-      </c>
-      <c r="D114" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>251,</v>
+        <v>277</v>
+      </c>
+      <c r="D114" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>277,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6">
       <c r="B115" t="s">
         <v>113</v>
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>301</v>
-      </c>
-      <c r="D115" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>301,</v>
+        <v>317</v>
+      </c>
+      <c r="D115" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>317,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6">
       <c r="B116" t="s">
         <v>114</v>
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>229</v>
-      </c>
-      <c r="D116" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>229,</v>
+        <v>239</v>
+      </c>
+      <c r="D116" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>239,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6">
       <c r="B117" t="s">
         <v>115</v>
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1001</v>
-      </c>
-      <c r="D117" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>1001,</v>
+        <v>1026</v>
+      </c>
+      <c r="D117" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1026,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6">
       <c r="B118" t="s">
         <v>116</v>
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>407</v>
-      </c>
-      <c r="D118" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>407,</v>
+        <v>427</v>
+      </c>
+      <c r="D118" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>427,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6">
       <c r="B119" t="s">
         <v>117</v>
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1051</v>
-      </c>
-      <c r="D119" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>1051,</v>
+        <v>1102</v>
+      </c>
+      <c r="D119" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1102,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6">
       <c r="B120" t="s">
         <v>118</v>
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>549</v>
-      </c>
-      <c r="D120" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>549,</v>
+        <v>579</v>
+      </c>
+      <c r="D120" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>579,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6">
       <c r="B121" t="s">
         <v>119</v>
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>217</v>
-      </c>
-      <c r="D121" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>217,</v>
+        <v>225</v>
+      </c>
+      <c r="D121" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>225,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6">
       <c r="B122" t="s">
         <v>120</v>
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>240</v>
-      </c>
-      <c r="D122" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>240,</v>
+        <v>258</v>
+      </c>
+      <c r="D122" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>258,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6">
       <c r="B123" t="s">
         <v>121</v>
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>527</v>
-      </c>
-      <c r="D123" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>527,</v>
+        <v>545</v>
+      </c>
+      <c r="D123" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>545,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6">
       <c r="B124" t="s">
         <v>122</v>
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>729</v>
-      </c>
-      <c r="D124" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>729,</v>
+        <v>761</v>
+      </c>
+      <c r="D124" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>761,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6">
       <c r="B125" t="s">
         <v>123</v>
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>1739</v>
-      </c>
-      <c r="D125" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>1739,</v>
+        <v>1771</v>
+      </c>
+      <c r="D125" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1771,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="2">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6">
       <c r="B126" t="s">
         <v>124</v>
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>500</v>
-      </c>
-      <c r="D126" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>500,</v>
+        <v>519</v>
+      </c>
+      <c r="D126" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>519,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>1739</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6">
       <c r="B127" t="s">
         <v>125</v>
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>200</v>
-      </c>
-      <c r="D127" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>200,</v>
+        <v>236</v>
+      </c>
+      <c r="D127" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>236,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6">
       <c r="B128" t="s">
         <v>126</v>
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>320</v>
-      </c>
-      <c r="D128" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>320,</v>
+        <v>338</v>
+      </c>
+      <c r="D128" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>338,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6">
       <c r="B129" t="s">
         <v>127</v>
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>143</v>
-      </c>
-      <c r="D129" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>143,</v>
+        <v>147</v>
+      </c>
+      <c r="D129" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>147,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6">
       <c r="B130" t="s">
         <v>128</v>
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>207</v>
-      </c>
-      <c r="D130" s="7" t="str">
-        <f t="shared" ref="D130:D151" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>207,</v>
+        <v>213</v>
+      </c>
+      <c r="D130" s="6" t="str">
+        <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
+        <v>213,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6">
       <c r="B131" t="s">
         <v>129</v>
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>107</v>
-      </c>
-      <c r="D131" s="7" t="str">
+        <v>110</v>
+      </c>
+      <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>107,</v>
+        <v>110,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6">
       <c r="B132" t="s">
         <v>130</v>
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>517</v>
-      </c>
-      <c r="D132" s="7" t="str">
+        <v>535</v>
+      </c>
+      <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>517,</v>
+        <v>535,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6">
       <c r="B133" t="s">
         <v>131</v>
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>402</v>
-      </c>
-      <c r="D133" s="7" t="str">
+        <v>424</v>
+      </c>
+      <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>402,</v>
+        <v>424,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6">
       <c r="B134" t="s">
         <v>132</v>
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>344</v>
-      </c>
-      <c r="D134" s="7" t="str">
+        <v>371</v>
+      </c>
+      <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>344,</v>
+        <v>371,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6">
       <c r="B135" t="s">
         <v>133</v>
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>609</v>
-      </c>
-      <c r="D135" s="7" t="str">
+        <v>627</v>
+      </c>
+      <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>609,</v>
+        <v>627,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6">
       <c r="B136" t="s">
         <v>134</v>
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>586</v>
-      </c>
-      <c r="D136" s="7" t="str">
+        <v>606</v>
+      </c>
+      <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>586,</v>
+        <v>606,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6">
       <c r="B137" t="s">
         <v>135</v>
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>766</v>
-      </c>
-      <c r="D137" s="7" t="str">
+        <v>786</v>
+      </c>
+      <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>766,</v>
+        <v>786,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6">
       <c r="B138" t="s">
         <v>136</v>
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>372</v>
-      </c>
-      <c r="D138" s="7" t="str">
+        <v>393</v>
+      </c>
+      <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>372,</v>
+        <v>393,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6">
       <c r="B139" t="s">
         <v>137</v>
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>742</v>
-      </c>
-      <c r="D139" s="7" t="str">
+        <v>761</v>
+      </c>
+      <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>742,</v>
+        <v>761,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6">
       <c r="B140" t="s">
         <v>138</v>
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>186</v>
-      </c>
-      <c r="D140" s="7" t="str">
+        <v>188</v>
+      </c>
+      <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>186,</v>
+        <v>188,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6">
       <c r="B141" t="s">
         <v>139</v>
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>679</v>
-      </c>
-      <c r="D141" s="7" t="str">
+        <v>735</v>
+      </c>
+      <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>679,</v>
+        <v>735,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6">
       <c r="B142" t="s">
         <v>140</v>
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>510</v>
-      </c>
-      <c r="D142" s="7" t="str">
+        <v>525</v>
+      </c>
+      <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>510,</v>
+        <v>525,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6">
       <c r="B143" t="s">
         <v>141</v>
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>354</v>
-      </c>
-      <c r="D143" s="7" t="str">
+        <v>375</v>
+      </c>
+      <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>354,</v>
+        <v>375,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6">
       <c r="B144" t="s">
         <v>142</v>
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>271</v>
-      </c>
-      <c r="D144" s="7" t="str">
+        <v>294</v>
+      </c>
+      <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>271,</v>
+        <v>294,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6">
       <c r="B145" t="s">
         <v>143</v>
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>163</v>
-      </c>
-      <c r="D145" s="7" t="str">
+        <v>166</v>
+      </c>
+      <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>163,</v>
+        <v>166,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6">
       <c r="B146" t="s">
         <v>144</v>
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>623</v>
-      </c>
-      <c r="D146" s="7" t="str">
+        <v>688</v>
+      </c>
+      <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>623,</v>
+        <v>688,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6">
       <c r="B147" t="s">
         <v>145</v>
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>201</v>
-      </c>
-      <c r="D147" s="7" t="str">
+        <v>210</v>
+      </c>
+      <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>201,</v>
+        <v>210,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6">
       <c r="B148" t="s">
         <v>146</v>
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>501</v>
-      </c>
-      <c r="D148" s="7" t="str">
+        <v>518</v>
+      </c>
+      <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>501,</v>
+        <v>518,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6">
       <c r="B149" t="s">
         <v>147</v>
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>718</v>
-      </c>
-      <c r="D149" s="7" t="str">
+        <v>762</v>
+      </c>
+      <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>718,</v>
+        <v>762,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="150" spans="2:6">
       <c r="B150" t="s">
         <v>148</v>
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>153</v>
-      </c>
-      <c r="D150" s="7" t="str">
+        <v>160</v>
+      </c>
+      <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>153,</v>
+        <v>160,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6">
       <c r="B151" t="s">
         <v>149</v>
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>2965</v>
-      </c>
-      <c r="D151" s="7" t="str">
+        <v>3311</v>
+      </c>
+      <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>2965</v>
+        <v>3311</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 18 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA05CB0-2611-0E4E-A940-BF4226604CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4563F0-40C0-7542-B84E-4B03CC64334D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="960" windowWidth="27480" windowHeight="17040" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>371,</v>
+        <v>383,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>6859</v>
+        <v>7203</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>6859,</v>
+        <v>7203,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>4780</v>
+        <v>4918</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1035</v>
+        <v>1055</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1035,</v>
+        <v>1055,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1035</v>
+        <v>1055</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>20215</v>
+        <v>20904</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>20215,</v>
+        <v>20904,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>6859</v>
+        <v>7203</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>433,</v>
+        <v>444,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>13498</v>
+        <v>13963</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13498,</v>
+        <v>13963,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>20215</v>
+        <v>20904</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>156,</v>
+        <v>161,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>11211</v>
+        <v>11739</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11211,</v>
+        <v>11739,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>4957</v>
+        <v>5115</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>268,</v>
+        <v>282,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>12687</v>
+        <v>13237</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12687,</v>
+        <v>13237,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>12687</v>
+        <v>13237</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>480,</v>
+        <v>491,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>11471</v>
+        <v>11885</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11471,</v>
+        <v>11885,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>11471</v>
+        <v>11885</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2064</v>
+        <v>2133</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2064,</v>
+        <v>2133,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2064</v>
+        <v>2133</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>4222</v>
+        <v>4448</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4222,</v>
+        <v>4448,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>4222</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>204,</v>
+        <v>213,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>3311</v>
+        <v>3643</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>3311,</v>
+        <v>3643,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>8718</v>
+        <v>9045</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>198,</v>
+        <v>209,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>83474</v>
+        <v>87022</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>83474</v>
+        <v>87022</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>6254</v>
+        <v>6624</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>482</v>
+        <v>512</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>482,</v>
+        <v>512,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>482</v>
+        <v>512</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>281,</v>
+        <v>295,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>143,</v>
+        <v>145,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>476</v>
+        <v>546</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>476,</v>
+        <v>546,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>476</v>
+        <v>546</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>83474</v>
+        <v>87022</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>83474,</v>
+        <v>87022,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>83474</v>
+        <v>87022</v>
       </c>
       <c r="M14" s="3">
-        <v>13133</v>
+        <v>13917</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1126</v>
+        <v>1160</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1126,</v>
+        <v>1160,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1126</v>
+        <v>1160</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>7409</v>
+        <v>7820</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>7409,</v>
+        <v>7820,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>2338</v>
+        <v>2486</v>
       </c>
       <c r="M15" s="2">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>268,</v>
+        <v>279,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>6645</v>
+        <v>6936</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6645,</v>
+        <v>6936,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>7409</v>
+        <v>7820</v>
       </c>
       <c r="M16" s="2">
-        <v>779</v>
+        <v>837</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>413</v>
+        <v>438</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>413,</v>
+        <v>438,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>413</v>
+        <v>438</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>2338</v>
+        <v>2486</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>2338</v>
+        <v>2486</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>6645</v>
+        <v>6936</v>
       </c>
       <c r="M17" s="2">
-        <v>506</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>842</v>
+        <v>874</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>842,</v>
+        <v>874,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>842</v>
+        <v>874</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>565</v>
+        <v>577</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>565,</v>
+        <v>577,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>565</v>
+        <v>577</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>272,</v>
+        <v>295,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>272</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>177,</v>
+        <v>183,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>341551</v>
+        <v>357023</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>341551,</v>
+        <v>357023,</v>
       </c>
       <c r="K21" s="9">
-        <v>341551</v>
+        <v>357023</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>453,</v>
+        <v>463,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>232859</v>
+        <v>242806</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>232859,</v>
+        <v>242806,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>474</v>
+        <v>489</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>474,</v>
+        <v>489,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>474</v>
+        <v>489</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>108692</v>
+        <v>114217</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>108692,</v>
+        <v>114217,</v>
       </c>
       <c r="K23" s="9">
-        <v>108692</v>
+        <v>114217</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>335,</v>
+        <v>352,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>14576</v>
+        <v>15464</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14576,</v>
+        <v>15464,</v>
       </c>
       <c r="K24" s="9">
-        <v>14576</v>
+        <v>15464</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>506</v>
+        <v>571</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>506,</v>
+        <v>571,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>506</v>
+        <v>571</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>497</v>
+        <v>525</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>497,</v>
+        <v>525,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>497</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>360,</v>
+        <v>368,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>829</v>
+        <v>857</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>829,</v>
+        <v>857,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>360</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>474</v>
+        <v>487</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>474,</v>
+        <v>487,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="2">
-        <v>829</v>
+        <v>857</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43938</v>
+        <v>43939</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1082</v>
+        <v>1140</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1082,</v>
+        <v>1140,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>474</v>
+        <v>487</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 17/04/2020,341551,232859,108692,14576,135</v>
+        <v>9:00 18/04/2020,357023,242806,114217,15464,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1403</v>
+        <v>1429</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1403,</v>
+        <v>1429,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1082</v>
+        <v>1140</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 17/04/2020,83474,7409,6645,2338</v>
+        <v>9:00 18/04/2020,87022,7820,6936,2486</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1948,11 +1948,11 @@
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1403</v>
+        <v>1429</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 17/04/2020,6859,20215,13498,11211,12687,11471,4222,3311,83474</v>
+        <v>9:00 18/04/2020,7203,20904,13963,11739,13237,11885,4448,3643,87022</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,11 +1961,11 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>384,</v>
+        <v>390,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 17/04/2020,371,1035,433,156,268,480,2064,204,198,482,281,143,476,1126,268,413,842,565,272,177,453,474,335,506,497,360,829,474,1082,1403,169,384,840,471,247,225,518,831,300,396,616,1721,513,825,533,550,230,417,1941,472,724,79,524,129,1695,571,530,58,352,389,2108,201,330,395,357,970,1842,784,442,609,752,551,1028,428,788,441,543,346,344,670,834,842,89,154,141,356,564,801,530,352,789,395,1070,120,189,217,263,566,202,304,291,429,12,392,660,578,1474,299,270,399,274,247,277,317,239,1026,427,1102,579,225,258,545,761,1771,519,236,338,147,213,110,535,424,371,627,606,786,393,761,188,735,525,375,294,166,688,210,518,762,160,3311</v>
+        <v>9:00 18/04/2020,383,1055,444,161,282,491,2133,213,209,512,295,145,546,1160,279,438,874,577,295,183,463,489,352,571,525,368,857,487,1140,1429,169,390,871,482,263,231,535,893,312,420,667,1781,533,887,555,556,235,445,2005,483,747,81,538,134,1752,587,546,67,361,397,2193,225,351,410,362,998,1918,840,455,635,766,579,1069,452,812,459,555,354,361,686,842,932,91,168,145,366,591,820,545,352,804,424,1111,127,190,222,262,581,206,311,310,453,12,414,677,600,1553,305,272,413,310,256,291,331,245,1053,431,1159,596,230,273,600,797,1832,559,247,349,150,217,110,543,431,385,654,623,811,408,787,189,782,544,397,328,168,727,210,533,805,160,3643</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>840</v>
+        <v>871</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>840,</v>
+        <v>871,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>471</v>
+        <v>482</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>471,</v>
+        <v>482,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="2">
-        <v>840</v>
+        <v>871</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>247,</v>
+        <v>263,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>471</v>
+        <v>482</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>225,</v>
+        <v>231,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>518</v>
+        <v>535</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>518,</v>
+        <v>535,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>831</v>
+        <v>893</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>831,</v>
+        <v>893,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>518</v>
+        <v>535</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>300,</v>
+        <v>312,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>831</v>
+        <v>893</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>396,</v>
+        <v>420,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>616</v>
+        <v>667</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>616,</v>
+        <v>667,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>396</v>
+        <v>420</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>1721</v>
+        <v>1781</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1721,</v>
+        <v>1781,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>616</v>
+        <v>667</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>513</v>
+        <v>533</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>513,</v>
+        <v>533,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>1721</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>825</v>
+        <v>887</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>825,</v>
+        <v>887,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>513</v>
+        <v>533</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>533</v>
+        <v>555</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>533,</v>
+        <v>555,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="2">
-        <v>825</v>
+        <v>887</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>550,</v>
+        <v>556,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>533</v>
+        <v>555</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>230,</v>
+        <v>235,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>537</v>
+        <v>543</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>417</v>
+        <v>445</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>417,</v>
+        <v>445,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>1941</v>
+        <v>2005</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1941,</v>
+        <v>2005,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>417</v>
+        <v>445</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>472</v>
+        <v>483</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>472,</v>
+        <v>483,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>1941</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>724</v>
+        <v>747</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>724,</v>
+        <v>747,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>472</v>
+        <v>483</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>79,</v>
+        <v>81,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>724</v>
+        <v>747</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>524,</v>
+        <v>538,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>129,</v>
+        <v>134,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>524</v>
+        <v>538</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1695</v>
+        <v>1752</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1695,</v>
+        <v>1752,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>571</v>
+        <v>587</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>571,</v>
+        <v>587,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1695</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>530</v>
+        <v>546</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>530,</v>
+        <v>546,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>571</v>
+        <v>587</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>58,</v>
+        <v>67,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>530</v>
+        <v>546</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>352,</v>
+        <v>361,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>389,</v>
+        <v>397,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>352</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2108</v>
+        <v>2193</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2108,</v>
+        <v>2193,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>389</v>
+        <v>397</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>201,</v>
+        <v>225,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2108</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>330,</v>
+        <v>351,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>201</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>395</v>
+        <v>410</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>395,</v>
+        <v>410,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>330</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>357,</v>
+        <v>362,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>395</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>970</v>
+        <v>998</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>970,</v>
+        <v>998,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>1842</v>
+        <v>1918</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1842,</v>
+        <v>1918,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="2">
-        <v>970</v>
+        <v>998</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>784</v>
+        <v>840</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>784,</v>
+        <v>840,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>1842</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>442,</v>
+        <v>455,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="2">
-        <v>784</v>
+        <v>840</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>609</v>
+        <v>635</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>609,</v>
+        <v>635,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>442</v>
+        <v>455</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>752</v>
+        <v>766</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>752,</v>
+        <v>766,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>609</v>
+        <v>635</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>551</v>
+        <v>579</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>551,</v>
+        <v>579,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>752</v>
+        <v>766</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1028</v>
+        <v>1069</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1028,</v>
+        <v>1069,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>551</v>
+        <v>579</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>428</v>
+        <v>452</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>428,</v>
+        <v>452,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1028</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>788</v>
+        <v>812</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>788,</v>
+        <v>812,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>428</v>
+        <v>452</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>441,</v>
+        <v>459,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>788</v>
+        <v>812</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>543</v>
+        <v>555</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>543,</v>
+        <v>555,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>441</v>
+        <v>459</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>346,</v>
+        <v>354,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>543</v>
+        <v>555</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>344</v>
+        <v>361</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>344,</v>
+        <v>361,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>346</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>670</v>
+        <v>686</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>670,</v>
+        <v>686,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>344</v>
+        <v>361</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>834</v>
+        <v>842</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>834,</v>
+        <v>842,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>670</v>
+        <v>686</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>842</v>
+        <v>932</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>842,</v>
+        <v>932,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>834</v>
+        <v>842</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>89,</v>
+        <v>91,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="2">
-        <v>842</v>
+        <v>932</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>154,</v>
+        <v>168,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>141,</v>
+        <v>145,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>356,</v>
+        <v>366,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>564</v>
+        <v>591</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>564,</v>
+        <v>591,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>356</v>
+        <v>366</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>801</v>
+        <v>820</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>801,</v>
+        <v>820,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>564</v>
+        <v>591</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>530</v>
+        <v>545</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>530,</v>
+        <v>545,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>801</v>
+        <v>820</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3077,7 +3077,7 @@
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>530</v>
+        <v>545</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,11 +3086,11 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>789</v>
+        <v>804</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>789,</v>
+        <v>804,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>395</v>
+        <v>424</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>395,</v>
+        <v>424,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>789</v>
+        <v>804</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1070</v>
+        <v>1111</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1070,</v>
+        <v>1111,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>395</v>
+        <v>424</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>120,</v>
+        <v>127,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1070</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>189,</v>
+        <v>190,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>217,</v>
+        <v>222,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>263,</v>
+        <v>262,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>566</v>
+        <v>581</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>566,</v>
+        <v>581,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>202,</v>
+        <v>206,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>566</v>
+        <v>581</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>304,</v>
+        <v>311,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>291,</v>
+        <v>310,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>304</v>
+        <v>311</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>429</v>
+        <v>453</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>429,</v>
+        <v>453,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>291</v>
+        <v>310</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>429</v>
+        <v>453</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>392</v>
+        <v>414</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>392,</v>
+        <v>414,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>660</v>
+        <v>677</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>660,</v>
+        <v>677,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>392</v>
+        <v>414</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>578</v>
+        <v>600</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>578,</v>
+        <v>600,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>660</v>
+        <v>677</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1474</v>
+        <v>1553</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1474,</v>
+        <v>1553,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>578</v>
+        <v>600</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>299,</v>
+        <v>305,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1474</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>270,</v>
+        <v>272,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>399,</v>
+        <v>413,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>274</v>
+        <v>310</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>274,</v>
+        <v>310,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>399</v>
+        <v>413</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>247,</v>
+        <v>256,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>274</v>
+        <v>310</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>277,</v>
+        <v>291,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>317,</v>
+        <v>331,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>239,</v>
+        <v>245,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>317</v>
+        <v>331</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1026</v>
+        <v>1053</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1026,</v>
+        <v>1053,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>427,</v>
+        <v>431,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1026</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1102</v>
+        <v>1159</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1102,</v>
+        <v>1159,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>579</v>
+        <v>596</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>579,</v>
+        <v>596,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1102</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>225,</v>
+        <v>230,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>579</v>
+        <v>596</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>258,</v>
+        <v>273,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>545</v>
+        <v>600</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>545,</v>
+        <v>600,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>761</v>
+        <v>797</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>761,</v>
+        <v>797,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>545</v>
+        <v>600</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>1771</v>
+        <v>1832</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1771,</v>
+        <v>1832,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="2">
-        <v>761</v>
+        <v>797</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>519</v>
+        <v>559</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>519,</v>
+        <v>559,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>1771</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>236,</v>
+        <v>247,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>519</v>
+        <v>559</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>338,</v>
+        <v>349,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>236</v>
+        <v>247</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>147,</v>
+        <v>150,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>338</v>
+        <v>349</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>213,</v>
+        <v>217,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3837,7 +3837,7 @@
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,11 +3846,11 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>535,</v>
+        <v>543,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>424,</v>
+        <v>431,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>535</v>
+        <v>543</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>371,</v>
+        <v>385,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>424</v>
+        <v>431</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>627</v>
+        <v>654</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>627,</v>
+        <v>654,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>371</v>
+        <v>385</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>606</v>
+        <v>623</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>606,</v>
+        <v>623,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>627</v>
+        <v>654</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>786</v>
+        <v>811</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>786,</v>
+        <v>811,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>606</v>
+        <v>623</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>393</v>
+        <v>408</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>393,</v>
+        <v>408,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>786</v>
+        <v>811</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>761</v>
+        <v>787</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>761,</v>
+        <v>787,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>393</v>
+        <v>408</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>188,</v>
+        <v>189,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>761</v>
+        <v>787</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>735</v>
+        <v>782</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>735,</v>
+        <v>782,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>525</v>
+        <v>544</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>525,</v>
+        <v>544,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>735</v>
+        <v>782</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>375</v>
+        <v>397</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>375,</v>
+        <v>397,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>525</v>
+        <v>544</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>294</v>
+        <v>328</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>294,</v>
+        <v>328,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>375</v>
+        <v>397</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>166,</v>
+        <v>168,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>294</v>
+        <v>328</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>688</v>
+        <v>727</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>688,</v>
+        <v>727,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4141,7 +4141,7 @@
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>688</v>
+        <v>727</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,11 +4150,11 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>518</v>
+        <v>533</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>518,</v>
+        <v>533,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>762</v>
+        <v>805</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>762,</v>
+        <v>805,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>518</v>
+        <v>533</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4198,7 +4198,7 @@
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>762</v>
+        <v>805</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,11 +4207,11 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>3311</v>
+        <v>3643</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>3311</v>
+        <v>3643</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
update data as of 19 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4563F0-40C0-7542-B84E-4B03CC64334D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77E35BB-4A6F-D147-AD0B-8771A918E889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>383,</v>
+        <v>393,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>7203</v>
+        <v>7476</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>7203,</v>
+        <v>7476,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>4918</v>
+        <v>5154</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1055</v>
+        <v>1069</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1055,</v>
+        <v>1069,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1055</v>
+        <v>1069</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>20904</v>
+        <v>21357</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>20904,</v>
+        <v>21357,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>7203</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>444,</v>
+        <v>454,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>13963</v>
+        <v>14581</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13963,</v>
+        <v>14581,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>20904</v>
+        <v>21357</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>161,</v>
+        <v>166,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>11739</v>
+        <v>12276</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11739,</v>
+        <v>12276,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>5115</v>
+        <v>5395</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>282,</v>
+        <v>289,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>13237</v>
+        <v>13871</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13237,</v>
+        <v>13871,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>13237</v>
+        <v>13871</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>491</v>
+        <v>501</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>491,</v>
+        <v>501,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>491</v>
+        <v>501</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>11885</v>
+        <v>12563</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11885,</v>
+        <v>12563,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>11885</v>
+        <v>12563</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2133</v>
+        <v>2243</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2133,</v>
+        <v>2243,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2133</v>
+        <v>2243</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>4448</v>
+        <v>4669</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4448,</v>
+        <v>4669,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>4448</v>
+        <v>4669</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>213,</v>
+        <v>222,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>3643</v>
+        <v>3836</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>3643,</v>
+        <v>3836,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>9045</v>
+        <v>9427</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>209,</v>
+        <v>224,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>87022</v>
+        <v>90629</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>87022</v>
+        <v>90629</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>6624</v>
+        <v>6881</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>512</v>
+        <v>545</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>512,</v>
+        <v>545,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>512</v>
+        <v>545</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>295,</v>
+        <v>308,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>295</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>145,</v>
+        <v>155,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>546</v>
+        <v>564</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>546,</v>
+        <v>564,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>546</v>
+        <v>564</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>87022</v>
+        <v>90629</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>87022,</v>
+        <v>90629,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>87022</v>
+        <v>90629</v>
       </c>
       <c r="M14" s="3">
-        <v>13917</v>
+        <v>14399</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1160</v>
+        <v>1182</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1160,</v>
+        <v>1182,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1160</v>
+        <v>1182</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>7820</v>
+        <v>8187</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>7820,</v>
+        <v>8187,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>2486</v>
+        <v>2645</v>
       </c>
       <c r="M15" s="2">
-        <v>176</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>279,</v>
+        <v>292,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>6936</v>
+        <v>7270</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6936,</v>
+        <v>7270,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>7820</v>
+        <v>8187</v>
       </c>
       <c r="M16" s="2">
-        <v>837</v>
+        <v>893</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>438,</v>
+        <v>454,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>2486</v>
+        <v>2645</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>2486</v>
+        <v>2645</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>6936</v>
+        <v>7270</v>
       </c>
       <c r="M17" s="2">
-        <v>534</v>
+        <v>575</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>874</v>
+        <v>900</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>874,</v>
+        <v>900,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>874</v>
+        <v>900</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>577</v>
+        <v>613</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>577,</v>
+        <v>613,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>577</v>
+        <v>613</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>295,</v>
+        <v>309,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>183,</v>
+        <v>189,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>357023</v>
+        <v>372967</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>357023,</v>
+        <v>372967,</v>
       </c>
       <c r="K21" s="9">
-        <v>357023</v>
+        <v>372967</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>463</v>
+        <v>502</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>463,</v>
+        <v>502,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>463</v>
+        <v>502</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>242806</v>
+        <v>252900</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>242806,</v>
+        <v>252900,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>489,</v>
+        <v>501,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>114217</v>
+        <v>120067</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>114217,</v>
+        <v>120067,</v>
       </c>
       <c r="K23" s="9">
-        <v>114217</v>
+        <v>120067</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>352,</v>
+        <v>360,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>15464</v>
+        <v>16060</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>15464,</v>
+        <v>16060,</v>
       </c>
       <c r="K24" s="9">
-        <v>15464</v>
+        <v>16060</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>571</v>
+        <v>588</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>571,</v>
+        <v>588,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>571</v>
+        <v>588</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>525</v>
+        <v>546</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>525,</v>
+        <v>546,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>525</v>
+        <v>546</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>368</v>
+        <v>396</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>368,</v>
+        <v>396,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>857</v>
+        <v>894</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>857,</v>
+        <v>894,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>368</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>487,</v>
+        <v>493,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="2">
-        <v>857</v>
+        <v>894</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43939</v>
+        <v>43940</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1140</v>
+        <v>1170</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1140,</v>
+        <v>1170,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 18/04/2020,357023,242806,114217,15464,135</v>
+        <v>9:00 19/04/2020,372967,252900,120067,16060,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1429</v>
+        <v>1467</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1429,</v>
+        <v>1467,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1140</v>
+        <v>1170</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 18/04/2020,87022,7820,6936,2486</v>
+        <v>9:00 19/04/2020,90629,8187,7270,2645</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>169,</v>
+        <v>178,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1429</v>
+        <v>1467</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 18/04/2020,7203,20904,13963,11739,13237,11885,4448,3643,87022</v>
+        <v>9:00 19/04/2020,7476,21357,14581,12276,13871,12563,4669,3836,90629</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>390,</v>
+        <v>401,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 18/04/2020,383,1055,444,161,282,491,2133,213,209,512,295,145,546,1160,279,438,874,577,295,183,463,489,352,571,525,368,857,487,1140,1429,169,390,871,482,263,231,535,893,312,420,667,1781,533,887,555,556,235,445,2005,483,747,81,538,134,1752,587,546,67,361,397,2193,225,351,410,362,998,1918,840,455,635,766,579,1069,452,812,459,555,354,361,686,842,932,91,168,145,366,591,820,545,352,804,424,1111,127,190,222,262,581,206,311,310,453,12,414,677,600,1553,305,272,413,310,256,291,331,245,1053,431,1159,596,230,273,600,797,1832,559,247,349,150,217,110,543,431,385,654,623,811,408,787,189,782,544,397,328,168,727,210,533,805,160,3643</v>
+        <v>9:00 19/04/2020,393,1069,454,166,289,501,2243,222,224,545,308,155,564,1182,292,454,900,613,309,189,502,501,360,588,546,396,894,493,1170,1467,178,401,901,517,265,239,564,906,330,433,672,1846,567,904,560,565,256,465,2122,484,761,84,552,141,1808,602,557,68,366,407,2308,241,365,421,390,1016,2018,893,463,678,810,584,1119,471,833,476,571,367,375,704,859,977,91,167,159,371,616,877,571,385,853,445,1158,136,199,232,307,589,212,325,318,478,12,445,735,636,1598,314,295,422,345,263,345,353,251,1075,457,1202,619,233,281,618,869,1941,574,259,365,159,218,123,548,454,392,665,631,830,437,805,202,820,551,416,337,182,762,231,558,845,182,3836</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>871</v>
+        <v>901</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>871,</v>
+        <v>901,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>390</v>
+        <v>401</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>482</v>
+        <v>517</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>482,</v>
+        <v>517,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="2">
-        <v>871</v>
+        <v>901</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>263,</v>
+        <v>265,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>482</v>
+        <v>517</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>231,</v>
+        <v>239,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>535</v>
+        <v>564</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>535,</v>
+        <v>564,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>893</v>
+        <v>906</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>893,</v>
+        <v>906,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>535</v>
+        <v>564</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>312,</v>
+        <v>330,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>893</v>
+        <v>906</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>420</v>
+        <v>433</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>420,</v>
+        <v>433,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>312</v>
+        <v>330</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>667,</v>
+        <v>672,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>420</v>
+        <v>433</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>1781</v>
+        <v>1846</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1781,</v>
+        <v>1846,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>667</v>
+        <v>672</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>533</v>
+        <v>567</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>533,</v>
+        <v>567,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>1781</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>887</v>
+        <v>904</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>887,</v>
+        <v>904,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>533</v>
+        <v>567</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>555,</v>
+        <v>560,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="2">
-        <v>887</v>
+        <v>904</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>556</v>
+        <v>565</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>556,</v>
+        <v>565,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>235,</v>
+        <v>256,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>543</v>
+        <v>552</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>445</v>
+        <v>465</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>445,</v>
+        <v>465,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>235</v>
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2005</v>
+        <v>2122</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2005,</v>
+        <v>2122,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>445</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>483,</v>
+        <v>484,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2005</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>747</v>
+        <v>761</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>747,</v>
+        <v>761,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>81,</v>
+        <v>84,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>747</v>
+        <v>761</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>538</v>
+        <v>552</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>538,</v>
+        <v>552,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>134,</v>
+        <v>141,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>538</v>
+        <v>552</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1752</v>
+        <v>1808</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1752,</v>
+        <v>1808,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>587</v>
+        <v>602</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>587,</v>
+        <v>602,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1752</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>546,</v>
+        <v>557,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>587</v>
+        <v>602</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>67,</v>
+        <v>68,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>546</v>
+        <v>557</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>361,</v>
+        <v>366,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>397,</v>
+        <v>407,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2193</v>
+        <v>2308</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2193,</v>
+        <v>2308,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>397</v>
+        <v>407</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>225,</v>
+        <v>241,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2193</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>351,</v>
+        <v>365,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>410,</v>
+        <v>421,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>351</v>
+        <v>365</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>362</v>
+        <v>390</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>362,</v>
+        <v>390,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>410</v>
+        <v>421</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>998</v>
+        <v>1016</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>998,</v>
+        <v>1016,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>362</v>
+        <v>390</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>1918</v>
+        <v>2018</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1918,</v>
+        <v>2018,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F68" s="2">
-        <v>998</v>
+      <c r="F68" s="3">
+        <v>1016</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>840</v>
+        <v>893</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>840,</v>
+        <v>893,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>1918</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>455,</v>
+        <v>463,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="2">
-        <v>840</v>
+        <v>893</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>635</v>
+        <v>678</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>635,</v>
+        <v>678,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>766</v>
+        <v>810</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>766,</v>
+        <v>810,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>635</v>
+        <v>678</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>579,</v>
+        <v>584,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>766</v>
+        <v>810</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1069</v>
+        <v>1119</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1069,</v>
+        <v>1119,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>579</v>
+        <v>584</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>452</v>
+        <v>471</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>452,</v>
+        <v>471,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1069</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>812</v>
+        <v>833</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>812,</v>
+        <v>833,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>452</v>
+        <v>471</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>459</v>
+        <v>476</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>459,</v>
+        <v>476,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>812</v>
+        <v>833</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>555</v>
+        <v>571</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>555,</v>
+        <v>571,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>459</v>
+        <v>476</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>354,</v>
+        <v>367,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>555</v>
+        <v>571</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>361,</v>
+        <v>375,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>354</v>
+        <v>367</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>686</v>
+        <v>704</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>686,</v>
+        <v>704,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>361</v>
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>842</v>
+        <v>859</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>842,</v>
+        <v>859,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>686</v>
+        <v>704</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>932</v>
+        <v>977</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>932,</v>
+        <v>977,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>842</v>
+        <v>859</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2944,7 +2944,7 @@
         <v>81</v>
       </c>
       <c r="F84" s="2">
-        <v>932</v>
+        <v>977</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,11 +2953,11 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>168,</v>
+        <v>167,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>145,</v>
+        <v>159,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>366,</v>
+        <v>371,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>145</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>591</v>
+        <v>616</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>591,</v>
+        <v>616,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>820</v>
+        <v>877</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>820,</v>
+        <v>877,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>591</v>
+        <v>616</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>545</v>
+        <v>571</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>545,</v>
+        <v>571,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>820</v>
+        <v>877</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>352</v>
+        <v>385</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>352,</v>
+        <v>385,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>545</v>
+        <v>571</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>804</v>
+        <v>853</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>804,</v>
+        <v>853,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>352</v>
+        <v>385</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>424</v>
+        <v>445</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>424,</v>
+        <v>445,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>804</v>
+        <v>853</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1111</v>
+        <v>1158</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1111,</v>
+        <v>1158,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>424</v>
+        <v>445</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>127,</v>
+        <v>136,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1111</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>190,</v>
+        <v>199,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>222,</v>
+        <v>232,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>262</v>
+        <v>307</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>262,</v>
+        <v>307,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>581,</v>
+        <v>589,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>262</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>206,</v>
+        <v>212,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>581</v>
+        <v>589</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>311,</v>
+        <v>325,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>310,</v>
+        <v>318,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>311</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>453</v>
+        <v>478</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>453,</v>
+        <v>478,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>453</v>
+        <v>478</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>414</v>
+        <v>445</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>414,</v>
+        <v>445,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>677</v>
+        <v>735</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>677,</v>
+        <v>735,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>414</v>
+        <v>445</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>636</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>600,</v>
+        <v>636,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>677</v>
+        <v>735</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1553</v>
+        <v>1598</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1553,</v>
+        <v>1598,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>600</v>
+        <v>636</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>305,</v>
+        <v>314,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1553</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>272,</v>
+        <v>295,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>413,</v>
+        <v>422,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>272</v>
+        <v>295</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>310</v>
+        <v>345</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>310,</v>
+        <v>345,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>256,</v>
+        <v>263,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>310</v>
+        <v>345</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>291</v>
+        <v>345</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>291,</v>
+        <v>345,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>331</v>
+        <v>353</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>331,</v>
+        <v>353,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>291</v>
+        <v>345</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>245,</v>
+        <v>251,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>331</v>
+        <v>353</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1053</v>
+        <v>1075</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1053,</v>
+        <v>1075,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>431</v>
+        <v>457</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>431,</v>
+        <v>457,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1053</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1159</v>
+        <v>1202</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1159,</v>
+        <v>1202,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>431</v>
+        <v>457</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>596</v>
+        <v>619</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>596,</v>
+        <v>619,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1159</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>230,</v>
+        <v>233,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>596</v>
+        <v>619</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>273,</v>
+        <v>281,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>618</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>600,</v>
+        <v>618,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>797</v>
+        <v>869</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>797,</v>
+        <v>869,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>600</v>
+        <v>618</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>1832</v>
+        <v>1941</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1832,</v>
+        <v>1941,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="2">
-        <v>797</v>
+        <v>869</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>559</v>
+        <v>574</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>559,</v>
+        <v>574,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>1832</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>247,</v>
+        <v>259,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>559</v>
+        <v>574</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>349,</v>
+        <v>365,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>150,</v>
+        <v>159,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>349</v>
+        <v>365</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>217,</v>
+        <v>218,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>110,</v>
+        <v>123,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>543,</v>
+        <v>548,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>431</v>
+        <v>454</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>431,</v>
+        <v>454,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>543</v>
+        <v>548</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>385,</v>
+        <v>392,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>431</v>
+        <v>454</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>654</v>
+        <v>665</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>654,</v>
+        <v>665,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>623,</v>
+        <v>631,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>654</v>
+        <v>665</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>811</v>
+        <v>830</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>811,</v>
+        <v>830,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>623</v>
+        <v>631</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>408</v>
+        <v>437</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>408,</v>
+        <v>437,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>811</v>
+        <v>830</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>787</v>
+        <v>805</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>787,</v>
+        <v>805,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>408</v>
+        <v>437</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>189,</v>
+        <v>202,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>787</v>
+        <v>805</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>782</v>
+        <v>820</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>782,</v>
+        <v>820,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>189</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>544,</v>
+        <v>551,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>782</v>
+        <v>820</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>397</v>
+        <v>416</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>397,</v>
+        <v>416,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>544</v>
+        <v>551</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>328,</v>
+        <v>337,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>397</v>
+        <v>416</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>168,</v>
+        <v>182,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>727</v>
+        <v>762</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>727,</v>
+        <v>762,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>210,</v>
+        <v>231,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>727</v>
+        <v>762</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>533</v>
+        <v>558</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>533,</v>
+        <v>558,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>210</v>
+        <v>231</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>805</v>
+        <v>845</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>805,</v>
+        <v>845,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>533</v>
+        <v>558</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>160,</v>
+        <v>182,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>805</v>
+        <v>845</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>3643</v>
+        <v>3836</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>3643</v>
+        <v>3836</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>160</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 20 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77E35BB-4A6F-D147-AD0B-8771A918E889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC1922-0FCB-5746-A5EB-004AF0234020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>393,</v>
+        <v>398,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>7476</v>
+        <v>7732</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>7476,</v>
+        <v>7732,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>5154</v>
+        <v>5251</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1069</v>
+        <v>1081</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1069,</v>
+        <v>1081,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1069</v>
+        <v>1081</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>21357</v>
+        <v>21654</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>21357,</v>
+        <v>21654,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>7476</v>
+        <v>7732</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>454,</v>
+        <v>458,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>14581</v>
+        <v>15038</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14581,</v>
+        <v>15038,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>21357</v>
+        <v>21654</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>166,</v>
+        <v>172,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>12276</v>
+        <v>12642</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12276,</v>
+        <v>12642,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>5395</v>
+        <v>5611</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>289</v>
+        <v>326</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>289,</v>
+        <v>326,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>289</v>
+        <v>326</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>13871</v>
+        <v>14328</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13871,</v>
+        <v>14328,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>13871</v>
+        <v>14328</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>501,</v>
+        <v>513,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>12563</v>
+        <v>12878</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12563,</v>
+        <v>12878,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>12563</v>
+        <v>12878</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2243</v>
+        <v>2310</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2243,</v>
+        <v>2310,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2243</v>
+        <v>2310</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>4669</v>
+        <v>4861</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4669,</v>
+        <v>4861,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>4669</v>
+        <v>4861</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>222,</v>
+        <v>231,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>3836</v>
+        <v>3897</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>3836,</v>
+        <v>3897,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>9427</v>
+        <v>9787</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>224,</v>
+        <v>245,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>90629</v>
+        <v>93030</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>90629</v>
+        <v>93030</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>6881</v>
+        <v>7031</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>545</v>
+        <v>559</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>545,</v>
+        <v>559,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>545</v>
+        <v>559</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>308,</v>
+        <v>312,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>155,</v>
+        <v>156,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>564,</v>
+        <v>571,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>90629</v>
+        <v>93030</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>90629,</v>
+        <v>93030,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>90629</v>
+        <v>93030</v>
       </c>
       <c r="M14" s="3">
-        <v>14399</v>
+        <v>14828</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1182</v>
+        <v>1206</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1182,</v>
+        <v>1206,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1182</v>
+        <v>1206</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>8187</v>
+        <v>8450</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>8187,</v>
+        <v>8450,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>2645</v>
+        <v>2728</v>
       </c>
       <c r="M15" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>292,</v>
+        <v>305,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>7270</v>
+        <v>7546</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>7270,</v>
+        <v>7546,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>8187</v>
+        <v>8450</v>
       </c>
       <c r="M16" s="2">
-        <v>893</v>
+        <v>903</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>454</v>
+        <v>469</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>454,</v>
+        <v>469,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>454</v>
+        <v>469</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>2645</v>
+        <v>2728</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>2645</v>
+        <v>2728</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>7270</v>
+        <v>7546</v>
       </c>
       <c r="M17" s="2">
-        <v>575</v>
+        <v>584</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>905</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>900,</v>
+        <v>905,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>900</v>
+        <v>905</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>613</v>
+        <v>625</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>613,</v>
+        <v>625,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>613</v>
+        <v>625</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>309</v>
+        <v>335</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>309,</v>
+        <v>335,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>309</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>189,</v>
+        <v>190,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>372967</v>
+        <v>386044</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>372967,</v>
+        <v>386044,</v>
       </c>
       <c r="K21" s="9">
-        <v>372967</v>
+        <v>386044</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>502</v>
+        <v>530</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>502,</v>
+        <v>530,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>502</v>
+        <v>530</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>252900</v>
+        <v>261301</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>252900,</v>
+        <v>261301,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>501,</v>
+        <v>504,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>120067</v>
+        <v>124743</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>120067,</v>
+        <v>124743,</v>
       </c>
       <c r="K23" s="9">
-        <v>120067</v>
+        <v>124743</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>360,</v>
+        <v>372,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>16060</v>
+        <v>16509</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16060,</v>
+        <v>16509,</v>
       </c>
       <c r="K24" s="9">
-        <v>16060</v>
+        <v>16509</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>588,</v>
+        <v>604,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>546</v>
+        <v>575</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>546,</v>
+        <v>575,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>546</v>
+        <v>575</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>396,</v>
+        <v>400,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>894</v>
+        <v>944</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>894,</v>
+        <v>944,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>493</v>
+        <v>515</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>493,</v>
+        <v>515,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="2">
-        <v>894</v>
+        <v>944</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43940</v>
+        <v>43941</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1170</v>
+        <v>1187</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1170,</v>
+        <v>1187,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>493</v>
+        <v>515</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 19/04/2020,372967,252900,120067,16060,135</v>
+        <v>9:00 20/04/2020,386044,261301,124743,16509,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1467</v>
+        <v>1496</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1467,</v>
+        <v>1496,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1170</v>
+        <v>1187</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 19/04/2020,90629,8187,7270,2645</v>
+        <v>9:00 20/04/2020,93030,8450,7546,2728</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>178,</v>
+        <v>187,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1467</v>
+        <v>1496</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 19/04/2020,7476,21357,14581,12276,13871,12563,4669,3836,90629</v>
+        <v>9:00 20/04/2020,7732,21654,15038,12642,14328,12878,4861,3897,93030</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>401,</v>
+        <v>405,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 19/04/2020,393,1069,454,166,289,501,2243,222,224,545,308,155,564,1182,292,454,900,613,309,189,502,501,360,588,546,396,894,493,1170,1467,178,401,901,517,265,239,564,906,330,433,672,1846,567,904,560,565,256,465,2122,484,761,84,552,141,1808,602,557,68,366,407,2308,241,365,421,390,1016,2018,893,463,678,810,584,1119,471,833,476,571,367,375,704,859,977,91,167,159,371,616,877,571,385,853,445,1158,136,199,232,307,589,212,325,318,478,12,445,735,636,1598,314,295,422,345,263,345,353,251,1075,457,1202,619,233,281,618,869,1941,574,259,365,159,218,123,548,454,392,665,631,830,437,805,202,820,551,416,337,182,762,231,558,845,182,3836</v>
+        <v>9:00 20/04/2020,398,1081,458,172,326,513,2310,231,245,559,312,156,571,1206,305,469,905,625,335,190,530,504,372,604,575,400,944,515,1187,1496,187,405,931,543,266,252,586,919,337,449,693,1892,585,934,564,568,263,482,2159,487,770,89,555,149,1864,623,567,69,373,412,2402,258,371,433,402,1026,2096,930,475,707,814,585,1145,473,852,478,583,394,390,722,862,997,92,171,168,378,629,882,600,386,868,462,1202,137,200,236,307,597,219,330,324,478,12,464,758,647,1631,330,296,431,361,274,357,354,255,1089,478,1248,640,238,296,656,898,1961,589,281,375,167,230,129,550,464,404,687,636,845,446,842,206,867,555,437,366,184,788,232,581,887,183,3897</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>901</v>
+        <v>931</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>901,</v>
+        <v>931,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>517</v>
+        <v>543</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>517,</v>
+        <v>543,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="2">
-        <v>901</v>
+        <v>931</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>265,</v>
+        <v>266,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>517</v>
+        <v>543</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>239,</v>
+        <v>252,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>564</v>
+        <v>586</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>564,</v>
+        <v>586,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>239</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>906</v>
+        <v>919</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>906,</v>
+        <v>919,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>564</v>
+        <v>586</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>330,</v>
+        <v>337,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>906</v>
+        <v>919</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>433</v>
+        <v>449</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>433,</v>
+        <v>449,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>672</v>
+        <v>693</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>672,</v>
+        <v>693,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>433</v>
+        <v>449</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>1846</v>
+        <v>1892</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1846,</v>
+        <v>1892,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>672</v>
+        <v>693</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>567</v>
+        <v>585</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>567,</v>
+        <v>585,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>1846</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>904</v>
+        <v>934</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>904,</v>
+        <v>934,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>567</v>
+        <v>585</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>560,</v>
+        <v>564,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="2">
-        <v>904</v>
+        <v>934</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>565,</v>
+        <v>568,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>256,</v>
+        <v>263,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>465</v>
+        <v>482</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>465,</v>
+        <v>482,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2122</v>
+        <v>2159</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2122,</v>
+        <v>2159,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>465</v>
+        <v>482</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>484,</v>
+        <v>487,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2122</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>761</v>
+        <v>770</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>761,</v>
+        <v>770,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>84,</v>
+        <v>89,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>761</v>
+        <v>770</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>552,</v>
+        <v>555,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>141,</v>
+        <v>149,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1808</v>
+        <v>1864</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1808,</v>
+        <v>1864,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>602</v>
+        <v>623</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>602,</v>
+        <v>623,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1808</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>557</v>
+        <v>567</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>557,</v>
+        <v>567,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>602</v>
+        <v>623</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>68,</v>
+        <v>69,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>557</v>
+        <v>567</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>366,</v>
+        <v>373,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>407,</v>
+        <v>412,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>366</v>
+        <v>373</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2308</v>
+        <v>2402</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2308,</v>
+        <v>2402,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>241,</v>
+        <v>258,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2308</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>365,</v>
+        <v>371,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>241</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>421,</v>
+        <v>433,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>390,</v>
+        <v>402,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>421</v>
+        <v>433</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1016</v>
+        <v>1026</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1016,</v>
+        <v>1026,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>390</v>
+        <v>402</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2018</v>
+        <v>2096</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2018,</v>
+        <v>2096,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1016</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>893</v>
+        <v>930</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>893,</v>
+        <v>930,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2018</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>463,</v>
+        <v>475,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="2">
-        <v>893</v>
+        <v>930</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>678</v>
+        <v>707</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>678,</v>
+        <v>707,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>463</v>
+        <v>475</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>810,</v>
+        <v>814,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>678</v>
+        <v>707</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>584,</v>
+        <v>585,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>810</v>
+        <v>814</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1119</v>
+        <v>1145</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1119,</v>
+        <v>1145,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>471,</v>
+        <v>473,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1119</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>833</v>
+        <v>852</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>833,</v>
+        <v>852,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>476,</v>
+        <v>478,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>833</v>
+        <v>852</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>571,</v>
+        <v>583,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>367,</v>
+        <v>394,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>571</v>
+        <v>583</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>375,</v>
+        <v>390,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>367</v>
+        <v>394</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>704</v>
+        <v>722</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>704,</v>
+        <v>722,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>375</v>
+        <v>390</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>859,</v>
+        <v>862,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>704</v>
+        <v>722</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>977</v>
+        <v>997</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>977,</v>
+        <v>997,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>859</v>
+        <v>862</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>91,</v>
+        <v>92,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="2">
-        <v>977</v>
+        <v>997</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>167,</v>
+        <v>171,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>159,</v>
+        <v>168,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>371,</v>
+        <v>378,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>616</v>
+        <v>629</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>616,</v>
+        <v>629,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>877,</v>
+        <v>882,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>616</v>
+        <v>629</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>571</v>
+        <v>600</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>571,</v>
+        <v>600,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>877</v>
+        <v>882</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>385,</v>
+        <v>386,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>571</v>
+        <v>600</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>853</v>
+        <v>868</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>853,</v>
+        <v>868,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>445</v>
+        <v>462</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>445,</v>
+        <v>462,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>853</v>
+        <v>868</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1158</v>
+        <v>1202</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1158,</v>
+        <v>1202,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>445</v>
+        <v>462</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>136,</v>
+        <v>137,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1158</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>199,</v>
+        <v>200,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>232,</v>
+        <v>236,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3210,7 +3210,7 @@
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,11 +3219,11 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>589,</v>
+        <v>597,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>212,</v>
+        <v>219,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>589</v>
+        <v>597</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>325,</v>
+        <v>330,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>318,</v>
+        <v>324,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3305,7 +3305,7 @@
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>445</v>
+        <v>464</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>445,</v>
+        <v>464,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>735</v>
+        <v>758</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>735,</v>
+        <v>758,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>445</v>
+        <v>464</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>636</v>
+        <v>647</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>636,</v>
+        <v>647,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>735</v>
+        <v>758</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1598</v>
+        <v>1631</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1598,</v>
+        <v>1631,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>636</v>
+        <v>647</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>314,</v>
+        <v>330,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1598</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>295,</v>
+        <v>296,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>314</v>
+        <v>330</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>422,</v>
+        <v>431,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>345,</v>
+        <v>361,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>263,</v>
+        <v>274,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>345</v>
+        <v>361</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>345,</v>
+        <v>357,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>263</v>
+        <v>274</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>353,</v>
+        <v>354,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>345</v>
+        <v>357</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>251,</v>
+        <v>255,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1075</v>
+        <v>1089</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1075,</v>
+        <v>1089,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>457</v>
+        <v>478</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>457,</v>
+        <v>478,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1075</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1202</v>
+        <v>1248</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1202,</v>
+        <v>1248,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>457</v>
+        <v>478</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>619</v>
+        <v>640</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>619,</v>
+        <v>640,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1202</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>233,</v>
+        <v>238,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>619</v>
+        <v>640</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>281,</v>
+        <v>296,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>618</v>
+        <v>656</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>618,</v>
+        <v>656,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>281</v>
+        <v>296</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>869</v>
+        <v>898</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>869,</v>
+        <v>898,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>618</v>
+        <v>656</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>1941</v>
+        <v>1961</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1941,</v>
+        <v>1961,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="2">
-        <v>869</v>
+        <v>898</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>574</v>
+        <v>589</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>574,</v>
+        <v>589,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>1941</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>259,</v>
+        <v>281,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>574</v>
+        <v>589</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>365,</v>
+        <v>375,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>259</v>
+        <v>281</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>159,</v>
+        <v>167,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>365</v>
+        <v>375</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>218,</v>
+        <v>230,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>123,</v>
+        <v>129,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>548,</v>
+        <v>550,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>454,</v>
+        <v>464,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>392,</v>
+        <v>404,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>454</v>
+        <v>464</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>665</v>
+        <v>687</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>665,</v>
+        <v>687,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>392</v>
+        <v>404</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>631,</v>
+        <v>636,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>665</v>
+        <v>687</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>830</v>
+        <v>845</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>830,</v>
+        <v>845,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>631</v>
+        <v>636</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>437,</v>
+        <v>446,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>830</v>
+        <v>845</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>805</v>
+        <v>842</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>805,</v>
+        <v>842,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>437</v>
+        <v>446</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>202,</v>
+        <v>206,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>805</v>
+        <v>842</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>820</v>
+        <v>867</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>820,</v>
+        <v>867,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>551,</v>
+        <v>555,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>820</v>
+        <v>867</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>416</v>
+        <v>437</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>416,</v>
+        <v>437,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>551</v>
+        <v>555</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>337</v>
+        <v>366</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>337,</v>
+        <v>366,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>416</v>
+        <v>437</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>182,</v>
+        <v>184,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>337</v>
+        <v>366</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>762</v>
+        <v>788</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>762,</v>
+        <v>788,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>231,</v>
+        <v>232,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>762</v>
+        <v>788</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>558</v>
+        <v>581</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>558,</v>
+        <v>581,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>845</v>
+        <v>887</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>845,</v>
+        <v>887,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>558</v>
+        <v>581</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>182,</v>
+        <v>183,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>845</v>
+        <v>887</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>3836</v>
+        <v>3897</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>3836</v>
+        <v>3897</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 21 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC1922-0FCB-5746-A5EB-004AF0234020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9185376D-9446-1642-87D1-606F4F8EB297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>398,</v>
+        <v>408,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>7732</v>
+        <v>7967</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>7732,</v>
+        <v>7967,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>5251</v>
+        <v>5371</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1081</v>
+        <v>1095</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1081,</v>
+        <v>1095,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1081</v>
+        <v>1095</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>21654</v>
+        <v>22072</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>21654,</v>
+        <v>22072,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>7732</v>
+        <v>7967</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>458</v>
+        <v>476</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>458,</v>
+        <v>476,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>458</v>
+        <v>476</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>15038</v>
+        <v>15488</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>15038,</v>
+        <v>15488,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>21654</v>
+        <v>22072</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>172,</v>
+        <v>179,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>12642</v>
+        <v>13057</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12642,</v>
+        <v>13057,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>5611</v>
+        <v>5775</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>326,</v>
+        <v>331,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>14328</v>
+        <v>14788</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14328,</v>
+        <v>14788,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>14328</v>
+        <v>14788</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>513</v>
+        <v>541</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>513,</v>
+        <v>541,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>513</v>
+        <v>541</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>12878</v>
+        <v>13656</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12878,</v>
+        <v>13656,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>12878</v>
+        <v>13656</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2310</v>
+        <v>2361</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2310,</v>
+        <v>2361,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2310</v>
+        <v>2361</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>4861</v>
+        <v>5045</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4861,</v>
+        <v>5045,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>4861</v>
+        <v>5045</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>231,</v>
+        <v>242,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>3897</v>
+        <v>4044</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>3897,</v>
+        <v>4044,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>9787</v>
+        <v>10117</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>245,</v>
+        <v>269,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>93030</v>
+        <v>96117</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>93030</v>
+        <v>96117</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>7031</v>
+        <v>7282</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>559</v>
+        <v>582</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>559,</v>
+        <v>582,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>559</v>
+        <v>582</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>312</v>
+        <v>346</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>312,</v>
+        <v>346,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>312</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>156,</v>
+        <v>172,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>571</v>
+        <v>602</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>571,</v>
+        <v>602,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>571</v>
+        <v>602</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>93030</v>
+        <v>96117</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>93030,</v>
+        <v>96117,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>93030</v>
+        <v>96117</v>
       </c>
       <c r="M14" s="3">
-        <v>14828</v>
+        <v>15606</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1206</v>
+        <v>1238</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1206,</v>
+        <v>1238,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1206</v>
+        <v>1238</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>8450</v>
+        <v>8672</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>8450,</v>
+        <v>8672,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>2728</v>
+        <v>2758</v>
       </c>
       <c r="M15" s="2">
-        <v>194</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>305,</v>
+        <v>319,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>7546</v>
+        <v>7850</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>7546,</v>
+        <v>7850,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>8450</v>
+        <v>8672</v>
       </c>
       <c r="M16" s="2">
-        <v>903</v>
+        <v>915</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>469,</v>
+        <v>477,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>2728</v>
+        <v>2758</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>2728</v>
+        <v>2758</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>7546</v>
+        <v>7850</v>
       </c>
       <c r="M17" s="2">
-        <v>584</v>
+        <v>609</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>905</v>
+        <v>927</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>905,</v>
+        <v>927,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>905</v>
+        <v>927</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>625</v>
+        <v>652</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>625,</v>
+        <v>652,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>625</v>
+        <v>652</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>335,</v>
+        <v>348,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>335</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>190,</v>
+        <v>196,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>386044</v>
+        <v>397670</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>386044,</v>
+        <v>397670,</v>
       </c>
       <c r="K21" s="9">
-        <v>386044</v>
+        <v>397670</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>530</v>
+        <v>549</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>530,</v>
+        <v>549,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>530</v>
+        <v>549</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>261301</v>
+        <v>268626</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>261301,</v>
+        <v>268626,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>504</v>
+        <v>521</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>504,</v>
+        <v>521,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>504</v>
+        <v>521</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>124743</v>
+        <v>129044</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>124743,</v>
+        <v>129044,</v>
       </c>
       <c r="K23" s="9">
-        <v>124743</v>
+        <v>129044</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>372,</v>
+        <v>379,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>16509</v>
+        <v>17337</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16509,</v>
+        <v>17337,</v>
       </c>
       <c r="K24" s="9">
-        <v>16509</v>
+        <v>17337</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>604</v>
+        <v>624</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>604,</v>
+        <v>624,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>604</v>
+        <v>624</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>575</v>
+        <v>593</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>575,</v>
+        <v>593,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>575</v>
+        <v>593</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>400,</v>
+        <v>410,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>944</v>
+        <v>966</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>944,</v>
+        <v>966,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>400</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>515</v>
+        <v>536</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>515,</v>
+        <v>536,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="2">
-        <v>944</v>
+        <v>966</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43941</v>
+        <v>43942</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1187</v>
+        <v>1214</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1187,</v>
+        <v>1214,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>515</v>
+        <v>536</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 20/04/2020,386044,261301,124743,16509,135</v>
+        <v>9:00 21/04/2020,397670,268626,129044,17337,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1496</v>
+        <v>1529</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1496,</v>
+        <v>1529,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1187</v>
+        <v>1214</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 20/04/2020,93030,8450,7546,2728</v>
+        <v>9:00 21/04/2020,96117,8672,7850,2758</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>187,</v>
+        <v>189,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1496</v>
+        <v>1529</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 20/04/2020,7732,21654,15038,12642,14328,12878,4861,3897,93030</v>
+        <v>9:00 21/04/2020,7967,22072,15488,13057,14788,13656,5045,4044,96117</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>405,</v>
+        <v>409,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 20/04/2020,398,1081,458,172,326,513,2310,231,245,559,312,156,571,1206,305,469,905,625,335,190,530,504,372,604,575,400,944,515,1187,1496,187,405,931,543,266,252,586,919,337,449,693,1892,585,934,564,568,263,482,2159,487,770,89,555,149,1864,623,567,69,373,412,2402,258,371,433,402,1026,2096,930,475,707,814,585,1145,473,852,478,583,394,390,722,862,997,92,171,168,378,629,882,600,386,868,462,1202,137,200,236,307,597,219,330,324,478,12,464,758,647,1631,330,296,431,361,274,357,354,255,1089,478,1248,640,238,296,656,898,1961,589,281,375,167,230,129,550,464,404,687,636,845,446,842,206,867,555,437,366,184,788,232,581,887,183,3897</v>
+        <v>9:00 21/04/2020,408,1095,476,179,331,541,2361,242,269,582,346,172,602,1238,319,477,927,652,348,196,549,521,379,624,593,410,966,536,1214,1529,189,409,946,561,280,258,607,932,346,457,713,1929,607,972,572,581,267,489,2251,491,791,95,569,159,1904,635,584,73,377,417,2597,259,384,444,425,1037,2170,958,496,731,826,593,1172,485,872,509,591,407,390,738,878,1053,93,171,169,395,656,904,621,391,888,485,1240,147,215,237,361,600,223,335,328,515,13,477,776,667,1684,352,317,443,366,281,371,365,255,1098,492,1287,658,241,303,701,922,2100,595,284,383,180,234,147,560,480,413,714,656,854,460,884,241,895,563,452,380,205,813,275,599,916,189,4044</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>931</v>
+        <v>946</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>931,</v>
+        <v>946,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>543</v>
+        <v>561</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>543,</v>
+        <v>561,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="2">
-        <v>931</v>
+        <v>946</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>266,</v>
+        <v>280,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>543</v>
+        <v>561</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>252,</v>
+        <v>258,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>266</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>586</v>
+        <v>607</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>586,</v>
+        <v>607,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>919</v>
+        <v>932</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>919,</v>
+        <v>932,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>586</v>
+        <v>607</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>337,</v>
+        <v>346,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>919</v>
+        <v>932</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>449,</v>
+        <v>457,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>693</v>
+        <v>713</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>693,</v>
+        <v>713,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>1892</v>
+        <v>1929</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1892,</v>
+        <v>1929,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>693</v>
+        <v>713</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>585</v>
+        <v>607</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>585,</v>
+        <v>607,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>1892</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>934</v>
+        <v>972</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>934,</v>
+        <v>972,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>585</v>
+        <v>607</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>564</v>
+        <v>572</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>564,</v>
+        <v>572,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="2">
-        <v>934</v>
+        <v>972</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>568</v>
+        <v>581</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>568,</v>
+        <v>581,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>564</v>
+        <v>572</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>263,</v>
+        <v>267,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>555</v>
+        <v>568</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>482,</v>
+        <v>489,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2159</v>
+        <v>2251</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2159,</v>
+        <v>2251,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>482</v>
+        <v>489</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>487,</v>
+        <v>491,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2159</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>770</v>
+        <v>791</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>770,</v>
+        <v>791,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>89,</v>
+        <v>95,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>770</v>
+        <v>791</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>555</v>
+        <v>569</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>555,</v>
+        <v>569,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>149,</v>
+        <v>159,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>555</v>
+        <v>569</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1864</v>
+        <v>1904</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1864,</v>
+        <v>1904,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>623</v>
+        <v>635</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>623,</v>
+        <v>635,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1864</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>567</v>
+        <v>584</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>567,</v>
+        <v>584,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>623</v>
+        <v>635</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>69,</v>
+        <v>73,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>567</v>
+        <v>584</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>373,</v>
+        <v>377,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>412,</v>
+        <v>417,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2402</v>
+        <v>2597</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2402,</v>
+        <v>2597,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>412</v>
+        <v>417</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>258,</v>
+        <v>259,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2402</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>371,</v>
+        <v>384,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>433,</v>
+        <v>444,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>371</v>
+        <v>384</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>402,</v>
+        <v>425,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>433</v>
+        <v>444</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1026</v>
+        <v>1037</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1026,</v>
+        <v>1037,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>402</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2096</v>
+        <v>2170</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2096,</v>
+        <v>2170,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1026</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>930</v>
+        <v>958</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>930,</v>
+        <v>958,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2096</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>475</v>
+        <v>496</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>475,</v>
+        <v>496,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="2">
-        <v>930</v>
+        <v>958</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>707</v>
+        <v>731</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>707,</v>
+        <v>731,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>475</v>
+        <v>496</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>814</v>
+        <v>826</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>814,</v>
+        <v>826,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>707</v>
+        <v>731</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>585,</v>
+        <v>593,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>814</v>
+        <v>826</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1145</v>
+        <v>1172</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1145,</v>
+        <v>1172,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>585</v>
+        <v>593</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>473,</v>
+        <v>485,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1145</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>852</v>
+        <v>872</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>852,</v>
+        <v>872,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>473</v>
+        <v>485</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>478,</v>
+        <v>509,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>852</v>
+        <v>872</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>583,</v>
+        <v>591,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>478</v>
+        <v>509</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>394,</v>
+        <v>407,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>583</v>
+        <v>591</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2868,7 +2868,7 @@
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>394</v>
+        <v>407</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,11 +2877,11 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>722</v>
+        <v>738</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>722,</v>
+        <v>738,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>862</v>
+        <v>878</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>862,</v>
+        <v>878,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>722</v>
+        <v>738</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>997</v>
+        <v>1053</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>997,</v>
+        <v>1053,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>862</v>
+        <v>878</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>92,</v>
+        <v>93,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F84" s="2">
-        <v>997</v>
+      <c r="F84" s="3">
+        <v>1053</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2963,7 +2963,7 @@
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>168,</v>
+        <v>169,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>378</v>
+        <v>395</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>378,</v>
+        <v>395,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>629</v>
+        <v>656</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>629,</v>
+        <v>656,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>378</v>
+        <v>395</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>882</v>
+        <v>904</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>882,</v>
+        <v>904,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>629</v>
+        <v>656</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>600</v>
+        <v>621</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>600,</v>
+        <v>621,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>882</v>
+        <v>904</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>386,</v>
+        <v>391,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>600</v>
+        <v>621</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>868</v>
+        <v>888</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>868,</v>
+        <v>888,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>386</v>
+        <v>391</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>462</v>
+        <v>485</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>462,</v>
+        <v>485,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>868</v>
+        <v>888</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1202</v>
+        <v>1240</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1202,</v>
+        <v>1240,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>462</v>
+        <v>485</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>137,</v>
+        <v>147,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1202</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>200,</v>
+        <v>215,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>236,</v>
+        <v>237,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>200</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>307</v>
+        <v>361</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>307,</v>
+        <v>361,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>597,</v>
+        <v>600,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>307</v>
+        <v>361</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>219,</v>
+        <v>223,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>330,</v>
+        <v>335,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>324,</v>
+        <v>328,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>478</v>
+        <v>515</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>478,</v>
+        <v>515,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C104" s="5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>12,</v>
+        <v>13,</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>478</v>
+        <v>515</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>464</v>
+        <v>477</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>464,</v>
+        <v>477,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F105" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>758</v>
+        <v>776</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>758,</v>
+        <v>776,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>464</v>
+        <v>477</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>647</v>
+        <v>667</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>647,</v>
+        <v>667,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>758</v>
+        <v>776</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1631</v>
+        <v>1684</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1631,</v>
+        <v>1684,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>647</v>
+        <v>667</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>330,</v>
+        <v>352,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1631</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>296</v>
+        <v>317</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>296,</v>
+        <v>317,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>330</v>
+        <v>352</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>431,</v>
+        <v>443,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>296</v>
+        <v>317</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>361,</v>
+        <v>366,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>431</v>
+        <v>443</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>274,</v>
+        <v>281,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>357,</v>
+        <v>371,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>354,</v>
+        <v>365,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>357</v>
+        <v>371</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3552,7 +3552,7 @@
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>354</v>
+        <v>365</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,11 +3561,11 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1089</v>
+        <v>1098</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1089,</v>
+        <v>1098,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>478,</v>
+        <v>492,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1089</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1248</v>
+        <v>1287</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1248,</v>
+        <v>1287,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>478</v>
+        <v>492</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>640</v>
+        <v>658</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>640,</v>
+        <v>658,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1248</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>238,</v>
+        <v>241,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>640</v>
+        <v>658</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>296,</v>
+        <v>303,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>656</v>
+        <v>701</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>656,</v>
+        <v>701,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>898</v>
+        <v>922</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>898,</v>
+        <v>922,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>656</v>
+        <v>701</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>1961</v>
+        <v>2100</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1961,</v>
+        <v>2100,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="2">
-        <v>898</v>
+        <v>922</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>589,</v>
+        <v>595,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>1961</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>281,</v>
+        <v>284,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>589</v>
+        <v>595</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>375,</v>
+        <v>383,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>167,</v>
+        <v>180,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>230,</v>
+        <v>234,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>129,</v>
+        <v>147,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>550,</v>
+        <v>560,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>129</v>
+        <v>147</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>464,</v>
+        <v>480,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>550</v>
+        <v>560</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>404,</v>
+        <v>413,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>464</v>
+        <v>480</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>687</v>
+        <v>714</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>687,</v>
+        <v>714,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>636</v>
+        <v>656</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>636,</v>
+        <v>656,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>687</v>
+        <v>714</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>845</v>
+        <v>854</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>845,</v>
+        <v>854,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>636</v>
+        <v>656</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>446,</v>
+        <v>460,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>845</v>
+        <v>854</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>842</v>
+        <v>884</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>842,</v>
+        <v>884,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>446</v>
+        <v>460</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>241</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>206,</v>
+        <v>241,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>842</v>
+        <v>884</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>867</v>
+        <v>895</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>867,</v>
+        <v>895,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>206</v>
+        <v>241</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>555,</v>
+        <v>563,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>867</v>
+        <v>895</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>437</v>
+        <v>452</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>437,</v>
+        <v>452,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>555</v>
+        <v>563</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>366,</v>
+        <v>380,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>437</v>
+        <v>452</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>184,</v>
+        <v>205,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>366</v>
+        <v>380</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>788</v>
+        <v>813</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>788,</v>
+        <v>813,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>184</v>
+        <v>205</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>232</v>
+        <v>275</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>232,</v>
+        <v>275,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>788</v>
+        <v>813</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>581</v>
+        <v>599</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>581,</v>
+        <v>599,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>232</v>
+        <v>275</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>887,</v>
+        <v>916,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>581</v>
+        <v>599</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>183,</v>
+        <v>189,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>887</v>
+        <v>916</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>3897</v>
+        <v>4044</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>3897</v>
+        <v>4044</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 22 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9185376D-9446-1642-87D1-606F4F8EB297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE2ADC7-5AFD-7A44-8612-6421D891F483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="E1" sqref="E1:F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>408,</v>
+        <v>418,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>7967</v>
+        <v>8218</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>7967,</v>
+        <v>8218,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>5371</v>
+        <v>5630</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1095</v>
+        <v>1101</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1095,</v>
+        <v>1101,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1095</v>
+        <v>1101</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>22072</v>
+        <v>22352</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>22072,</v>
+        <v>22352,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>7967</v>
+        <v>8218</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>476,</v>
+        <v>488,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>15488</v>
+        <v>16093</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>15488,</v>
+        <v>16093,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>22072</v>
+        <v>22352</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>179,</v>
+        <v>182,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>13057</v>
+        <v>13777</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13057,</v>
+        <v>13777,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>5775</v>
+        <v>6095</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>331,</v>
+        <v>340,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>14788</v>
+        <v>15209</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14788,</v>
+        <v>15209,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>14788</v>
+        <v>15209</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>541</v>
+        <v>549</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>541,</v>
+        <v>549,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>541</v>
+        <v>549</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>13656</v>
+        <v>14053</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13656,</v>
+        <v>14053,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>13656</v>
+        <v>14053</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2361</v>
+        <v>2431</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2361,</v>
+        <v>2431,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2361</v>
+        <v>2431</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>5045</v>
+        <v>5229</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5045,</v>
+        <v>5229,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>5045</v>
+        <v>5229</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>242,</v>
+        <v>248,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>4044</v>
+        <v>4206</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4044,</v>
+        <v>4206,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>10117</v>
+        <v>10463</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>269</v>
+        <v>294</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>269,</v>
+        <v>294,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>269</v>
+        <v>294</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>96117</v>
+        <v>99137</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>96117</v>
+        <v>99137</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>7282</v>
+        <v>7682</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>582</v>
+        <v>601</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>582,</v>
+        <v>601,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>582</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>346,</v>
+        <v>355,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>346</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>172,</v>
+        <v>174,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>602</v>
+        <v>618</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>602,</v>
+        <v>618,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>602</v>
+        <v>618</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>96117</v>
+        <v>99137</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>96117,</v>
+        <v>99137,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>96117</v>
+        <v>99137</v>
       </c>
       <c r="M14" s="3">
-        <v>15606</v>
+        <v>16271</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1238</v>
+        <v>1254</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1238,</v>
+        <v>1254,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1238</v>
+        <v>1254</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>8672</v>
+        <v>9038</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>8672,</v>
+        <v>9038,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>2758</v>
+        <v>2874</v>
       </c>
       <c r="M15" s="2">
-        <v>207</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>319,</v>
+        <v>322,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>7850</v>
+        <v>8124</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>7850,</v>
+        <v>8124,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>8672</v>
+        <v>9038</v>
       </c>
       <c r="M16" s="2">
-        <v>915</v>
+        <v>985</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>477</v>
+        <v>496</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>477,</v>
+        <v>496,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>477</v>
+        <v>496</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>2758</v>
+        <v>2874</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>2758</v>
+        <v>2874</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>7850</v>
+        <v>8124</v>
       </c>
       <c r="M17" s="2">
-        <v>609</v>
+        <v>624</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>927</v>
+        <v>942</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>927,</v>
+        <v>942,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>927</v>
+        <v>942</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>652</v>
+        <v>681</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>652,</v>
+        <v>681,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>652</v>
+        <v>681</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>348,</v>
+        <v>354,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>196,</v>
+        <v>200,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>397670</v>
+        <v>411192</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>397670,</v>
+        <v>411192,</v>
       </c>
       <c r="K21" s="9">
-        <v>397670</v>
+        <v>411192</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>549</v>
+        <v>569</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>549,</v>
+        <v>569,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>549</v>
+        <v>569</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>268626</v>
+        <v>277697</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>268626,</v>
+        <v>277697,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>521</v>
+        <v>531</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>521,</v>
+        <v>531,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>521</v>
+        <v>531</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>129044</v>
+        <v>133495</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>129044,</v>
+        <v>133495,</v>
       </c>
       <c r="K23" s="9">
-        <v>129044</v>
+        <v>133495</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>379,</v>
+        <v>392,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>17337</v>
+        <v>18100</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17337,</v>
+        <v>18100,</v>
       </c>
       <c r="K24" s="9">
-        <v>17337</v>
+        <v>18100</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>624</v>
+        <v>654</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>624,</v>
+        <v>654,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>624</v>
+        <v>654</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>593</v>
+        <v>608</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>593,</v>
+        <v>608,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>593</v>
+        <v>608</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>410,</v>
+        <v>427,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>966</v>
+        <v>1027</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>966,</v>
+        <v>1027,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>410</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>536,</v>
+        <v>539,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="2">
-        <v>966</v>
+      <c r="F29" s="3">
+        <v>1027</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43942</v>
+        <v>43943</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1214</v>
+        <v>1226</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1214,</v>
+        <v>1226,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 21/04/2020,397670,268626,129044,17337,135</v>
+        <v>9:00 22/04/2020,411192,277697,133495,18100,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1529</v>
+        <v>1543</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1529,</v>
+        <v>1543,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1214</v>
+        <v>1226</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 21/04/2020,96117,8672,7850,2758</v>
+        <v>9:00 22/04/2020,99137,9038,8124,2874</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>189,</v>
+        <v>203,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1529</v>
+        <v>1543</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 21/04/2020,7967,22072,15488,13057,14788,13656,5045,4044,96117</v>
+        <v>9:00 22/04/2020,8218,22352,16093,13777,15209,14053,5229,4206,99137</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>409,</v>
+        <v>413,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 21/04/2020,408,1095,476,179,331,541,2361,242,269,582,346,172,602,1238,319,477,927,652,348,196,549,521,379,624,593,410,966,536,1214,1529,189,409,946,561,280,258,607,932,346,457,713,1929,607,972,572,581,267,489,2251,491,791,95,569,159,1904,635,584,73,377,417,2597,259,384,444,425,1037,2170,958,496,731,826,593,1172,485,872,509,591,407,390,738,878,1053,93,171,169,395,656,904,621,391,888,485,1240,147,215,237,361,600,223,335,328,515,13,477,776,667,1684,352,317,443,366,281,371,365,255,1098,492,1287,658,241,303,701,922,2100,595,284,383,180,234,147,560,480,413,714,656,854,460,884,241,895,563,452,380,205,813,275,599,916,189,4044</v>
+        <v>9:00 22/04/2020,418,1101,488,182,340,549,2431,248,294,601,355,174,618,1254,322,496,942,681,354,200,569,531,392,654,608,427,1027,539,1226,1543,203,413,969,581,309,268,617,953,386,471,723,1980,634,989,579,585,277,495,2336,505,803,98,574,168,1954,655,593,74,377,419,2685,303,390,456,445,1047,2229,1010,520,757,837,669,1210,501,894,526,602,413,395,766,885,1118,104,218,175,408,687,945,647,416,928,495,1288,155,227,238,368,610,229,342,344,530,13,487,805,690,1746,366,325,455,384,288,412,382,258,1105,509,1346,671,249,325,715,1009,2134,599,299,389,194,236,161,563,486,429,735,663,860,472,906,255,910,567,479,397,206,830,283,613,963,198,4206</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>946</v>
+        <v>969</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>946,</v>
+        <v>969,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>561</v>
+        <v>581</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>561,</v>
+        <v>581,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="2">
-        <v>946</v>
+        <v>969</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>280</v>
+        <v>309</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>280,</v>
+        <v>309,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>561</v>
+        <v>581</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>258,</v>
+        <v>268,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>280</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>607</v>
+        <v>617</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>607,</v>
+        <v>617,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>932</v>
+        <v>953</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>932,</v>
+        <v>953,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>607</v>
+        <v>617</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>346</v>
+        <v>386</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>346,</v>
+        <v>386,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>932</v>
+        <v>953</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>457,</v>
+        <v>471,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>346</v>
+        <v>386</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>713</v>
+        <v>723</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>713,</v>
+        <v>723,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>457</v>
+        <v>471</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>1929</v>
+        <v>1980</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1929,</v>
+        <v>1980,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>713</v>
+        <v>723</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>607</v>
+        <v>634</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>607,</v>
+        <v>634,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>1929</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>972</v>
+        <v>989</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>972,</v>
+        <v>989,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>607</v>
+        <v>634</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>572,</v>
+        <v>579,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="2">
-        <v>972</v>
+        <v>989</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>581,</v>
+        <v>585,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>572</v>
+        <v>579</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>267,</v>
+        <v>277,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>489,</v>
+        <v>495,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2251</v>
+        <v>2336</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2251,</v>
+        <v>2336,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>491,</v>
+        <v>505,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2251</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>791</v>
+        <v>803</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>791,</v>
+        <v>803,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>491</v>
+        <v>505</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>95,</v>
+        <v>98,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>791</v>
+        <v>803</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>569,</v>
+        <v>574,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>159,</v>
+        <v>168,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>569</v>
+        <v>574</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1904</v>
+        <v>1954</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1904,</v>
+        <v>1954,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>635</v>
+        <v>655</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>635,</v>
+        <v>655,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1904</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>584</v>
+        <v>593</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>584,</v>
+        <v>593,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>635</v>
+        <v>655</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>73,</v>
+        <v>74,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>584</v>
+        <v>593</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2488,7 +2488,7 @@
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>417,</v>
+        <v>419,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2597</v>
+        <v>2685</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2597,</v>
+        <v>2685,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>259</v>
+        <v>303</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>259,</v>
+        <v>303,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2597</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>384,</v>
+        <v>390,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>259</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>444,</v>
+        <v>456,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>425</v>
+        <v>445</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>425,</v>
+        <v>445,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>444</v>
+        <v>456</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1037</v>
+        <v>1047</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1037,</v>
+        <v>1047,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>425</v>
+        <v>445</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2170</v>
+        <v>2229</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2170,</v>
+        <v>2229,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1037</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>958</v>
+        <v>1010</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>958,</v>
+        <v>1010,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2170</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>496</v>
+        <v>520</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>496,</v>
+        <v>520,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F70" s="2">
-        <v>958</v>
+      <c r="F70" s="3">
+        <v>1010</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>731</v>
+        <v>757</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>731,</v>
+        <v>757,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>496</v>
+        <v>520</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>826</v>
+        <v>837</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>826,</v>
+        <v>837,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>731</v>
+        <v>757</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>593</v>
+        <v>669</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>593,</v>
+        <v>669,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>826</v>
+        <v>837</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1172</v>
+        <v>1210</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1172,</v>
+        <v>1210,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>593</v>
+        <v>669</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>485</v>
+        <v>501</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>485,</v>
+        <v>501,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1172</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>872</v>
+        <v>894</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>872,</v>
+        <v>894,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>485</v>
+        <v>501</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>509</v>
+        <v>526</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>509,</v>
+        <v>526,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>872</v>
+        <v>894</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>591,</v>
+        <v>602,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>509</v>
+        <v>526</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>407,</v>
+        <v>413,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>591</v>
+        <v>602</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>390,</v>
+        <v>395,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>407</v>
+        <v>413</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>738</v>
+        <v>766</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>738,</v>
+        <v>766,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>390</v>
+        <v>395</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>878</v>
+        <v>885</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>878,</v>
+        <v>885,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>738</v>
+        <v>766</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1053</v>
+        <v>1118</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1053,</v>
+        <v>1118,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>878</v>
+        <v>885</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>93,</v>
+        <v>104,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1053</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>171</v>
+        <v>218</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>171,</v>
+        <v>218,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>169,</v>
+        <v>175,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>171</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>395,</v>
+        <v>408,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>656</v>
+        <v>687</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>656,</v>
+        <v>687,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>395</v>
+        <v>408</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>904</v>
+        <v>945</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>904,</v>
+        <v>945,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>656</v>
+        <v>687</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>621</v>
+        <v>647</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>621,</v>
+        <v>647,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>904</v>
+        <v>945</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>391,</v>
+        <v>416,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>621</v>
+        <v>647</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>888</v>
+        <v>928</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>888,</v>
+        <v>928,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>391</v>
+        <v>416</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>485</v>
+        <v>495</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>485,</v>
+        <v>495,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>888</v>
+        <v>928</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1240</v>
+        <v>1288</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1240,</v>
+        <v>1288,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>485</v>
+        <v>495</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>147,</v>
+        <v>155,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1240</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>215,</v>
+        <v>227,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>237,</v>
+        <v>238,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>361,</v>
+        <v>368,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>600,</v>
+        <v>610,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>361</v>
+        <v>368</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>223,</v>
+        <v>229,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>600</v>
+        <v>610</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>335,</v>
+        <v>342,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>328,</v>
+        <v>344,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>515</v>
+        <v>530</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>515,</v>
+        <v>530,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>328</v>
+        <v>344</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>515</v>
+        <v>530</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>477,</v>
+        <v>487,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>776</v>
+        <v>805</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>776,</v>
+        <v>805,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>477</v>
+        <v>487</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>667</v>
+        <v>690</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>667,</v>
+        <v>690,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>776</v>
+        <v>805</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1684</v>
+        <v>1746</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1684,</v>
+        <v>1746,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>667</v>
+        <v>690</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>352,</v>
+        <v>366,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1684</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>317,</v>
+        <v>325,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>352</v>
+        <v>366</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>443,</v>
+        <v>455,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>366</v>
+        <v>384</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>366,</v>
+        <v>384,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>281,</v>
+        <v>288,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>366</v>
+        <v>384</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>371</v>
+        <v>412</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>371,</v>
+        <v>412,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>365</v>
+        <v>382</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>365,</v>
+        <v>382,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>371</v>
+        <v>412</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>255,</v>
+        <v>258,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>365</v>
+        <v>382</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1098</v>
+        <v>1105</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1098,</v>
+        <v>1105,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>492</v>
+        <v>509</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>492,</v>
+        <v>509,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1098</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1287</v>
+        <v>1346</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1287,</v>
+        <v>1346,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>492</v>
+        <v>509</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>658,</v>
+        <v>671,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1287</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>241,</v>
+        <v>249,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>658</v>
+        <v>671</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>303,</v>
+        <v>325,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>701</v>
+        <v>715</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>701,</v>
+        <v>715,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>303</v>
+        <v>325</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>922</v>
+        <v>1009</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>922,</v>
+        <v>1009,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>701</v>
+        <v>715</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2100</v>
+        <v>2134</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2100,</v>
+        <v>2134,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F125" s="2">
-        <v>922</v>
+      <c r="F125" s="3">
+        <v>1009</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>595,</v>
+        <v>599,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2100</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>284,</v>
+        <v>299,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>383,</v>
+        <v>389,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>284</v>
+        <v>299</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>180,</v>
+        <v>194,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>234,</v>
+        <v>236,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>147,</v>
+        <v>161,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>560,</v>
+        <v>563,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>480,</v>
+        <v>486,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>413</v>
+        <v>429</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>413,</v>
+        <v>429,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>480</v>
+        <v>486</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>714</v>
+        <v>735</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>714,</v>
+        <v>735,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>413</v>
+        <v>429</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>656</v>
+        <v>663</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>656,</v>
+        <v>663,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>714</v>
+        <v>735</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>854</v>
+        <v>860</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>854,</v>
+        <v>860,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>656</v>
+        <v>663</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>460,</v>
+        <v>472,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>854</v>
+        <v>860</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>884</v>
+        <v>906</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>884,</v>
+        <v>906,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>460</v>
+        <v>472</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>241,</v>
+        <v>255,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>884</v>
+        <v>906</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>895</v>
+        <v>910</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>895,</v>
+        <v>910,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>241</v>
+        <v>255</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>563,</v>
+        <v>567,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>895</v>
+        <v>910</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>452</v>
+        <v>479</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>452,</v>
+        <v>479,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>380</v>
+        <v>397</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>380,</v>
+        <v>397,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>452</v>
+        <v>479</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>205,</v>
+        <v>206,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>380</v>
+        <v>397</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>813</v>
+        <v>830</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>813,</v>
+        <v>830,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>275,</v>
+        <v>283,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>813</v>
+        <v>830</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>599</v>
+        <v>613</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>599,</v>
+        <v>613,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>275</v>
+        <v>283</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>916</v>
+        <v>963</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>916,</v>
+        <v>963,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>599</v>
+        <v>613</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>189,</v>
+        <v>198,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>916</v>
+        <v>963</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>4044</v>
+        <v>4206</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>4044</v>
+        <v>4206</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 23 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE2ADC7-5AFD-7A44-8612-6421D891F483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10915A8-0034-CC45-93F8-CD88C3035BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE15D73-8EAA-6046-85A1-3798C28E97CA}">
   <dimension ref="B1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F151"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>418,</v>
+        <v>428,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>8218</v>
+        <v>8654</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>8218,</v>
+        <v>8654,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>5630</v>
+        <v>5802</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1101</v>
+        <v>1119</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1101,</v>
+        <v>1119,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1101</v>
+        <v>1119</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>22352</v>
+        <v>22767</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>22352,</v>
+        <v>22767,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>8218</v>
+        <v>8654</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>488,</v>
+        <v>495,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>16093</v>
+        <v>16663</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16093,</v>
+        <v>16663,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>22352</v>
+        <v>22767</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>182,</v>
+        <v>187,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>13777</v>
+        <v>14246</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>13777,</v>
+        <v>14246,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>6095</v>
+        <v>6318</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>340,</v>
+        <v>353,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>15209</v>
+        <v>15682</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>15209,</v>
+        <v>15682,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>15209</v>
+        <v>15682</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>549,</v>
+        <v>560,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>14053</v>
+        <v>14412</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14053,</v>
+        <v>14412,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>14053</v>
+        <v>14412</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2431</v>
+        <v>2483</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2431,</v>
+        <v>2483,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2431</v>
+        <v>2483</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>5229</v>
+        <v>5411</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5229,</v>
+        <v>5411,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>5229</v>
+        <v>5411</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>248,</v>
+        <v>256,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>4206</v>
+        <v>4386</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4206,</v>
+        <v>4386,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>10463</v>
+        <v>10861</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>294,</v>
+        <v>311,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>99137</v>
+        <v>102221</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>99137</v>
+        <v>102221</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>7682</v>
+        <v>7928</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>601</v>
+        <v>623</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>601,</v>
+        <v>623,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>601</v>
+        <v>623</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>355,</v>
+        <v>369,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>355</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>618</v>
+        <v>647</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>618,</v>
+        <v>647,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>618</v>
+        <v>647</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>99137</v>
+        <v>102221</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>99137,</v>
+        <v>102221,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>99137</v>
+        <v>102221</v>
       </c>
       <c r="M14" s="3">
-        <v>16271</v>
+        <v>16785</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1254</v>
+        <v>1276</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1254,</v>
+        <v>1276,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1254</v>
+        <v>1276</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>9038</v>
+        <v>9409</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9038,</v>
+        <v>9409,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>2874</v>
+        <v>3016</v>
       </c>
       <c r="M15" s="2">
-        <v>220</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>322,</v>
+        <v>334,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>8124</v>
+        <v>8358</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>8124,</v>
+        <v>8358,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>9038</v>
-      </c>
-      <c r="M16" s="2">
-        <v>985</v>
+        <v>9409</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1062</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>496</v>
+        <v>519</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>496,</v>
+        <v>519,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>496</v>
+        <v>519</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>2874</v>
+        <v>3016</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>2874</v>
+        <v>3016</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>8124</v>
+        <v>8358</v>
       </c>
       <c r="M17" s="2">
-        <v>624</v>
+        <v>641</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>942</v>
+        <v>953</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>942,</v>
+        <v>953,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>942</v>
+        <v>953</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>681</v>
+        <v>691</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>681,</v>
+        <v>691,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>681</v>
+        <v>691</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>354,</v>
+        <v>369,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>354</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>200,</v>
+        <v>204,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>411192</v>
+        <v>425821</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>411192,</v>
+        <v>425821,</v>
       </c>
       <c r="K21" s="9">
-        <v>411192</v>
+        <v>425821</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>569</v>
+        <v>603</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>569,</v>
+        <v>603,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>569</v>
+        <v>603</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>277697</v>
+        <v>287743</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>277697,</v>
+        <v>287743,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>531,</v>
+        <v>537,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>133495</v>
+        <v>138078</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>133495,</v>
+        <v>138078,</v>
       </c>
       <c r="K23" s="9">
-        <v>133495</v>
+        <v>138078</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>392</v>
+        <v>421</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>392,</v>
+        <v>421,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>392</v>
+        <v>421</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>18100</v>
+        <v>18738</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18100,</v>
+        <v>18738,</v>
       </c>
       <c r="K24" s="9">
-        <v>18100</v>
+        <v>18738</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>654</v>
+        <v>689</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>654,</v>
+        <v>689,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>654</v>
+        <v>689</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>608</v>
+        <v>634</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>608,</v>
+        <v>634,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>608</v>
+        <v>634</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,17 +1831,17 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>427,</v>
+        <v>436,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
       </c>
       <c r="F27" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:13">
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1027</v>
+        <v>1071</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1027,</v>
+        <v>1071,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>539</v>
+        <v>567</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>539,</v>
+        <v>567,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1027</v>
+        <v>1071</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43943</v>
+        <v>43944</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1226</v>
+        <v>1253</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1226,</v>
+        <v>1253,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>539</v>
+        <v>567</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 22/04/2020,411192,277697,133495,18100,135</v>
+        <v>9:00 23/04/2020,425821,287743,138078,18738,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1543</v>
+        <v>1584</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1543,</v>
+        <v>1584,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1226</v>
+        <v>1253</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 22/04/2020,99137,9038,8124,2874</v>
+        <v>9:00 23/04/2020,102221,9409,8358,3016</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>203,</v>
+        <v>208,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1543</v>
+        <v>1584</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 22/04/2020,8218,22352,16093,13777,15209,14053,5229,4206,99137</v>
+        <v>9:00 23/04/2020,8654,22767,16663,14246,15682,14412,5411,4386,102221</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>413,</v>
+        <v>423,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 22/04/2020,418,1101,488,182,340,549,2431,248,294,601,355,174,618,1254,322,496,942,681,354,200,569,531,392,654,608,427,1027,539,1226,1543,203,413,969,581,309,268,617,953,386,471,723,1980,634,989,579,585,277,495,2336,505,803,98,574,168,1954,655,593,74,377,419,2685,303,390,456,445,1047,2229,1010,520,757,837,669,1210,501,894,526,602,413,395,766,885,1118,104,218,175,408,687,945,647,416,928,495,1288,155,227,238,368,610,229,342,344,530,13,487,805,690,1746,366,325,455,384,288,412,382,258,1105,509,1346,671,249,325,715,1009,2134,599,299,389,194,236,161,563,486,429,735,663,860,472,906,255,910,567,479,397,206,830,283,613,963,198,4206</v>
+        <v>9:00 23/04/2020,428,1119,495,187,353,560,2483,256,311,623,369,174,647,1276,334,519,953,691,369,204,603,537,421,689,634,436,1071,567,1253,1584,208,423,987,594,326,275,643,973,412,479,755,2069,668,1021,587,596,283,504,2371,509,818,113,587,175,1996,667,601,76,387,423,2826,320,401,466,440,1063,2305,1049,545,776,854,712,1234,548,929,548,615,427,403,781,898,1169,109,244,183,412,718,952,668,448,946,509,1314,171,246,238,369,625,239,347,358,537,13,503,831,699,1751,398,325,476,401,304,425,398,266,1126,510,1405,699,280,345,814,1026,2176,609,307,394,205,244,169,578,504,441,753,677,871,497,955,256,943,570,505,400,206,847,285,640,985,209,4386</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>969</v>
+        <v>987</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>969,</v>
+        <v>987,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>413</v>
+        <v>423</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>581</v>
+        <v>594</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>581,</v>
+        <v>594,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="2">
-        <v>969</v>
+        <v>987</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>309,</v>
+        <v>326,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>581</v>
+        <v>594</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>268,</v>
+        <v>275,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>309</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>617</v>
+        <v>643</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>617,</v>
+        <v>643,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>953</v>
+        <v>973</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>953,</v>
+        <v>973,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>617</v>
+        <v>643</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>386,</v>
+        <v>412,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>953</v>
+        <v>973</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>471,</v>
+        <v>479,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>386</v>
+        <v>412</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>723</v>
+        <v>755</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>723,</v>
+        <v>755,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>1980</v>
+        <v>2069</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1980,</v>
+        <v>2069,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>723</v>
+        <v>755</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>634</v>
+        <v>668</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>634,</v>
+        <v>668,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>1980</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>989</v>
+        <v>1021</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>989,</v>
+        <v>1021,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>634</v>
+        <v>668</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>579,</v>
+        <v>587,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="2">
-        <v>989</v>
+      <c r="F46" s="3">
+        <v>1021</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>585</v>
+        <v>596</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>585,</v>
+        <v>596,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>579</v>
+        <v>587</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>277,</v>
+        <v>283,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>572</v>
+        <v>580</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>495,</v>
+        <v>504,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2336</v>
+        <v>2371</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2336,</v>
+        <v>2371,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>495</v>
+        <v>504</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>505,</v>
+        <v>509,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2336</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>803</v>
+        <v>818</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>803,</v>
+        <v>818,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>98,</v>
+        <v>113,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>803</v>
+        <v>818</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>574</v>
+        <v>587</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>574,</v>
+        <v>587,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>168,</v>
+        <v>175,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>574</v>
+        <v>587</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1954</v>
+        <v>1996</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1954,</v>
+        <v>1996,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>655</v>
+        <v>667</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>655,</v>
+        <v>667,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1954</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>593,</v>
+        <v>601,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>655</v>
+        <v>667</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>74,</v>
+        <v>76,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>593</v>
+        <v>601</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>377,</v>
+        <v>387,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>419,</v>
+        <v>423,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>377</v>
+        <v>387</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2685</v>
+        <v>2826</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2685,</v>
+        <v>2826,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>303,</v>
+        <v>320,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2685</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>390,</v>
+        <v>401,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>303</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>456,</v>
+        <v>466,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>390</v>
+        <v>401</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>445,</v>
+        <v>440,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>456</v>
+        <v>466</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1047</v>
+        <v>1063</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1047,</v>
+        <v>1063,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2229</v>
+        <v>2305</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2229,</v>
+        <v>2305,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1047</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1010</v>
+        <v>1049</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1010,</v>
+        <v>1049,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2229</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>520</v>
+        <v>545</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>520,</v>
+        <v>545,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1010</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>757</v>
+        <v>776</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>757,</v>
+        <v>776,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>520</v>
+        <v>545</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>837</v>
+        <v>854</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>837,</v>
+        <v>854,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>757</v>
+        <v>776</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>669</v>
+        <v>712</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>669,</v>
+        <v>712,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>837</v>
+        <v>854</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1210</v>
+        <v>1234</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1210,</v>
+        <v>1234,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>669</v>
+        <v>712</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>501</v>
+        <v>548</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>501,</v>
+        <v>548,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1210</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>894</v>
+        <v>929</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>894,</v>
+        <v>929,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>501</v>
+        <v>548</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>526</v>
+        <v>548</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>526,</v>
+        <v>548,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>894</v>
+        <v>929</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>602</v>
+        <v>615</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>602,</v>
+        <v>615,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>526</v>
+        <v>548</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>413,</v>
+        <v>427,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>602</v>
+        <v>615</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>395,</v>
+        <v>403,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>413</v>
+        <v>427</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>766</v>
+        <v>781</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>766,</v>
+        <v>781,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>885</v>
+        <v>898</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>885,</v>
+        <v>898,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>766</v>
+        <v>781</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1118</v>
+        <v>1169</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1118,</v>
+        <v>1169,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>885</v>
+        <v>898</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>104,</v>
+        <v>109,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1118</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>218,</v>
+        <v>244,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>175,</v>
+        <v>183,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>218</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>408,</v>
+        <v>412,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>687</v>
+        <v>718</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>687,</v>
+        <v>718,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>945</v>
+        <v>952</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>945,</v>
+        <v>952,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>687</v>
+        <v>718</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>647</v>
+        <v>668</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>647,</v>
+        <v>668,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>945</v>
+        <v>952</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>416</v>
+        <v>448</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>416,</v>
+        <v>448,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>647</v>
+        <v>668</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>928</v>
+        <v>946</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>928,</v>
+        <v>946,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>416</v>
+        <v>448</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>495,</v>
+        <v>509,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>928</v>
+        <v>946</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1288</v>
+        <v>1314</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1288,</v>
+        <v>1314,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>495</v>
+        <v>509</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>155,</v>
+        <v>171,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1288</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>227,</v>
+        <v>246,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>155</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3191,7 +3191,7 @@
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>227</v>
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,11 +3200,11 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>368,</v>
+        <v>369,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>610</v>
+        <v>625</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>610,</v>
+        <v>625,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>229,</v>
+        <v>239,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>610</v>
+        <v>625</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>342,</v>
+        <v>347,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>344,</v>
+        <v>358,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>530,</v>
+        <v>537,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>344</v>
+        <v>358</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>530</v>
+        <v>537</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>487</v>
+        <v>503</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>487,</v>
+        <v>503,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>805</v>
+        <v>831</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>805,</v>
+        <v>831,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>487</v>
+        <v>503</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>690,</v>
+        <v>699,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>805</v>
+        <v>831</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1746</v>
+        <v>1751</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1746,</v>
+        <v>1751,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>690</v>
+        <v>699</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>366</v>
+        <v>398</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>366,</v>
+        <v>398,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1746</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3438,7 +3438,7 @@
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>366</v>
+        <v>398</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,11 +3447,11 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>455</v>
+        <v>476</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>455,</v>
+        <v>476,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>384,</v>
+        <v>401,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>455</v>
+        <v>476</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>288,</v>
+        <v>304,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>384</v>
+        <v>401</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>412,</v>
+        <v>425,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>288</v>
+        <v>304</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>382,</v>
+        <v>398,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>412</v>
+        <v>425</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>258,</v>
+        <v>266,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>382</v>
+        <v>398</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1105</v>
+        <v>1126</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1105,</v>
+        <v>1126,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>509,</v>
+        <v>510,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1105</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1346</v>
+        <v>1405</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1346,</v>
+        <v>1405,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>671</v>
+        <v>699</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>671,</v>
+        <v>699,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1346</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>249</v>
+        <v>280</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>249,</v>
+        <v>280,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>671</v>
+        <v>699</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>325,</v>
+        <v>345,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>249</v>
+        <v>280</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>715</v>
+        <v>814</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>715,</v>
+        <v>814,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>325</v>
+        <v>345</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1009</v>
+        <v>1026</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1009,</v>
+        <v>1026,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>715</v>
+        <v>814</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2134</v>
+        <v>2176</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2134,</v>
+        <v>2176,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1009</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>599,</v>
+        <v>609,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2134</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>299,</v>
+        <v>307,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>599</v>
+        <v>609</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>389,</v>
+        <v>394,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>194,</v>
+        <v>205,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>236,</v>
+        <v>244,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>194</v>
+        <v>205</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>161,</v>
+        <v>169,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>563</v>
+        <v>578</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>563,</v>
+        <v>578,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>486</v>
+        <v>504</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>486,</v>
+        <v>504,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>563</v>
+        <v>578</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>429,</v>
+        <v>441,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>486</v>
+        <v>504</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>735</v>
+        <v>753</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>735,</v>
+        <v>753,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>429</v>
+        <v>441</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>663</v>
+        <v>677</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>663,</v>
+        <v>677,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>735</v>
+        <v>753</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>860</v>
+        <v>871</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>860,</v>
+        <v>871,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>663</v>
+        <v>677</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>472</v>
+        <v>497</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>472,</v>
+        <v>497,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>860</v>
+        <v>871</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>906</v>
+        <v>955</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>906,</v>
+        <v>955,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>472</v>
+        <v>497</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>255,</v>
+        <v>256,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>906</v>
+        <v>955</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>910</v>
+        <v>943</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>910,</v>
+        <v>943,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>567,</v>
+        <v>570,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>910</v>
+        <v>943</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>479</v>
+        <v>505</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>479,</v>
+        <v>505,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>397,</v>
+        <v>400,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>479</v>
+        <v>505</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4103,7 +4103,7 @@
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,11 +4112,11 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>830</v>
+        <v>847</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>830,</v>
+        <v>847,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>283,</v>
+        <v>285,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>830</v>
+        <v>847</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>613</v>
+        <v>640</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>613,</v>
+        <v>640,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>963</v>
+        <v>985</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>963,</v>
+        <v>985,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>613</v>
+        <v>640</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>198,</v>
+        <v>209,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>963</v>
+        <v>985</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>4206</v>
+        <v>4386</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>4206</v>
+        <v>4386</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>198</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 24 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10915A8-0034-CC45-93F8-CD88C3035BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A40702E-662E-8D47-BC6A-7FA67D5C937C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1006,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE15D73-8EAA-6046-85A1-3798C28E97CA}">
   <dimension ref="B1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>428,</v>
+        <v>437,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>8654</v>
+        <v>8878</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>8654,</v>
+        <v>8878,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>5802</v>
+        <v>5941</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1119</v>
+        <v>1134</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1119,</v>
+        <v>1134,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1119</v>
+        <v>1134</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>22767</v>
+        <v>23063</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>22767,</v>
+        <v>23063,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>8654</v>
+        <v>8878</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>495</v>
+        <v>530</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>495,</v>
+        <v>530,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>495</v>
+        <v>530</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>16663</v>
+        <v>17113</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16663,</v>
+        <v>17113,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>22767</v>
+        <v>23063</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>187,</v>
+        <v>192,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>14246</v>
+        <v>14872</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14246,</v>
+        <v>14872,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>6318</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>353,</v>
+        <v>361,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>15682</v>
+        <v>16252</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>15682,</v>
+        <v>16252,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>15682</v>
+        <v>16252</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>560,</v>
+        <v>561,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>14412</v>
+        <v>14974</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14412,</v>
+        <v>14974,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>14412</v>
+        <v>14974</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2483</v>
+        <v>2552</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2483,</v>
+        <v>2552,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2483</v>
+        <v>2552</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>5411</v>
+        <v>5528</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5411,</v>
+        <v>5528,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>5411</v>
+        <v>5528</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>256,</v>
+        <v>265,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>4386</v>
+        <v>4545</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4386,</v>
+        <v>4545,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>10861</v>
+        <v>11172</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>311,</v>
+        <v>333,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>102221</v>
+        <v>105225</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>102221</v>
+        <v>105225</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>7928</v>
+        <v>8326</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>623</v>
+        <v>643</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>623,</v>
+        <v>643,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>623</v>
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>369,</v>
+        <v>371,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>174,</v>
+        <v>183,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>647</v>
+        <v>669</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>647,</v>
+        <v>669,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>647</v>
+        <v>669</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>102221</v>
+        <v>105225</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>102221,</v>
+        <v>105225,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>102221</v>
+        <v>105225</v>
       </c>
       <c r="M14" s="3">
-        <v>16785</v>
+        <v>17372</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1276</v>
+        <v>1289</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1276,</v>
+        <v>1289,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1276</v>
+        <v>1289</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>9409</v>
+        <v>9697</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9409,</v>
+        <v>9697,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3016</v>
+        <v>3122</v>
       </c>
       <c r="M15" s="2">
-        <v>250</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>334,</v>
+        <v>337,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>8358</v>
+        <v>8601</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>8358,</v>
+        <v>8601,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>9409</v>
+        <v>9697</v>
       </c>
       <c r="M16" s="3">
-        <v>1062</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>519</v>
+        <v>543</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>519,</v>
+        <v>543,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>519</v>
+        <v>543</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3016</v>
+        <v>3122</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3016</v>
+        <v>3122</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>8358</v>
+        <v>8601</v>
       </c>
       <c r="M17" s="2">
-        <v>641</v>
+        <v>751</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>953</v>
+        <v>959</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>953,</v>
+        <v>959,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>953</v>
+        <v>959</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>691</v>
+        <v>709</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>691,</v>
+        <v>709,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>691</v>
+        <v>709</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>369,</v>
+        <v>382,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>369</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>204,</v>
+        <v>210,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>425821</v>
+        <v>444222</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>425821,</v>
+        <v>444222,</v>
       </c>
       <c r="K21" s="9">
-        <v>425821</v>
+        <v>444222</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>603</v>
+        <v>624</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>603,</v>
+        <v>624,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>603</v>
+        <v>624</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>287743</v>
+        <v>300758</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>287743,</v>
+        <v>300758,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>537,</v>
+        <v>543,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>138078</v>
+        <v>143464</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>138078,</v>
+        <v>143464,</v>
       </c>
       <c r="K23" s="9">
-        <v>138078</v>
+        <v>143464</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>421,</v>
+        <v>427,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>18738</v>
+        <v>19506</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18738,</v>
+        <v>19506,</v>
       </c>
       <c r="K24" s="9">
-        <v>18738</v>
+        <v>19506</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>689,</v>
+        <v>702,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>634</v>
+        <v>665</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>634,</v>
+        <v>665,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>634</v>
+        <v>665</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>436,</v>
+        <v>444,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1071</v>
+        <v>1115</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1071,</v>
+        <v>1115,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>567</v>
+        <v>591</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>567,</v>
+        <v>591,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1071</v>
+        <v>1115</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43944</v>
+        <v>43946</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1253</v>
+        <v>1268</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1253,</v>
+        <v>1268,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>567</v>
+        <v>591</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 23/04/2020,425821,287743,138078,18738,135</v>
+        <v>9:00 25/04/2020,444222,300758,143464,19506,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1584</v>
+        <v>1633</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1584,</v>
+        <v>1633,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1253</v>
+        <v>1268</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 23/04/2020,102221,9409,8358,3016</v>
+        <v>9:00 25/04/2020,105225,9697,8601,3122</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>208,</v>
+        <v>218,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1584</v>
+        <v>1633</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 23/04/2020,8654,22767,16663,14246,15682,14412,5411,4386,102221</v>
+        <v>9:00 25/04/2020,8878,23063,17113,14872,16252,14974,5528,4545,105225</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>423</v>
+        <v>431</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>423,</v>
+        <v>431,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 23/04/2020,428,1119,495,187,353,560,2483,256,311,623,369,174,647,1276,334,519,953,691,369,204,603,537,421,689,634,436,1071,567,1253,1584,208,423,987,594,326,275,643,973,412,479,755,2069,668,1021,587,596,283,504,2371,509,818,113,587,175,1996,667,601,76,387,423,2826,320,401,466,440,1063,2305,1049,545,776,854,712,1234,548,929,548,615,427,403,781,898,1169,109,244,183,412,718,952,668,448,946,509,1314,171,246,238,369,625,239,347,358,537,13,503,831,699,1751,398,325,476,401,304,425,398,266,1126,510,1405,699,280,345,814,1026,2176,609,307,394,205,244,169,578,504,441,753,677,871,497,955,256,943,570,505,400,206,847,285,640,985,209,4386</v>
+        <v>9:00 25/04/2020,437,1134,530,192,361,561,2552,265,333,643,371,183,669,1289,337,543,959,709,382,210,624,543,427,702,665,444,1115,591,1268,1633,218,431,1038,604,350,272,653,988,429,491,763,2119,698,1053,592,602,293,524,2439,514,841,131,601,198,2034,680,613,82,389,429,2959,342,411,473,471,1071,2381,1111,560,802,857,725,1257,554,951,557,621,451,412,790,912,1208,114,257,190,421,740,966,681,451,953,529,1336,185,256,249,402,639,259,349,382,573,15,514,856,724,1856,402,341,487,424,311,442,411,271,1137,556,1455,717,303,361,850,1037,2288,622,322,407,210,245,177,582,525,448,778,683,880,516,976,276,974,572,529,369,217,877,311,656,997,224,4545</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>987</v>
+        <v>1038</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>987,</v>
+        <v>1038,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>594,</v>
+        <v>604,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="2">
-        <v>987</v>
+      <c r="F35" s="3">
+        <v>1038</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>326</v>
+        <v>350</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>326,</v>
+        <v>350,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>594</v>
+        <v>604</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>275,</v>
+        <v>272,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>326</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>643,</v>
+        <v>653,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>973</v>
+        <v>988</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>973,</v>
+        <v>988,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>643</v>
+        <v>653</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>412</v>
+        <v>429</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>412,</v>
+        <v>429,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>973</v>
+        <v>988</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>479,</v>
+        <v>491,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>412</v>
+        <v>429</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>755</v>
+        <v>763</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>755,</v>
+        <v>763,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>479</v>
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2069</v>
+        <v>2119</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2069,</v>
+        <v>2119,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>755</v>
+        <v>763</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>668</v>
+        <v>698</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>668,</v>
+        <v>698,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2069</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1021</v>
+        <v>1053</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1021,</v>
+        <v>1053,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>668</v>
+        <v>698</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>587,</v>
+        <v>592,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1021</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>596,</v>
+        <v>602,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>587</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>283,</v>
+        <v>293,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>580</v>
+        <v>586</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>504</v>
+        <v>524</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>504,</v>
+        <v>524,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2371</v>
+        <v>2439</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2371,</v>
+        <v>2439,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>504</v>
+        <v>524</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>509,</v>
+        <v>514,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2371</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>818</v>
+        <v>841</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>818,</v>
+        <v>841,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>113,</v>
+        <v>131,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>818</v>
+        <v>841</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>587</v>
+        <v>601</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>587,</v>
+        <v>601,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>113</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>175,</v>
+        <v>198,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>587</v>
+        <v>601</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>1996</v>
+        <v>2034</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1996,</v>
+        <v>2034,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>667</v>
+        <v>680</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>667,</v>
+        <v>680,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>1996</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>601</v>
+        <v>613</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>601,</v>
+        <v>613,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>667</v>
+        <v>680</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>76,</v>
+        <v>82,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>601</v>
+        <v>613</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>387,</v>
+        <v>389,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>423,</v>
+        <v>429,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2826</v>
+        <v>2959</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2826,</v>
+        <v>2959,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>320,</v>
+        <v>342,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2826</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>401,</v>
+        <v>411,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>320</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>466,</v>
+        <v>473,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>401</v>
+        <v>411</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>440</v>
+        <v>471</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>440,</v>
+        <v>471,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>466</v>
+        <v>473</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1063</v>
+        <v>1071</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1063,</v>
+        <v>1071,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>440</v>
+        <v>471</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2305</v>
+        <v>2381</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2305,</v>
+        <v>2381,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1063</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1049</v>
+        <v>1111</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1049,</v>
+        <v>1111,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2305</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>545</v>
+        <v>560</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>545,</v>
+        <v>560,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1049</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>776</v>
+        <v>802</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>776,</v>
+        <v>802,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>545</v>
+        <v>560</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>854,</v>
+        <v>857,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>776</v>
+        <v>802</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>712</v>
+        <v>725</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>712,</v>
+        <v>725,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>854</v>
+        <v>857</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1234</v>
+        <v>1257</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1234,</v>
+        <v>1257,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>712</v>
+        <v>725</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>548,</v>
+        <v>554,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1234</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>929</v>
+        <v>951</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>929,</v>
+        <v>951,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>548</v>
+        <v>554</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>548</v>
+        <v>557</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>548,</v>
+        <v>557,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>929</v>
+        <v>951</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>615,</v>
+        <v>621,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>548</v>
+        <v>557</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>427</v>
+        <v>451</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>427,</v>
+        <v>451,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>615</v>
+        <v>621</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>403,</v>
+        <v>412,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>427</v>
+        <v>451</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>781,</v>
+        <v>790,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>898</v>
+        <v>912</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>898,</v>
+        <v>912,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>781</v>
+        <v>790</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1169</v>
+        <v>1208</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1169,</v>
+        <v>1208,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>898</v>
+        <v>912</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>109,</v>
+        <v>114,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1169</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>244,</v>
+        <v>257,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>183,</v>
+        <v>190,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>244</v>
+        <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>412,</v>
+        <v>421,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>718</v>
+        <v>740</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>718,</v>
+        <v>740,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>952</v>
+        <v>966</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>952,</v>
+        <v>966,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>718</v>
+        <v>740</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>668</v>
+        <v>681</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>668,</v>
+        <v>681,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>952</v>
+        <v>966</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>448,</v>
+        <v>451,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>668</v>
+        <v>681</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>946</v>
+        <v>953</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>946,</v>
+        <v>953,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>509</v>
+        <v>529</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>509,</v>
+        <v>529,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>946</v>
+        <v>953</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1314</v>
+        <v>1336</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1314,</v>
+        <v>1336,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>509</v>
+        <v>529</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>171,</v>
+        <v>185,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1314</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>246,</v>
+        <v>256,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>171</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>238,</v>
+        <v>249,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>369</v>
+        <v>402</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>369,</v>
+        <v>402,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>238</v>
+        <v>249</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>625</v>
+        <v>639</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>625,</v>
+        <v>639,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>369</v>
+        <v>402</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>239,</v>
+        <v>259,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>625</v>
+        <v>639</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>347,</v>
+        <v>349,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>239</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>358</v>
+        <v>382</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>358,</v>
+        <v>382,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>537</v>
+        <v>573</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>537,</v>
+        <v>573,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>358</v>
+        <v>382</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C104" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>13,</v>
+        <v>15,</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>537</v>
+        <v>573</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>503,</v>
+        <v>514,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F105" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>831</v>
+        <v>856</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>831,</v>
+        <v>856,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>503</v>
+        <v>514</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>699</v>
+        <v>724</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>699,</v>
+        <v>724,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>831</v>
+        <v>856</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1751</v>
+        <v>1856</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1751,</v>
+        <v>1856,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>699</v>
+        <v>724</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>398,</v>
+        <v>402,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1751</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>325,</v>
+        <v>341,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>476</v>
+        <v>487</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>476,</v>
+        <v>487,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>325</v>
+        <v>341</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>401</v>
+        <v>424</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>401,</v>
+        <v>424,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>476</v>
+        <v>487</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>304,</v>
+        <v>311,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>401</v>
+        <v>424</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>425</v>
+        <v>442</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>425,</v>
+        <v>442,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>304</v>
+        <v>311</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>398</v>
+        <v>411</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>398,</v>
+        <v>411,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>425</v>
+        <v>442</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>266,</v>
+        <v>271,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>398</v>
+        <v>411</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1126</v>
+        <v>1137</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1126,</v>
+        <v>1137,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>510</v>
+        <v>556</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>510,</v>
+        <v>556,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1126</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1405</v>
+        <v>1455</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1405,</v>
+        <v>1455,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>510</v>
+        <v>556</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>699</v>
+        <v>717</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>699,</v>
+        <v>717,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1405</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>280,</v>
+        <v>303,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>699</v>
+        <v>717</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>345,</v>
+        <v>361,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>280</v>
+        <v>303</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>814</v>
+        <v>850</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>814,</v>
+        <v>850,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>345</v>
+        <v>361</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1026</v>
+        <v>1037</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1026,</v>
+        <v>1037,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>814</v>
+        <v>850</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2176</v>
+        <v>2288</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2176,</v>
+        <v>2288,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1026</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>609</v>
+        <v>622</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>609,</v>
+        <v>622,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2176</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>307,</v>
+        <v>322,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>609</v>
+        <v>622</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>394,</v>
+        <v>407,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>307</v>
+        <v>322</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>205,</v>
+        <v>210,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>394</v>
+        <v>407</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>244,</v>
+        <v>245,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>169,</v>
+        <v>177,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>578,</v>
+        <v>582,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>504</v>
+        <v>525</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>504,</v>
+        <v>525,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>441,</v>
+        <v>448,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>504</v>
+        <v>525</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>753</v>
+        <v>778</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>753,</v>
+        <v>778,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>441</v>
+        <v>448</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>677,</v>
+        <v>683,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>753</v>
+        <v>778</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>871</v>
+        <v>880</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>871,</v>
+        <v>880,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>677</v>
+        <v>683</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>497</v>
+        <v>516</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>497,</v>
+        <v>516,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>871</v>
+        <v>880</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>955</v>
+        <v>976</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>955,</v>
+        <v>976,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>497</v>
+        <v>516</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>256,</v>
+        <v>276,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="2">
-        <v>955</v>
+        <v>976</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>943</v>
+        <v>974</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>943,</v>
+        <v>974,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>570,</v>
+        <v>572,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>943</v>
+        <v>974</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>505,</v>
+        <v>529,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>400,</v>
+        <v>369,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>505</v>
+        <v>529</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>206,</v>
+        <v>217,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>400</v>
+        <v>369</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>847</v>
+        <v>877</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>847,</v>
+        <v>877,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>285</v>
+        <v>311</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>285,</v>
+        <v>311,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>847</v>
+        <v>877</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>640</v>
+        <v>656</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>640,</v>
+        <v>656,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>285</v>
+        <v>311</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>985</v>
+        <v>997</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>985,</v>
+        <v>997,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>640</v>
+        <v>656</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>209,</v>
+        <v>224,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="2">
-        <v>985</v>
+        <v>997</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>4386</v>
+        <v>4545</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>4386</v>
+        <v>4545</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>209</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 26 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A40702E-662E-8D47-BC6A-7FA67D5C937C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C763AE9-F3F6-0B4F-9216-8913613548A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>437,</v>
+        <v>441,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>8878</v>
+        <v>9175</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>8878,</v>
+        <v>9175,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>5941</v>
+        <v>6090</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1134</v>
+        <v>1147</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1134,</v>
+        <v>1147,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1134</v>
+        <v>1147</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>23063</v>
+        <v>23341</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>23063,</v>
+        <v>23341,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>8878</v>
+        <v>9175</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>530</v>
+        <v>544</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>530,</v>
+        <v>544,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>530</v>
+        <v>544</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>17113</v>
+        <v>17582</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17113,</v>
+        <v>17582,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>23063</v>
+        <v>23341</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>192,</v>
+        <v>198,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>14872</v>
+        <v>15431</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14872,</v>
+        <v>15431,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>6546</v>
+        <v>6772</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>361,</v>
+        <v>376,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>16252</v>
+        <v>16709</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16252,</v>
+        <v>16709,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>16252</v>
+        <v>16709</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>561</v>
+        <v>576</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>561,</v>
+        <v>576,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>561</v>
+        <v>576</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>14974</v>
+        <v>15453</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>14974,</v>
+        <v>15453,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>14974</v>
+        <v>15453</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2552</v>
+        <v>2618</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2552,</v>
+        <v>2618,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2552</v>
+        <v>2618</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>5528</v>
+        <v>5701</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5528,</v>
+        <v>5701,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>5528</v>
+        <v>5701</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>265,</v>
+        <v>271,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>4545</v>
+        <v>4659</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4545,</v>
+        <v>4659,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>11172</v>
+        <v>11492</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>333,</v>
+        <v>350,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>105225</v>
+        <v>108051</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>105225</v>
+        <v>108051</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>8326</v>
+        <v>8659</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>643</v>
+        <v>659</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>643,</v>
+        <v>659,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>643</v>
+        <v>659</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>371,</v>
+        <v>385,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>371</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>183,</v>
+        <v>185,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>669</v>
+        <v>703</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>669,</v>
+        <v>703,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>669</v>
+        <v>703</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>105225</v>
+        <v>108051</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>105225,</v>
+        <v>108051,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>105225</v>
+        <v>108051</v>
       </c>
       <c r="M14" s="3">
-        <v>17372</v>
+        <v>18083</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1289</v>
+        <v>1298</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1289,</v>
+        <v>1298,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1289</v>
+        <v>1298</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>9697</v>
+        <v>10051</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9697,</v>
+        <v>10051,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3122</v>
+        <v>3226</v>
       </c>
       <c r="M15" s="2">
-        <v>263</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>337,</v>
+        <v>339,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>8601</v>
+        <v>8900</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>8601,</v>
+        <v>8900,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>9697</v>
+        <v>10051</v>
       </c>
       <c r="M16" s="3">
-        <v>1120</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>543,</v>
+        <v>559,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3122</v>
+        <v>3226</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3122</v>
+        <v>3226</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>8601</v>
+        <v>8900</v>
       </c>
       <c r="M17" s="2">
-        <v>751</v>
+        <v>774</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>959</v>
+        <v>968</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>959,</v>
+        <v>968,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="2">
-        <v>959</v>
+        <v>968</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>709</v>
+        <v>730</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>709,</v>
+        <v>730,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>709</v>
+        <v>730</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>382</v>
+        <v>396</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>382,</v>
+        <v>396,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>382</v>
+        <v>396</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>210,</v>
+        <v>216,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>444222</v>
+        <v>517836</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>444222,</v>
+        <v>517836,</v>
       </c>
       <c r="K21" s="9">
-        <v>444222</v>
+        <v>517836</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>624</v>
+        <v>638</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>624,</v>
+        <v>638,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>624</v>
+        <v>638</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>300758</v>
+        <v>369459</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>300758,</v>
+        <v>369459,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>543,</v>
+        <v>549,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>143464</v>
+        <v>148377</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>143464,</v>
+        <v>148377,</v>
       </c>
       <c r="K23" s="9">
-        <v>143464</v>
+        <v>148377</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>427,</v>
+        <v>439,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>19506</v>
+        <v>20319</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>19506,</v>
+        <v>20319,</v>
       </c>
       <c r="K24" s="9">
-        <v>19506</v>
+        <v>20319</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>702</v>
+        <v>734</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>702,</v>
+        <v>734,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>702</v>
+        <v>734</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>665</v>
+        <v>681</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>665,</v>
+        <v>681,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>665</v>
+        <v>681</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>444,</v>
+        <v>454,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1115</v>
+        <v>1152</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1115,</v>
+        <v>1152,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>444</v>
+        <v>454</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>591,</v>
+        <v>602,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1115</v>
+        <v>1152</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43946</v>
+        <v>43947</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1268</v>
+        <v>1280</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1268,</v>
+        <v>1280,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 25/04/2020,444222,300758,143464,19506,135</v>
+        <v>9:00 26/04/2020,517836,369459,148377,20319,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1633</v>
+        <v>1675</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1633,</v>
+        <v>1675,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1268</v>
+        <v>1280</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 25/04/2020,105225,9697,8601,3122</v>
+        <v>9:00 26/04/2020,108051,10051,8900,3226</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>218,</v>
+        <v>223,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1633</v>
+        <v>1675</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 25/04/2020,8878,23063,17113,14872,16252,14974,5528,4545,105225</v>
+        <v>9:00 26/04/2020,9175,23341,17582,15431,16709,15453,5701,4659,108051</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>431,</v>
+        <v>440,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 25/04/2020,437,1134,530,192,361,561,2552,265,333,643,371,183,669,1289,337,543,959,709,382,210,624,543,427,702,665,444,1115,591,1268,1633,218,431,1038,604,350,272,653,988,429,491,763,2119,698,1053,592,602,293,524,2439,514,841,131,601,198,2034,680,613,82,389,429,2959,342,411,473,471,1071,2381,1111,560,802,857,725,1257,554,951,557,621,451,412,790,912,1208,114,257,190,421,740,966,681,451,953,529,1336,185,256,249,402,639,259,349,382,573,15,514,856,724,1856,402,341,487,424,311,442,411,271,1137,556,1455,717,303,361,850,1037,2288,622,322,407,210,245,177,582,525,448,778,683,880,516,976,276,974,572,529,369,217,877,311,656,997,224,4545</v>
+        <v>9:00 26/04/2020,441,1147,544,198,376,576,2618,271,350,659,385,185,703,1298,339,559,968,730,396,216,638,549,439,734,681,454,1152,602,1280,1675,223,440,1048,629,372,287,661,993,452,499,775,2202,725,1084,602,606,299,551,2519,521,854,149,605,211,2092,694,615,86,393,447,3126,355,416,484,479,1087,2461,1171,579,821,872,748,1278,564,976,574,624,472,425,811,922,1268,123,280,200,429,776,975,692,468,993,549,1369,188,266,260,410,645,269,352,395,589,18,528,870,739,1901,409,345,496,428,312,464,429,275,1142,576,1506,729,320,380,877,1066,2333,631,332,417,219,256,182,586,534,461,798,693,883,533,1008,283,997,573,549,385,219,901,325,693,1021,232,4659</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1038</v>
+        <v>1048</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1038,</v>
+        <v>1048,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>431</v>
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>604</v>
+        <v>629</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>604,</v>
+        <v>629,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1038</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>350,</v>
+        <v>372,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>604</v>
+        <v>629</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>272,</v>
+        <v>287,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>350</v>
+        <v>372</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>653</v>
+        <v>661</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>653,</v>
+        <v>661,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>272</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>988,</v>
+        <v>993,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>653</v>
+        <v>661</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>429</v>
+        <v>452</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>429,</v>
+        <v>452,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <v>988</v>
+        <v>993</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>491,</v>
+        <v>499,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>429</v>
+        <v>452</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>763</v>
+        <v>775</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>763,</v>
+        <v>775,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2119</v>
+        <v>2202</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2119,</v>
+        <v>2202,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>763</v>
+        <v>775</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>698</v>
+        <v>725</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>698,</v>
+        <v>725,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2119</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1053</v>
+        <v>1084</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1053,</v>
+        <v>1084,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>698</v>
+        <v>725</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>592</v>
+        <v>602</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>592,</v>
+        <v>602,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1053</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>602,</v>
+        <v>606,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>592</v>
+        <v>602</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>293,</v>
+        <v>299,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>524</v>
+        <v>551</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>524,</v>
+        <v>551,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2439</v>
+        <v>2519</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2439,</v>
+        <v>2519,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>524</v>
+        <v>551</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>514,</v>
+        <v>521,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2439</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>841</v>
+        <v>854</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>841,</v>
+        <v>854,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>514</v>
+        <v>521</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>131,</v>
+        <v>149,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>841</v>
+        <v>854</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>601,</v>
+        <v>605,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>131</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>198,</v>
+        <v>211,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>601</v>
+        <v>605</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2034</v>
+        <v>2092</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2034,</v>
+        <v>2092,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>198</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>680</v>
+        <v>694</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>680,</v>
+        <v>694,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2034</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>613,</v>
+        <v>615,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>680</v>
+        <v>694</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>82,</v>
+        <v>86,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>389,</v>
+        <v>393,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>429</v>
+        <v>447</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>429,</v>
+        <v>447,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>2959</v>
+        <v>3126</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2959,</v>
+        <v>3126,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>429</v>
+        <v>447</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>342,</v>
+        <v>355,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>2959</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>411,</v>
+        <v>416,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>342</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>473,</v>
+        <v>484,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>471,</v>
+        <v>479,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>473</v>
+        <v>484</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1071</v>
+        <v>1087</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1071,</v>
+        <v>1087,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2381</v>
+        <v>2461</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2381,</v>
+        <v>2461,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1071</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1111</v>
+        <v>1171</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1111,</v>
+        <v>1171,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2381</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>560</v>
+        <v>579</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>560,</v>
+        <v>579,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1111</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>802</v>
+        <v>821</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>802,</v>
+        <v>821,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>560</v>
+        <v>579</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>857</v>
+        <v>872</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>857,</v>
+        <v>872,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>802</v>
+        <v>821</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>725</v>
+        <v>748</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>725,</v>
+        <v>748,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>857</v>
+        <v>872</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1257</v>
+        <v>1278</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1257,</v>
+        <v>1278,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>725</v>
+        <v>748</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>554,</v>
+        <v>564,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1257</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>951</v>
+        <v>976</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>951,</v>
+        <v>976,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>554</v>
+        <v>564</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>557</v>
+        <v>574</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>557,</v>
+        <v>574,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="2">
-        <v>951</v>
+        <v>976</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>621,</v>
+        <v>624,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>557</v>
+        <v>574</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>451</v>
+        <v>472</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>451,</v>
+        <v>472,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>412,</v>
+        <v>425,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>451</v>
+        <v>472</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>790</v>
+        <v>811</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>790,</v>
+        <v>811,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>412</v>
+        <v>425</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>912</v>
+        <v>922</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>912,</v>
+        <v>922,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>790</v>
+        <v>811</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1208</v>
+        <v>1268</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1208,</v>
+        <v>1268,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>912</v>
+        <v>922</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>114,</v>
+        <v>123,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1208</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>257,</v>
+        <v>280,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>190,</v>
+        <v>200,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>257</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>421,</v>
+        <v>429,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>740</v>
+        <v>776</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>740,</v>
+        <v>776,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>966</v>
+        <v>975</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>966,</v>
+        <v>975,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>740</v>
+        <v>776</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>681</v>
+        <v>692</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>681,</v>
+        <v>692,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>966</v>
+        <v>975</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>451</v>
+        <v>468</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>451,</v>
+        <v>468,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>681</v>
+        <v>692</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>953</v>
+        <v>993</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>953,</v>
+        <v>993,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>451</v>
+        <v>468</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>529</v>
+        <v>549</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>529,</v>
+        <v>549,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="2">
-        <v>953</v>
+        <v>993</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1336</v>
+        <v>1369</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1336,</v>
+        <v>1369,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>529</v>
+        <v>549</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>185,</v>
+        <v>188,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1336</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>256,</v>
+        <v>266,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>249,</v>
+        <v>260,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>402,</v>
+        <v>410,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>639</v>
+        <v>645</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>639,</v>
+        <v>645,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>259,</v>
+        <v>269,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>639</v>
+        <v>645</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>349,</v>
+        <v>352,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>382,</v>
+        <v>395,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>573</v>
+        <v>589</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>573,</v>
+        <v>589,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>382</v>
+        <v>395</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C104" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>15,</v>
+        <v>18,</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>573</v>
+        <v>589</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>514</v>
+        <v>528</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>514,</v>
+        <v>528,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F105" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>856</v>
+        <v>870</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>856,</v>
+        <v>870,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>514</v>
+        <v>528</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>724,</v>
+        <v>739,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>856</v>
+        <v>870</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1856</v>
+        <v>1901</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1856,</v>
+        <v>1901,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>724</v>
+        <v>739</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>402,</v>
+        <v>409,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1856</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>341,</v>
+        <v>345,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>487</v>
+        <v>496</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>487,</v>
+        <v>496,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>424,</v>
+        <v>428,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>487</v>
+        <v>496</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>311,</v>
+        <v>312,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>442</v>
+        <v>464</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>442,</v>
+        <v>464,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>411,</v>
+        <v>429,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>442</v>
+        <v>464</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>271,</v>
+        <v>275,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>411</v>
+        <v>429</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1137</v>
+        <v>1142</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1137,</v>
+        <v>1142,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>556</v>
+        <v>576</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>556,</v>
+        <v>576,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1137</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1455</v>
+        <v>1506</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1455,</v>
+        <v>1506,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>556</v>
+        <v>576</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>717</v>
+        <v>729</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>717,</v>
+        <v>729,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1455</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>303,</v>
+        <v>320,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>717</v>
+        <v>729</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>361</v>
+        <v>380</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>361,</v>
+        <v>380,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>303</v>
+        <v>320</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>850</v>
+        <v>877</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>850,</v>
+        <v>877,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>361</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1037</v>
+        <v>1066</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1037,</v>
+        <v>1066,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>850</v>
+        <v>877</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2288</v>
+        <v>2333</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2288,</v>
+        <v>2333,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1037</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>622,</v>
+        <v>631,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2288</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>322,</v>
+        <v>332,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>622</v>
+        <v>631</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>407,</v>
+        <v>417,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>322</v>
+        <v>332</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>210,</v>
+        <v>219,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>407</v>
+        <v>417</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>245,</v>
+        <v>256,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>177,</v>
+        <v>182,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>582,</v>
+        <v>586,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>525</v>
+        <v>534</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>525,</v>
+        <v>534,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>448,</v>
+        <v>461,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>525</v>
+        <v>534</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>778</v>
+        <v>798</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>778,</v>
+        <v>798,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>448</v>
+        <v>461</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>683,</v>
+        <v>693,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>778</v>
+        <v>798</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>880,</v>
+        <v>883,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>683</v>
+        <v>693</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>516</v>
+        <v>533</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>516,</v>
+        <v>533,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>880</v>
+        <v>883</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>976</v>
+        <v>1008</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>976,</v>
+        <v>1008,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>516</v>
+        <v>533</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>276,</v>
+        <v>283,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F140" s="2">
-        <v>976</v>
+      <c r="F140" s="3">
+        <v>1008</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>974</v>
+        <v>997</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>974,</v>
+        <v>997,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>572,</v>
+        <v>573,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="2">
-        <v>974</v>
+        <v>997</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>529</v>
+        <v>549</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>529,</v>
+        <v>549,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>369</v>
+        <v>385</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>369,</v>
+        <v>385,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>529</v>
+        <v>549</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>217,</v>
+        <v>219,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>369</v>
+        <v>385</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>877</v>
+        <v>901</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>877,</v>
+        <v>901,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>311,</v>
+        <v>325,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>877</v>
+        <v>901</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>656</v>
+        <v>693</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>656,</v>
+        <v>693,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>311</v>
+        <v>325</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>997</v>
+        <v>1021</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>997,</v>
+        <v>1021,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>656</v>
+        <v>693</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>224,</v>
+        <v>232,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F150" s="2">
-        <v>997</v>
+      <c r="F150" s="3">
+        <v>1021</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>4545</v>
+        <v>4659</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>4545</v>
+        <v>4659</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 27 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802C3A7F-F63E-1C44-9710-34EF4E25CCA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9683D239-91BB-5B46-93ED-3410DAF7FBC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE15D73-8EAA-6046-85A1-3798C28E97CA}">
   <dimension ref="B1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F151"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>442,</v>
+        <v>445,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>9325</v>
+        <v>9569</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>9325,</v>
+        <v>9569,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>6187</v>
+        <v>6307</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1155</v>
+        <v>1161</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1155,</v>
+        <v>1161,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1155</v>
+        <v>1161</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>23608</v>
+        <v>23833</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>23608,</v>
+        <v>23833,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>9325</v>
+        <v>9569</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>553</v>
+        <v>569</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>553,</v>
+        <v>569,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>553</v>
+        <v>569</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>17975</v>
+        <v>18359</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17975,</v>
+        <v>18359,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>23608</v>
+        <v>23833</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1172,17 +1172,17 @@
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>15822</v>
+        <v>16292</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>15822,</v>
+        <v>16292,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>6931</v>
+        <v>7070</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>381,</v>
+        <v>389,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>17089</v>
+        <v>17483</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17089,</v>
+        <v>17483,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>17089</v>
+        <v>17483</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>581,</v>
+        <v>592,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>15810</v>
+        <v>16128</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>15810,</v>
+        <v>16128,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>15810</v>
+        <v>16128</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2659</v>
+        <v>2705</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2659,</v>
+        <v>2705,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2659</v>
+        <v>2705</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>5797</v>
+        <v>5902</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5797,</v>
+        <v>5902,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>5797</v>
+        <v>5902</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>281,</v>
+        <v>289,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>4777</v>
+        <v>4901</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4777,</v>
+        <v>4901,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>11788</v>
+        <v>12052</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>353,</v>
+        <v>377,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>110203</v>
+        <v>112467</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>110203</v>
+        <v>112467</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>8891</v>
+        <v>9222</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>698,</v>
+        <v>711,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>698</v>
+        <v>711</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>389,</v>
+        <v>391,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>191,</v>
+        <v>200,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>726</v>
+        <v>768</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>726,</v>
+        <v>768,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>726</v>
+        <v>768</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>110203</v>
+        <v>112467</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>110203,</v>
+        <v>112467,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>110203</v>
+        <v>112467</v>
       </c>
       <c r="M14" s="3">
-        <v>18419</v>
+        <v>18748</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1310</v>
+        <v>1320</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1310,</v>
+        <v>1320,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1310</v>
+        <v>1320</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>10324</v>
+        <v>10521</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10324,</v>
+        <v>10521,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3308</v>
+        <v>3374</v>
       </c>
       <c r="M15" s="2">
-        <v>294</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>343,</v>
+        <v>345,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>9078</v>
+        <v>9280</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9078,</v>
+        <v>9280,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>10324</v>
+        <v>10521</v>
       </c>
       <c r="M16" s="3">
-        <v>1231</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>571,</v>
+        <v>576,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3308</v>
+        <v>3374</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3308</v>
+        <v>3374</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>9078</v>
+        <v>9280</v>
       </c>
       <c r="M17" s="2">
-        <v>788</v>
+        <v>796</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>998</v>
+        <v>1007</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>998,</v>
+        <v>1007,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F18" s="2">
-        <v>998</v>
+      <c r="F18" s="3">
+        <v>1007</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>745</v>
+        <v>765</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>745,</v>
+        <v>765,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>745</v>
+        <v>765</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>407,</v>
+        <v>425,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>407</v>
+        <v>425</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>218,</v>
+        <v>229,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>543413</v>
+        <v>569768</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>543413,</v>
+        <v>569768,</v>
       </c>
       <c r="K21" s="9">
-        <v>543413</v>
+        <v>569768</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>654</v>
+        <v>673</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>654,</v>
+        <v>673,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>654</v>
+        <v>673</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>390573</v>
+        <v>412619</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>390573,</v>
+        <v>412619,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>557,</v>
+        <v>563,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>152840</v>
+        <v>157149</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>152840,</v>
+        <v>157149,</v>
       </c>
       <c r="K23" s="9">
-        <v>152840</v>
+        <v>157149</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>441,</v>
+        <v>451,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>20732</v>
+        <v>21092</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20732,</v>
+        <v>21092,</v>
       </c>
       <c r="K24" s="9">
-        <v>20732</v>
+        <v>21092</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>757</v>
+        <v>782</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>757,</v>
+        <v>782,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>757</v>
+        <v>782</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>702</v>
+        <v>725</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>702,</v>
+        <v>725,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>702</v>
+        <v>725</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>459,</v>
+        <v>464,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1193</v>
+        <v>1233</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1193,</v>
+        <v>1233,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>621,</v>
+        <v>629,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1193</v>
+        <v>1233</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43947</v>
+        <v>43948</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1310</v>
+        <v>1325</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1310,</v>
+        <v>1325,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 26/04/2020,543413,390573,152840,20732,135</v>
+        <v>9:00 27/04/2020,569768,412619,157149,21092,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1697</v>
+        <v>1734</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1697,</v>
+        <v>1734,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1310</v>
+        <v>1325</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 26/04/2020,110203,10324,9078,3308</v>
+        <v>9:00 27/04/2020,112467,10521,9280,3374</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>232,</v>
+        <v>239,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1697</v>
+        <v>1734</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 26/04/2020,9325,23608,17975,15822,17089,15810,5797,4777,110203</v>
+        <v>9:00 27/04/2020,9569,23833,18359,16292,17483,16128,5902,4901,112467</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>441,</v>
+        <v>451,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 26/04/2020,442,1155,553,201,381,581,2659,281,353,698,389,191,726,1310,343,571,998,745,407,218,654,557,441,757,702,459,1193,621,1310,1697,232,441,1063,643,372,291,685,1005,472,504,781,2244,746,1098,607,611,299,592,2577,526,861,159,607,231,2101,698,620,101,397,451,3185,378,424,495,495,1101,2517,1209,592,836,878,759,1308,566,989,580,628,481,432,820,926,1315,125,296,205,438,803,984,695,485,1008,561,1413,189,268,268,426,649,278,353,403,605,19,547,886,742,1928,418,354,519,441,321,486,437,277,1150,584,1560,750,325,395,896,1078,2381,640,337,422,222,261,182,586,542,469,821,697,889,550,1031,291,1019,578,565,391,224,920,339,705,1035,242,4777</v>
+        <v>9:00 27/04/2020,445,1161,569,201,389,592,2705,289,377,711,391,200,768,1320,345,576,1007,765,425,229,673,563,451,782,725,464,1233,629,1325,1734,239,451,1100,652,391,297,691,1014,501,521,809,2320,750,1112,611,612,301,599,2624,531,869,165,616,244,2141,701,626,103,401,451,3232,396,427,521,496,1110,2585,1273,606,858,886,781,1333,567,1011,586,632,496,436,828,935,1355,128,313,210,440,836,990,709,488,1014,570,1452,190,272,270,437,652,294,356,414,616,19,558,913,746,1952,424,361,538,454,333,495,439,282,1160,596,1595,765,328,409,936,1093,2434,651,347,430,225,265,199,591,553,478,836,704,893,558,1054,300,1047,583,580,394,229,944,347,742,1047,251,4901</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1063</v>
+        <v>1100</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1063,</v>
+        <v>1100,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>441</v>
+        <v>451</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>643,</v>
+        <v>652,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1063</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>372</v>
+        <v>391</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>372,</v>
+        <v>391,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>643</v>
+        <v>652</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>291,</v>
+        <v>297,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>372</v>
+        <v>391</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>685,</v>
+        <v>691,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1005</v>
+        <v>1014</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1005,</v>
+        <v>1014,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>685</v>
+        <v>691</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>472</v>
+        <v>501</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>472,</v>
+        <v>501,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1005</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>504</v>
+        <v>521</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>504,</v>
+        <v>521,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>472</v>
+        <v>501</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>781</v>
+        <v>809</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>781,</v>
+        <v>809,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>504</v>
+        <v>521</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2244</v>
+        <v>2320</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2244,</v>
+        <v>2320,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>781</v>
+        <v>809</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>746,</v>
+        <v>750,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2244</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1098</v>
+        <v>1112</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1098,</v>
+        <v>1112,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>746</v>
+        <v>750</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>607,</v>
+        <v>611,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1098</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>611,</v>
+        <v>612,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>607</v>
+        <v>611</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>299,</v>
+        <v>301,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>592,</v>
+        <v>599,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2577</v>
+        <v>2624</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2577,</v>
+        <v>2624,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>592</v>
+        <v>599</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>526,</v>
+        <v>531,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2577</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>861</v>
+        <v>869</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>861,</v>
+        <v>869,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>526</v>
+        <v>531</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>159,</v>
+        <v>165,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>861</v>
+        <v>869</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>607</v>
+        <v>616</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>607,</v>
+        <v>616,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>231,</v>
+        <v>244,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>607</v>
+        <v>616</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2101</v>
+        <v>2141</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2101,</v>
+        <v>2141,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>231</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>698,</v>
+        <v>701,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2101</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>620</v>
+        <v>626</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>620,</v>
+        <v>626,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>101,</v>
+        <v>103,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>620</v>
+        <v>626</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>397,</v>
+        <v>401,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2507,7 +2507,7 @@
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,11 +2516,11 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3185</v>
+        <v>3232</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3185,</v>
+        <v>3232,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>378</v>
+        <v>396</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>378,</v>
+        <v>396,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3185</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>424,</v>
+        <v>427,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>378</v>
+        <v>396</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>495</v>
+        <v>521</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>495,</v>
+        <v>521,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>495,</v>
+        <v>496,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>495</v>
+        <v>521</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1101</v>
+        <v>1110</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1101,</v>
+        <v>1110,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2517</v>
+        <v>2585</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2517,</v>
+        <v>2585,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1101</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1209</v>
+        <v>1273</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1209,</v>
+        <v>1273,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2517</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>592</v>
+        <v>606</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>592,</v>
+        <v>606,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1209</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>836</v>
+        <v>858</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>836,</v>
+        <v>858,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>592</v>
+        <v>606</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>878</v>
+        <v>886</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>878,</v>
+        <v>886,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>836</v>
+        <v>858</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>759</v>
+        <v>781</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>759,</v>
+        <v>781,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>878</v>
+        <v>886</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1308</v>
+        <v>1333</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1308,</v>
+        <v>1333,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>566,</v>
+        <v>567,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1308</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>989</v>
+        <v>1011</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>989,</v>
+        <v>1011,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>580,</v>
+        <v>586,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F77" s="2">
-        <v>989</v>
+      <c r="F77" s="3">
+        <v>1011</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>628,</v>
+        <v>632,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>580</v>
+        <v>586</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>481</v>
+        <v>496</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>481,</v>
+        <v>496,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>628</v>
+        <v>632</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>432,</v>
+        <v>436,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>481</v>
+        <v>496</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>820</v>
+        <v>828</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>820,</v>
+        <v>828,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>926,</v>
+        <v>935,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>820</v>
+        <v>828</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1315</v>
+        <v>1355</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1315,</v>
+        <v>1355,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>926</v>
+        <v>935</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>125,</v>
+        <v>128,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1315</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>296,</v>
+        <v>313,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>205,</v>
+        <v>210,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>296</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>438,</v>
+        <v>440,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>803</v>
+        <v>836</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>803,</v>
+        <v>836,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>984,</v>
+        <v>990,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>803</v>
+        <v>836</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>695</v>
+        <v>709</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>695,</v>
+        <v>709,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="2">
-        <v>984</v>
+        <v>990</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>485,</v>
+        <v>488,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>695</v>
+        <v>709</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1008,</v>
+        <v>1014,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>561</v>
+        <v>570</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>561,</v>
+        <v>570,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1008</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1413</v>
+        <v>1452</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1413,</v>
+        <v>1452,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>561</v>
+        <v>570</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>189,</v>
+        <v>190,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1413</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>268,</v>
+        <v>272,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>268,</v>
+        <v>270,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>426</v>
+        <v>437</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>426,</v>
+        <v>437,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>649,</v>
+        <v>652,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>426</v>
+        <v>437</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>278,</v>
+        <v>294,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>649</v>
+        <v>652</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>353,</v>
+        <v>356,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>403,</v>
+        <v>414,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>605</v>
+        <v>616</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>605,</v>
+        <v>616,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>403</v>
+        <v>414</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>605</v>
+        <v>616</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>547,</v>
+        <v>558,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>886</v>
+        <v>913</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>886,</v>
+        <v>913,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>547</v>
+        <v>558</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>742,</v>
+        <v>746,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>886</v>
+        <v>913</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1928</v>
+        <v>1952</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1928,</v>
+        <v>1952,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>742</v>
+        <v>746</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>418,</v>
+        <v>424,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1928</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>354,</v>
+        <v>361,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>519</v>
+        <v>538</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>519,</v>
+        <v>538,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>441,</v>
+        <v>454,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>519</v>
+        <v>538</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>321,</v>
+        <v>333,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>441</v>
+        <v>454</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>486</v>
+        <v>495</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>486,</v>
+        <v>495,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>437,</v>
+        <v>439,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>486</v>
+        <v>495</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>277,</v>
+        <v>282,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1150</v>
+        <v>1160</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1150,</v>
+        <v>1160,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>584,</v>
+        <v>596,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1150</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1560</v>
+        <v>1595</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1560,</v>
+        <v>1595,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>584</v>
+        <v>596</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>750</v>
+        <v>765</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>750,</v>
+        <v>765,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1560</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>325,</v>
+        <v>328,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>750</v>
+        <v>765</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>395,</v>
+        <v>409,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>896</v>
+        <v>936</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>896,</v>
+        <v>936,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>395</v>
+        <v>409</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1078</v>
+        <v>1093</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1078,</v>
+        <v>1093,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>896</v>
+        <v>936</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2381</v>
+        <v>2434</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2381,</v>
+        <v>2434,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1078</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>640</v>
+        <v>651</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>640,</v>
+        <v>651,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2381</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>337,</v>
+        <v>347,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>640</v>
+        <v>651</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>422,</v>
+        <v>430,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>222,</v>
+        <v>225,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>422</v>
+        <v>430</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>261,</v>
+        <v>265,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>182,</v>
+        <v>199,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>586,</v>
+        <v>591,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>182</v>
+        <v>199</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>542,</v>
+        <v>553,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>586</v>
+        <v>591</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>469,</v>
+        <v>478,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>542</v>
+        <v>553</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>821</v>
+        <v>836</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>821,</v>
+        <v>836,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>469</v>
+        <v>478</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>697,</v>
+        <v>704,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>821</v>
+        <v>836</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>889,</v>
+        <v>893,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>697</v>
+        <v>704</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>550</v>
+        <v>558</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>550,</v>
+        <v>558,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>889</v>
+        <v>893</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1031</v>
+        <v>1054</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1031,</v>
+        <v>1054,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>291,</v>
+        <v>300,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1031</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1019</v>
+        <v>1047</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1019,</v>
+        <v>1047,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>291</v>
+        <v>300</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>578,</v>
+        <v>583,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1019</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>565</v>
+        <v>580</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>565,</v>
+        <v>580,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>578</v>
+        <v>583</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>391,</v>
+        <v>394,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>565</v>
+        <v>580</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>224,</v>
+        <v>229,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>920</v>
+        <v>944</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>920,</v>
+        <v>944,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>339,</v>
+        <v>347,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>920</v>
+        <v>944</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>705</v>
+        <v>742</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>705,</v>
+        <v>742,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1035</v>
+        <v>1047</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1035,</v>
+        <v>1047,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>705</v>
+        <v>742</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>242,</v>
+        <v>251,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1035</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>4777</v>
+        <v>4901</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>4777</v>
+        <v>4901</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 28 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9683D239-91BB-5B46-93ED-3410DAF7FBC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C1BCB5-7D75-1A4B-8EFA-CD46B9E66F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1006,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE15D73-8EAA-6046-85A1-3798C28E97CA}">
   <dimension ref="B1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -1064,17 +1064,17 @@
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>9569</v>
+        <v>9907</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>9569,</v>
+        <v>9907,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>6307</v>
+        <v>6411</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1161</v>
+        <v>1170</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1161,</v>
+        <v>1170,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1161</v>
+        <v>1170</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>23833</v>
+        <v>23979</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>23833,</v>
+        <v>23979,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>9569</v>
+        <v>9907</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>569</v>
+        <v>590</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>569,</v>
+        <v>590,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>569</v>
+        <v>590</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>18359</v>
+        <v>18804</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18359,</v>
+        <v>18804,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>23833</v>
+        <v>23979</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>201,</v>
+        <v>203,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>16292</v>
+        <v>16673</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16292,</v>
+        <v>16673,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>7070</v>
+        <v>7174</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>389</v>
+        <v>424</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>389,</v>
+        <v>424,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>389</v>
+        <v>424</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>17483</v>
+        <v>17823</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17483,</v>
+        <v>17823,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>17483</v>
+        <v>17823</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>592,</v>
+        <v>596,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>16128</v>
+        <v>16323</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16128,</v>
+        <v>16323,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>16128</v>
+        <v>16323</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2705</v>
+        <v>2733</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2705,</v>
+        <v>2733,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2705</v>
+        <v>2733</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>5902</v>
+        <v>5986</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5902,</v>
+        <v>5986,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>5902</v>
+        <v>5986</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>289,</v>
+        <v>293,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>4901</v>
+        <v>4961</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4901,</v>
+        <v>4961,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>12052</v>
+        <v>12393</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>377,</v>
+        <v>388,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>112467</v>
+        <v>114456</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>112467</v>
+        <v>114456</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>9222</v>
+        <v>9499</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>711,</v>
+        <v>717,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>711</v>
+        <v>717</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>391,</v>
+        <v>397,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>391</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>200,</v>
+        <v>201,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>768</v>
+        <v>795</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>768,</v>
+        <v>795,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>768</v>
+        <v>795</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>112467</v>
+        <v>114456</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>112467,</v>
+        <v>114456,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>112467</v>
+        <v>114456</v>
       </c>
       <c r="M14" s="3">
-        <v>18748</v>
+        <v>19294</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1320</v>
+        <v>1328</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1320,</v>
+        <v>1328,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1320</v>
+        <v>1328</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>10521</v>
+        <v>10721</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10521,</v>
+        <v>10721,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3374</v>
+        <v>3408</v>
       </c>
       <c r="M15" s="2">
-        <v>299</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>345,</v>
+        <v>346,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>9280</v>
+        <v>9512</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9280,</v>
+        <v>9512,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>10521</v>
+        <v>10721</v>
       </c>
       <c r="M16" s="3">
-        <v>1249</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>576,</v>
+        <v>584,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3374</v>
+        <v>3408</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3374</v>
+        <v>3408</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>9280</v>
+        <v>9512</v>
       </c>
       <c r="M17" s="2">
-        <v>796</v>
+        <v>813</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1007</v>
+        <v>1016</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1007,</v>
+        <v>1016,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1007</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>765</v>
+        <v>784</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>765,</v>
+        <v>784,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>765</v>
+        <v>784</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>425,</v>
+        <v>429,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>229,</v>
+        <v>231,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>569768</v>
+        <v>599339</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>569768,</v>
+        <v>599339,</v>
       </c>
       <c r="K21" s="9">
-        <v>569768</v>
+        <v>599339</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>673</v>
+        <v>703</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>673,</v>
+        <v>703,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>673</v>
+        <v>703</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>412619</v>
+        <v>438194</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>412619,</v>
+        <v>438194,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>563,</v>
+        <v>564,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>157149</v>
+        <v>161145</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>157149,</v>
+        <v>161145,</v>
       </c>
       <c r="K23" s="9">
-        <v>157149</v>
+        <v>161145</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>451,</v>
+        <v>456,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>21092</v>
+        <v>21678</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>21092,</v>
+        <v>21678,</v>
       </c>
       <c r="K24" s="9">
-        <v>21092</v>
+        <v>21678</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>782</v>
+        <v>812</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>782,</v>
+        <v>812,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>782</v>
+        <v>812</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>725</v>
+        <v>743</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>725,</v>
+        <v>743,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>725</v>
+        <v>743</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>464,</v>
+        <v>473,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1233</v>
+        <v>1256</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1233,</v>
+        <v>1256,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>629,</v>
+        <v>636,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1233</v>
+        <v>1256</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43948</v>
+        <v>43949</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1902,11 +1902,11 @@
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 27/04/2020,569768,412619,157149,21092,135</v>
+        <v>9:00 28/04/2020,599339,438194,161145,21678,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,11 +1915,11 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1734</v>
+        <v>1761</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1734,</v>
+        <v>1761,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 27/04/2020,112467,10521,9280,3374</v>
+        <v>9:00 28/04/2020,114456,10721,9512,3408</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>239,</v>
+        <v>244,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1734</v>
+        <v>1761</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 27/04/2020,9569,23833,18359,16292,17483,16128,5902,4901,112467</v>
+        <v>9:00 28/04/2020,9907,23979,18804,16673,17823,16323,5986,4961,114456</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>451,</v>
+        <v>456,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 27/04/2020,445,1161,569,201,389,592,2705,289,377,711,391,200,768,1320,345,576,1007,765,425,229,673,563,451,782,725,464,1233,629,1325,1734,239,451,1100,652,391,297,691,1014,501,521,809,2320,750,1112,611,612,301,599,2624,531,869,165,616,244,2141,701,626,103,401,451,3232,396,427,521,496,1110,2585,1273,606,858,886,781,1333,567,1011,586,632,496,436,828,935,1355,128,313,210,440,836,990,709,488,1014,570,1452,190,272,270,437,652,294,356,414,616,19,558,913,746,1952,424,361,538,454,333,495,439,282,1160,596,1595,765,328,409,936,1093,2434,651,347,430,225,265,199,591,553,478,836,704,893,558,1054,300,1047,583,580,394,229,944,347,742,1047,251,4901</v>
+        <v>9:00 28/04/2020,445,1170,590,203,424,596,2733,293,388,717,397,201,795,1328,346,584,1016,784,429,231,703,564,456,812,743,473,1256,636,1325,1761,244,456,1119,658,411,300,717,1025,512,524,822,2424,752,1139,619,613,308,602,2652,534,884,165,620,259,2183,707,632,104,401,454,3243,396,429,532,511,1114,2634,1308,620,874,896,804,1345,571,1033,592,633,509,441,843,936,1386,129,322,211,450,864,1008,729,488,1022,576,1489,216,273,275,448,654,297,357,414,655,20,567,926,761,2009,462,365,543,462,336,501,443,288,1163,616,1637,780,330,423,987,1098,2462,653,348,440,242,269,199,593,565,487,888,711,898,575,1090,303,1061,585,595,403,233,960,357,765,1072,258,4961</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1100</v>
+        <v>1119</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1100,</v>
+        <v>1119,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>451</v>
+        <v>456</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>652,</v>
+        <v>658,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1100</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>391,</v>
+        <v>411,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>652</v>
+        <v>658</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>297,</v>
+        <v>300,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>391</v>
+        <v>411</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>691</v>
+        <v>717</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>691,</v>
+        <v>717,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1014</v>
+        <v>1025</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1014,</v>
+        <v>1025,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>691</v>
+        <v>717</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>501</v>
+        <v>512</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>501,</v>
+        <v>512,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1014</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>521,</v>
+        <v>524,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>501</v>
+        <v>512</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>809</v>
+        <v>822</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>809,</v>
+        <v>822,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2320</v>
+        <v>2424</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2320,</v>
+        <v>2424,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>809</v>
+        <v>822</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>750,</v>
+        <v>752,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2320</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1112</v>
+        <v>1139</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1112,</v>
+        <v>1139,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>750</v>
+        <v>752</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>611,</v>
+        <v>619,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1112</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>612,</v>
+        <v>613,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>611</v>
+        <v>619</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>301,</v>
+        <v>308,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>599,</v>
+        <v>602,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>301</v>
+        <v>308</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2624</v>
+        <v>2652</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2624,</v>
+        <v>2652,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>531,</v>
+        <v>534,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2624</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>869</v>
+        <v>884</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>869,</v>
+        <v>884,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2355,7 +2355,7 @@
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>869</v>
+        <v>884</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,11 +2364,11 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>616,</v>
+        <v>620,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>244,</v>
+        <v>259,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>616</v>
+        <v>620</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2141</v>
+        <v>2183</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2141,</v>
+        <v>2183,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>244</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>701,</v>
+        <v>707,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2141</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>626,</v>
+        <v>632,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>701</v>
+        <v>707</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>103,</v>
+        <v>104,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>626</v>
+        <v>632</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2488,7 +2488,7 @@
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>451,</v>
+        <v>454,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3232</v>
+        <v>3243</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3232,</v>
+        <v>3243,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2545,7 +2545,7 @@
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3232</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,11 +2554,11 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>427,</v>
+        <v>429,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>521</v>
+        <v>532</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>521,</v>
+        <v>532,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>496</v>
+        <v>511</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>496,</v>
+        <v>511,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>521</v>
+        <v>532</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1110</v>
+        <v>1114</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1110,</v>
+        <v>1114,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>496</v>
+        <v>511</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2585</v>
+        <v>2634</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2585,</v>
+        <v>2634,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1110</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1273</v>
+        <v>1308</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1273,</v>
+        <v>1308,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2585</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>606</v>
+        <v>620</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>606,</v>
+        <v>620,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1273</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>858</v>
+        <v>874</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>858,</v>
+        <v>874,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>606</v>
+        <v>620</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>886</v>
+        <v>896</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>886,</v>
+        <v>896,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>858</v>
+        <v>874</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>781</v>
+        <v>804</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>781,</v>
+        <v>804,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>886</v>
+        <v>896</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1333</v>
+        <v>1345</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1333,</v>
+        <v>1345,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>781</v>
+        <v>804</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>567,</v>
+        <v>571,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1333</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1011</v>
+        <v>1033</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1011,</v>
+        <v>1033,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>567</v>
+        <v>571</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>586,</v>
+        <v>592,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1011</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>632,</v>
+        <v>633,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>586</v>
+        <v>592</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>496</v>
+        <v>509</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>496,</v>
+        <v>509,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>436,</v>
+        <v>441,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>496</v>
+        <v>509</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>828</v>
+        <v>843</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>828,</v>
+        <v>843,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>436</v>
+        <v>441</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>935,</v>
+        <v>936,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>828</v>
+        <v>843</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1355</v>
+        <v>1386</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1355,</v>
+        <v>1386,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>128,</v>
+        <v>129,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1355</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>313,</v>
+        <v>322,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>210,</v>
+        <v>211,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>313</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>440,</v>
+        <v>450,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>836</v>
+        <v>864</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>836,</v>
+        <v>864,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>440</v>
+        <v>450</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>990</v>
+        <v>1008</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>990,</v>
+        <v>1008,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>836</v>
+        <v>864</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>709</v>
+        <v>729</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>709,</v>
+        <v>729,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F90" s="2">
-        <v>990</v>
+      <c r="F90" s="3">
+        <v>1008</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3077,7 +3077,7 @@
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>709</v>
+        <v>729</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,11 +3086,11 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1014</v>
+        <v>1022</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1014,</v>
+        <v>1022,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>570,</v>
+        <v>576,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1014</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1452</v>
+        <v>1489</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1452,</v>
+        <v>1489,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>570</v>
+        <v>576</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>190,</v>
+        <v>216,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1452</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>272,</v>
+        <v>273,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>270,</v>
+        <v>275,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>437,</v>
+        <v>448,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>652,</v>
+        <v>654,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>437</v>
+        <v>448</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>294,</v>
+        <v>297,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>356,</v>
+        <v>357,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3286,7 +3286,7 @@
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,11 +3295,11 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>616</v>
+        <v>655</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>616,</v>
+        <v>655,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C104" s="5">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>19,</v>
+        <v>20,</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>616</v>
+        <v>655</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>558,</v>
+        <v>567,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F105" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>913</v>
+        <v>926</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>913,</v>
+        <v>926,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>558</v>
+        <v>567</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>746</v>
+        <v>761</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>746,</v>
+        <v>761,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>913</v>
+        <v>926</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>1952</v>
+        <v>2009</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1952,</v>
+        <v>2009,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>746</v>
+        <v>761</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>424</v>
+        <v>462</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>424,</v>
+        <v>462,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>1952</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>361,</v>
+        <v>365,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>424</v>
+        <v>462</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>538,</v>
+        <v>543,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>454,</v>
+        <v>462,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>538</v>
+        <v>543</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>333,</v>
+        <v>336,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>454</v>
+        <v>462</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>495,</v>
+        <v>501,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>439,</v>
+        <v>443,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>495</v>
+        <v>501</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>282,</v>
+        <v>288,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1160</v>
+        <v>1163</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1160,</v>
+        <v>1163,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>596</v>
+        <v>616</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>596,</v>
+        <v>616,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1160</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1595</v>
+        <v>1637</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1595,</v>
+        <v>1637,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>596</v>
+        <v>616</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>765</v>
+        <v>780</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>765,</v>
+        <v>780,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1595</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>328,</v>
+        <v>330,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>765</v>
+        <v>780</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>409,</v>
+        <v>423,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>936</v>
+        <v>987</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>936,</v>
+        <v>987,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>409</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1093</v>
+        <v>1098</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1093,</v>
+        <v>1098,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>936</v>
+        <v>987</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2434</v>
+        <v>2462</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2434,</v>
+        <v>2462,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1093</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>651,</v>
+        <v>653,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2434</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>347,</v>
+        <v>348,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>430,</v>
+        <v>440,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>225,</v>
+        <v>242,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>430</v>
+        <v>440</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>265,</v>
+        <v>269,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>225</v>
+        <v>242</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3837,7 +3837,7 @@
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,11 +3846,11 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>591,</v>
+        <v>593,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>553</v>
+        <v>565</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>553,</v>
+        <v>565,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>478,</v>
+        <v>487,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>553</v>
+        <v>565</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>836</v>
+        <v>888</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>836,</v>
+        <v>888,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>478</v>
+        <v>487</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>704</v>
+        <v>711</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>704,</v>
+        <v>711,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>836</v>
+        <v>888</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>893</v>
+        <v>898</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>893,</v>
+        <v>898,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>704</v>
+        <v>711</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>558</v>
+        <v>575</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>558,</v>
+        <v>575,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>893</v>
+        <v>898</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1054</v>
+        <v>1090</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1054,</v>
+        <v>1090,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>558</v>
+        <v>575</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>300,</v>
+        <v>303,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1054</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1047</v>
+        <v>1061</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1047,</v>
+        <v>1061,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>583,</v>
+        <v>585,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1047</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>580</v>
+        <v>595</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>580,</v>
+        <v>595,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>394,</v>
+        <v>403,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>580</v>
+        <v>595</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>229,</v>
+        <v>233,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>394</v>
+        <v>403</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>944,</v>
+        <v>960,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>347,</v>
+        <v>357,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>944</v>
+        <v>960</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>742</v>
+        <v>765</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>742,</v>
+        <v>765,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>347</v>
+        <v>357</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1047</v>
+        <v>1072</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1047,</v>
+        <v>1072,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>742</v>
+        <v>765</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>251,</v>
+        <v>258,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1047</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>4901</v>
+        <v>4961</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>4901</v>
+        <v>4961</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 29 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C1BCB5-7D75-1A4B-8EFA-CD46B9E66F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85825AD8-C1B9-244E-AFCA-CA7D5C90D49B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>445,</v>
+        <v>448,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>9907</v>
+        <v>10035</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>9907,</v>
+        <v>10035,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>6411</v>
+        <v>6530</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1170</v>
+        <v>1176</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1170,</v>
+        <v>1176,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1170</v>
+        <v>1176</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>23979</v>
+        <v>24090</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>23979,</v>
+        <v>24090,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>9907</v>
+        <v>10035</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>590</v>
+        <v>608</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>590,</v>
+        <v>608,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>590</v>
+        <v>608</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>18804</v>
+        <v>19123</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18804,</v>
+        <v>19123,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>23979</v>
+        <v>24090</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1172,17 +1172,17 @@
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>16673</v>
+        <v>16889</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16673,</v>
+        <v>16889,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>7174</v>
+        <v>7224</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1208,17 +1208,17 @@
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>17823</v>
+        <v>18106</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17823,</v>
+        <v>18106,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>17823</v>
+        <v>18106</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>596,</v>
+        <v>597,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>16323</v>
+        <v>16559</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16323,</v>
+        <v>16559,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>16323</v>
+        <v>16559</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2733</v>
+        <v>2782</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2733,</v>
+        <v>2782,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2733</v>
+        <v>2782</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>5986</v>
+        <v>6056</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5986,</v>
+        <v>6056,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>5986</v>
+        <v>6056</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>293,</v>
+        <v>301,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>4961</v>
+        <v>5001</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>4961,</v>
+        <v>5001,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>12393</v>
+        <v>12593</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>388,</v>
+        <v>413,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>114456</v>
+        <v>115859</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>114456</v>
+        <v>115859</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>9499</v>
+        <v>9665</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>717</v>
+        <v>732</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>717,</v>
+        <v>732,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>717</v>
+        <v>732</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>397,</v>
+        <v>400,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>201,</v>
+        <v>205,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>795,</v>
+        <v>796,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>114456</v>
+        <v>115859</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>114456,</v>
+        <v>115859,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>114456</v>
+        <v>115859</v>
       </c>
       <c r="M14" s="3">
-        <v>19294</v>
+        <v>23550</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1328</v>
+        <v>1330</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1328,</v>
+        <v>1330,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1328</v>
+        <v>1330</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>10721</v>
+        <v>11034</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10721,</v>
+        <v>11034,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3408</v>
+        <v>3463</v>
       </c>
       <c r="M15" s="2">
-        <v>309</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>346,</v>
+        <v>354,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>9512</v>
+        <v>9629</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9512,</v>
+        <v>9629,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>10721</v>
+        <v>11034</v>
       </c>
       <c r="M16" s="3">
-        <v>1262</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>584</v>
+        <v>593</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>584,</v>
+        <v>593,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>584</v>
+        <v>593</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3408</v>
+        <v>3463</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3408</v>
+        <v>3463</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>9512</v>
+        <v>9629</v>
       </c>
       <c r="M17" s="2">
-        <v>813</v>
+        <v>886</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1016</v>
+        <v>1027</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1016,</v>
+        <v>1027,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1016</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>784,</v>
+        <v>789,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>784</v>
+        <v>789</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>429,</v>
+        <v>434,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>429</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>703</v>
+        <v>718</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>703,</v>
+        <v>718,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>703</v>
+        <v>718</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>438194</v>
+        <v>434118</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>438194,</v>
+        <v>434118,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>564,</v>
+        <v>567,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>161145</v>
+        <v>165221</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>161145,</v>
+        <v>165221,</v>
       </c>
       <c r="K23" s="9">
-        <v>161145</v>
+        <v>165221</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>456,</v>
+        <v>457,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>21678</v>
+        <v>26097</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>21678,</v>
+        <v>26097,</v>
       </c>
       <c r="K24" s="9">
-        <v>21678</v>
+        <v>26097</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>812,</v>
+        <v>813,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>743,</v>
+        <v>746,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>743</v>
+        <v>746</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>473,</v>
+        <v>482,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1256</v>
+        <v>1279</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1256,</v>
+        <v>1279,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>473</v>
+        <v>482</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>636</v>
+        <v>649</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>636,</v>
+        <v>649,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1256</v>
+        <v>1279</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43949</v>
+        <v>43950</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1325</v>
+        <v>1336</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1325,</v>
+        <v>1336,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>636</v>
+        <v>649</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 28/04/2020,599339,438194,161145,21678,135</v>
+        <v>9:00 29/04/2020,599339,434118,165221,26097,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1761</v>
+        <v>1793</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1761,</v>
+        <v>1793,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1325</v>
+        <v>1336</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 28/04/2020,114456,10721,9512,3408</v>
+        <v>9:00 29/04/2020,115859,11034,9629,3463</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>244,</v>
+        <v>253,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1761</v>
+        <v>1793</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 28/04/2020,9907,23979,18804,16673,17823,16323,5986,4961,114456</v>
+        <v>9:00 29/04/2020,10035,24090,19123,16889,18106,16559,6056,5001,115859</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>456,</v>
+        <v>466,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 28/04/2020,445,1170,590,203,424,596,2733,293,388,717,397,201,795,1328,346,584,1016,784,429,231,703,564,456,812,743,473,1256,636,1325,1761,244,456,1119,658,411,300,717,1025,512,524,822,2424,752,1139,619,613,308,602,2652,534,884,165,620,259,2183,707,632,104,401,454,3243,396,429,532,511,1114,2634,1308,620,874,896,804,1345,571,1033,592,633,509,441,843,936,1386,129,322,211,450,864,1008,729,488,1022,576,1489,216,273,275,448,654,297,357,414,655,20,567,926,761,2009,462,365,543,462,336,501,443,288,1163,616,1637,780,330,423,987,1098,2462,653,348,440,242,269,199,593,565,487,888,711,898,575,1090,303,1061,585,595,403,233,960,357,765,1072,258,4961</v>
+        <v>9:00 29/04/2020,448,1176,608,203,424,597,2782,301,413,732,400,205,796,1330,354,593,1027,789,434,231,718,567,457,813,746,482,1279,649,1336,1793,253,466,1195,676,426,301,720,1030,539,552,824,2451,752,1152,620,613,309,605,2689,539,886,167,623,282,2202,711,635,104,406,456,3272,422,435,533,516,1117,2695,1322,630,884,898,804,1363,575,1047,592,637,509,443,852,938,1427,130,329,218,450,872,1013,732,488,1030,582,1515,223,273,281,454,658,297,358,417,666,20,583,940,770,2039,464,370,544,464,339,501,444,290,1167,614,1650,796,334,424,999,1098,2498,656,350,444,244,269,200,593,574,494,920,712,904,578,1116,312,1083,588,615,405,240,971,362,777,1081,258,5001</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1119</v>
+        <v>1195</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1119,</v>
+        <v>1195,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>456</v>
+        <v>466</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>658</v>
+        <v>676</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>658,</v>
+        <v>676,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1119</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>411</v>
+        <v>426</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>411,</v>
+        <v>426,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>658</v>
+        <v>676</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>300,</v>
+        <v>301,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>411</v>
+        <v>426</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>717,</v>
+        <v>720,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1025,</v>
+        <v>1030,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>717</v>
+        <v>720</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>512</v>
+        <v>539</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>512,</v>
+        <v>539,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1025</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>524</v>
+        <v>552</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>524,</v>
+        <v>552,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>512</v>
+        <v>539</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>822,</v>
+        <v>824,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>524</v>
+        <v>552</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2424</v>
+        <v>2451</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2424,</v>
+        <v>2451,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>822</v>
+        <v>824</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2184,7 +2184,7 @@
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2424</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1139</v>
+        <v>1152</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1139,</v>
+        <v>1152,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>619,</v>
+        <v>620,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1139</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2241,7 +2241,7 @@
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,11 +2250,11 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>308,</v>
+        <v>309,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>602,</v>
+        <v>605,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2652</v>
+        <v>2689</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2652,</v>
+        <v>2689,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>534,</v>
+        <v>539,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2652</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>884,</v>
+        <v>886,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>534</v>
+        <v>539</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>165,</v>
+        <v>167,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>884</v>
+        <v>886</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>620,</v>
+        <v>623,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>259,</v>
+        <v>282,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2183</v>
+        <v>2202</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2183,</v>
+        <v>2202,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>259</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>707,</v>
+        <v>711,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2183</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>632,</v>
+        <v>635,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2469,7 +2469,7 @@
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>632</v>
+        <v>635</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,11 +2478,11 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>401,</v>
+        <v>406,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>454,</v>
+        <v>456,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>401</v>
+        <v>406</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3243</v>
+        <v>3272</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3243,</v>
+        <v>3272,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>396</v>
+        <v>422</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>396,</v>
+        <v>422,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3243</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>429,</v>
+        <v>435,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>396</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>532,</v>
+        <v>533,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>511,</v>
+        <v>516,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1114</v>
+        <v>1117</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1114,</v>
+        <v>1117,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2634</v>
+        <v>2695</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2634,</v>
+        <v>2695,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1114</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1308</v>
+        <v>1322</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1308,</v>
+        <v>1322,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2634</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>620,</v>
+        <v>630,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1308</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>874</v>
+        <v>884</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>874,</v>
+        <v>884,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>620</v>
+        <v>630</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>896,</v>
+        <v>898,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>874</v>
+        <v>884</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2735,7 +2735,7 @@
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>896</v>
+        <v>898</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,11 +2744,11 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1345</v>
+        <v>1363</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1345,</v>
+        <v>1363,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>571,</v>
+        <v>575,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1345</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1033</v>
+        <v>1047</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1033,</v>
+        <v>1047,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2811,7 +2811,7 @@
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1033</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,11 +2820,11 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>633,</v>
+        <v>637,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
@@ -2849,7 +2849,7 @@
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,11 +2858,11 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>441,</v>
+        <v>443,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>843</v>
+        <v>852</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>843,</v>
+        <v>852,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>936,</v>
+        <v>938,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>843</v>
+        <v>852</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1386</v>
+        <v>1427</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1386,</v>
+        <v>1427,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>936</v>
+        <v>938</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>129,</v>
+        <v>130,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1386</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>322,</v>
+        <v>329,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>211,</v>
+        <v>218,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -3001,7 +3001,7 @@
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,11 +3010,11 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>864</v>
+        <v>872</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>864,</v>
+        <v>872,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1008</v>
+        <v>1013</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1008,</v>
+        <v>1013,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>864</v>
+        <v>872</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>729,</v>
+        <v>732,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1008</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3077,7 +3077,7 @@
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>729</v>
+        <v>732</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,11 +3086,11 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1022</v>
+        <v>1030</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1022,</v>
+        <v>1030,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>576,</v>
+        <v>582,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1022</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1489</v>
+        <v>1515</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1489,</v>
+        <v>1515,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>576</v>
+        <v>582</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>216,</v>
+        <v>223,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1489</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3172,7 +3172,7 @@
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>275,</v>
+        <v>281,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>448,</v>
+        <v>454,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>654,</v>
+        <v>658,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>448</v>
+        <v>454</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3248,7 +3248,7 @@
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,11 +3257,11 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>357,</v>
+        <v>358,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>414,</v>
+        <v>417,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>655</v>
+        <v>666</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>655,</v>
+        <v>666,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>655</v>
+        <v>666</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>567</v>
+        <v>583</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>567,</v>
+        <v>583,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>926</v>
+        <v>940</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>926,</v>
+        <v>940,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>567</v>
+        <v>583</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>761</v>
+        <v>770</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>761,</v>
+        <v>770,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>926</v>
+        <v>940</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2009</v>
+        <v>2039</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2009,</v>
+        <v>2039,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>761</v>
+        <v>770</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>462,</v>
+        <v>464,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2009</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>365,</v>
+        <v>370,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>543,</v>
+        <v>544,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>462,</v>
+        <v>464,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>336,</v>
+        <v>339,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3514,7 +3514,7 @@
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,11 +3523,11 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>443,</v>
+        <v>444,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>288,</v>
+        <v>290,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1163</v>
+        <v>1167</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1163,</v>
+        <v>1167,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>616,</v>
+        <v>614,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1163</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1637</v>
+        <v>1650</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1637,</v>
+        <v>1650,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>780</v>
+        <v>796</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>780,</v>
+        <v>796,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1637</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>330,</v>
+        <v>334,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>780</v>
+        <v>796</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>423,</v>
+        <v>424,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>987</v>
+        <v>999</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>987,</v>
+        <v>999,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3704,7 +3704,7 @@
         <v>121</v>
       </c>
       <c r="F124" s="2">
-        <v>987</v>
+        <v>999</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2462</v>
+        <v>2498</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2462,</v>
+        <v>2498,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>653,</v>
+        <v>656,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2462</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>348,</v>
+        <v>350,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>440,</v>
+        <v>444,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>242,</v>
+        <v>244,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3818,7 +3818,7 @@
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,11 +3827,11 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>199,</v>
+        <v>200,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
@@ -3856,7 +3856,7 @@
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,11 +3865,11 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>565</v>
+        <v>574</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>565,</v>
+        <v>574,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>487,</v>
+        <v>494,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>565</v>
+        <v>574</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>888</v>
+        <v>920</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>888,</v>
+        <v>920,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>487</v>
+        <v>494</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>711,</v>
+        <v>712,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>888</v>
+        <v>920</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>898</v>
+        <v>904</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>898,</v>
+        <v>904,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>575,</v>
+        <v>578,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>898</v>
+        <v>904</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1090</v>
+        <v>1116</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1090,</v>
+        <v>1116,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>303,</v>
+        <v>312,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1090</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1061</v>
+        <v>1083</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1061,</v>
+        <v>1083,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>585,</v>
+        <v>588,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1061</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>595</v>
+        <v>615</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>595,</v>
+        <v>615,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>403,</v>
+        <v>405,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>595</v>
+        <v>615</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>233,</v>
+        <v>240,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>960</v>
+        <v>971</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>960,</v>
+        <v>971,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>357,</v>
+        <v>362,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>960</v>
+        <v>971</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>765</v>
+        <v>777</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>765,</v>
+        <v>777,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1072</v>
+        <v>1081</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1072,</v>
+        <v>1081,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>765</v>
+        <v>777</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4198,7 +4198,7 @@
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1072</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,11 +4207,11 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>4961</v>
+        <v>5001</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>4961</v>
+        <v>5001</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
ammend data as of 29 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85825AD8-C1B9-244E-AFCA-CA7D5C90D49B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A1E0AF-8247-4E44-A467-A92C7D168919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1667,14 +1667,14 @@
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>599339</v>
+        <v>632794</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>599339,</v>
+        <v>632794,</v>
       </c>
       <c r="K21" s="9">
-        <v>599339</v>
+        <v>632794</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1700,11 +1700,11 @@
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>434118</v>
+        <v>467573</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>434118,</v>
+        <v>467573,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43950</v>
+        <v>43951</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 29/04/2020,599339,434118,165221,26097,135</v>
+        <v>9:00 30/04/2020,632794,467573,165221,26097,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 29/04/2020,115859,11034,9629,3463</v>
+        <v>9:00 30/04/2020,115859,11034,9629,3463</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 29/04/2020,10035,24090,19123,16889,18106,16559,6056,5001,115859</v>
+        <v>9:00 30/04/2020,10035,24090,19123,16889,18106,16559,6056,5001,115859</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 29/04/2020,448,1176,608,203,424,597,2782,301,413,732,400,205,796,1330,354,593,1027,789,434,231,718,567,457,813,746,482,1279,649,1336,1793,253,466,1195,676,426,301,720,1030,539,552,824,2451,752,1152,620,613,309,605,2689,539,886,167,623,282,2202,711,635,104,406,456,3272,422,435,533,516,1117,2695,1322,630,884,898,804,1363,575,1047,592,637,509,443,852,938,1427,130,329,218,450,872,1013,732,488,1030,582,1515,223,273,281,454,658,297,358,417,666,20,583,940,770,2039,464,370,544,464,339,501,444,290,1167,614,1650,796,334,424,999,1098,2498,656,350,444,244,269,200,593,574,494,920,712,904,578,1116,312,1083,588,615,405,240,971,362,777,1081,258,5001</v>
+        <v>9:00 30/04/2020,448,1176,608,203,424,597,2782,301,413,732,400,205,796,1330,354,593,1027,789,434,231,718,567,457,813,746,482,1279,649,1336,1793,253,466,1195,676,426,301,720,1030,539,552,824,2451,752,1152,620,613,309,605,2689,539,886,167,623,282,2202,711,635,104,406,456,3272,422,435,533,516,1117,2695,1322,630,884,898,804,1363,575,1047,592,637,509,443,852,938,1427,130,329,218,450,872,1013,732,488,1030,582,1515,223,273,281,454,658,297,358,417,666,20,583,940,770,2039,464,370,544,464,339,501,444,290,1167,614,1650,796,334,424,999,1098,2498,656,350,444,244,269,200,593,574,494,920,712,904,578,1116,312,1083,588,615,405,240,971,362,777,1081,258,5001</v>
       </c>
     </row>
     <row r="34" spans="2:8">

</xml_diff>

<commit_message>
update data as of 30 April 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A1E0AF-8247-4E44-A467-A92C7D168919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDA800D-7667-8B41-BE3D-BED0F8280682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>448,</v>
+        <v>450,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>10035</v>
+        <v>10274</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>10035,</v>
+        <v>10274,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>6530</v>
+        <v>6747</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1176</v>
+        <v>1184</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1176,</v>
+        <v>1184,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1176</v>
+        <v>1184</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>24090</v>
+        <v>24297</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>24090,</v>
+        <v>24297,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>10035</v>
+        <v>10274</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>608</v>
+        <v>622</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>608,</v>
+        <v>622,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>608</v>
+        <v>622</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>19123</v>
+        <v>19615</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>19123,</v>
+        <v>19615,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>24090</v>
+        <v>24297</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>203,</v>
+        <v>206,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>16889</v>
+        <v>17562</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16889,</v>
+        <v>17562,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>7224</v>
+        <v>7552</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>424,</v>
+        <v>436,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>18106</v>
+        <v>18523</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18106,</v>
+        <v>18523,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>18106</v>
+        <v>18523</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>597</v>
+        <v>608</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>597,</v>
+        <v>608,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>597</v>
+        <v>608</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>16559</v>
+        <v>16831</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16559,</v>
+        <v>16831,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>16559</v>
+        <v>16831</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2782</v>
+        <v>2801</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2782,</v>
+        <v>2801,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2782</v>
+        <v>2801</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>6056</v>
+        <v>6177</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6056,</v>
+        <v>6177,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>6056</v>
+        <v>6177</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>301,</v>
+        <v>306,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>5001</v>
+        <v>5064</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5001,</v>
+        <v>5064,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>12593</v>
+        <v>12868</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>413,</v>
+        <v>427,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>115859</v>
+        <v>118343</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>115859</v>
+        <v>118343</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>9665</v>
+        <v>10010</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>732</v>
+        <v>739</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>732,</v>
+        <v>739,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>732</v>
+        <v>739</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>400,</v>
+        <v>404,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>205,</v>
+        <v>209,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>796</v>
+        <v>849</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>796,</v>
+        <v>849,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>796</v>
+        <v>849</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>115859</v>
+        <v>118343</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>115859,</v>
+        <v>118343,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>115859</v>
+        <v>118343</v>
       </c>
       <c r="M14" s="3">
-        <v>23550</v>
+        <v>24110</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1330</v>
+        <v>1338</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1330,</v>
+        <v>1338,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1330</v>
+        <v>1338</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>11034</v>
+        <v>11353</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11034,</v>
+        <v>11353,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3463</v>
+        <v>3536</v>
       </c>
       <c r="M15" s="2">
-        <v>329</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>354,</v>
+        <v>355,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>9629</v>
+        <v>9812</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9629,</v>
+        <v>9812,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>11034</v>
+        <v>11353</v>
       </c>
       <c r="M16" s="3">
-        <v>1332</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>593,</v>
+        <v>601,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3463</v>
+        <v>3536</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3463</v>
+        <v>3536</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>9629</v>
+        <v>9812</v>
       </c>
       <c r="M17" s="2">
-        <v>886</v>
+        <v>908</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1027</v>
+        <v>1036</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1027,</v>
+        <v>1036,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1027</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>789</v>
+        <v>801</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>789,</v>
+        <v>801,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>789</v>
+        <v>801</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>434</v>
+        <v>457</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>434,</v>
+        <v>457,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>434</v>
+        <v>457</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>231,</v>
+        <v>238,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>632794</v>
+        <v>687369</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>632794,</v>
+        <v>687369,</v>
       </c>
       <c r="K21" s="9">
-        <v>632794</v>
+        <v>687369</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>718,</v>
+        <v>722,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>467573</v>
+        <v>516116</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>467573,</v>
+        <v>516116,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>567,</v>
+        <v>569,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>165221</v>
+        <v>171253</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>165221,</v>
+        <v>171253,</v>
       </c>
       <c r="K23" s="9">
-        <v>165221</v>
+        <v>171253</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>457,</v>
+        <v>471,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>26097</v>
+        <v>26771</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>26097,</v>
+        <v>26771,</v>
       </c>
       <c r="K24" s="9">
-        <v>26097</v>
+        <v>26771</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>813</v>
+        <v>851</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>813,</v>
+        <v>851,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>813</v>
+        <v>851</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>746</v>
+        <v>777</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>746,</v>
+        <v>777,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>746</v>
+        <v>777</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>482,</v>
+        <v>485,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1279</v>
+        <v>1340</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1279,</v>
+        <v>1340,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>649,</v>
+        <v>654,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1279</v>
+        <v>1340</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43951</v>
+        <v>43952</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1336</v>
+        <v>1358</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1336,</v>
+        <v>1358,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 30/04/2020,632794,467573,165221,26097,135</v>
+        <v>9:00 01/05/2020,687369,516116,171253,26771,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1793</v>
+        <v>1819</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1793,</v>
+        <v>1819,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1336</v>
+        <v>1358</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 30/04/2020,115859,11034,9629,3463</v>
+        <v>9:00 01/05/2020,118343,11353,9812,3536</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>253,</v>
+        <v>269,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1793</v>
+        <v>1819</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 30/04/2020,10035,24090,19123,16889,18106,16559,6056,5001,115859</v>
+        <v>9:00 01/05/2020,10274,24297,19615,17562,18523,16831,6177,5064,118343</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>466</v>
+        <v>476</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>466,</v>
+        <v>476,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 30/04/2020,448,1176,608,203,424,597,2782,301,413,732,400,205,796,1330,354,593,1027,789,434,231,718,567,457,813,746,482,1279,649,1336,1793,253,466,1195,676,426,301,720,1030,539,552,824,2451,752,1152,620,613,309,605,2689,539,886,167,623,282,2202,711,635,104,406,456,3272,422,435,533,516,1117,2695,1322,630,884,898,804,1363,575,1047,592,637,509,443,852,938,1427,130,329,218,450,872,1013,732,488,1030,582,1515,223,273,281,454,658,297,358,417,666,20,583,940,770,2039,464,370,544,464,339,501,444,290,1167,614,1650,796,334,424,999,1098,2498,656,350,444,244,269,200,593,574,494,920,712,904,578,1116,312,1083,588,615,405,240,971,362,777,1081,258,5001</v>
+        <v>9:00 01/05/2020,450,1184,622,206,436,608,2801,306,427,739,404,209,849,1338,355,601,1036,801,457,238,722,569,471,851,777,485,1340,654,1358,1819,269,476,1243,686,440,304,734,1044,567,570,827,2506,800,1181,623,616,312,605,2734,543,903,180,631,298,2243,717,637,107,409,459,3331,428,443,551,532,1124,2736,1367,648,906,904,828,1392,595,1060,610,641,541,448,884,943,1481,134,350,231,460,908,1019,748,518,1089,594,1540,224,278,284,460,667,311,361,434,680,20,595,957,789,2093,479,376,556,482,341,538,454,294,1179,634,1697,808,343,459,1027,1138,2530,662,361,451,254,275,202,597,584,512,934,718,909,594,1141,315,1100,592,642,415,245,990,362,797,1107,271,5064</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1195</v>
+        <v>1243</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1195,</v>
+        <v>1243,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>466</v>
+        <v>476</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>676</v>
+        <v>686</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>676,</v>
+        <v>686,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1195</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>426,</v>
+        <v>440,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>676</v>
+        <v>686</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>301,</v>
+        <v>304,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>426</v>
+        <v>440</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>720</v>
+        <v>734</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>720,</v>
+        <v>734,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1030</v>
+        <v>1044</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1030,</v>
+        <v>1044,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>720</v>
+        <v>734</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>539</v>
+        <v>567</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>539,</v>
+        <v>567,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1030</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>552</v>
+        <v>570</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>552,</v>
+        <v>570,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>539</v>
+        <v>567</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>824,</v>
+        <v>827,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>552</v>
+        <v>570</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2451</v>
+        <v>2506</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2451,</v>
+        <v>2506,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>824</v>
+        <v>827</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>752</v>
+        <v>800</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>752,</v>
+        <v>800,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2451</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1152</v>
+        <v>1181</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1152,</v>
+        <v>1181,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>752</v>
+        <v>800</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>620,</v>
+        <v>623,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1152</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>613,</v>
+        <v>616,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>309,</v>
+        <v>312,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2279,7 +2279,7 @@
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2689</v>
+        <v>2734</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2689,</v>
+        <v>2734,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>539,</v>
+        <v>543,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2689</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>886</v>
+        <v>903</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>886,</v>
+        <v>903,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>167,</v>
+        <v>180,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>886</v>
+        <v>903</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>623,</v>
+        <v>631,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>282,</v>
+        <v>298,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>623</v>
+        <v>631</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2202</v>
+        <v>2243</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2202,</v>
+        <v>2243,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>282</v>
+        <v>298</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>711,</v>
+        <v>717,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2202</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>635,</v>
+        <v>637,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>711</v>
+        <v>717</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>104,</v>
+        <v>107,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>406,</v>
+        <v>409,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>456,</v>
+        <v>459,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3272</v>
+        <v>3331</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3272,</v>
+        <v>3331,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>422,</v>
+        <v>428,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3272</v>
+        <v>3331</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>435,</v>
+        <v>443,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>422</v>
+        <v>428</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>533</v>
+        <v>551</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>533,</v>
+        <v>551,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>435</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>516,</v>
+        <v>532,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>533</v>
+        <v>551</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1117</v>
+        <v>1124</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1117,</v>
+        <v>1124,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>516</v>
+        <v>532</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2695</v>
+        <v>2736</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2695,</v>
+        <v>2736,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1117</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1322</v>
+        <v>1367</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1322,</v>
+        <v>1367,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2695</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>630</v>
+        <v>648</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>630,</v>
+        <v>648,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1322</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>884</v>
+        <v>906</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>884,</v>
+        <v>906,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>630</v>
+        <v>648</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>898</v>
+        <v>904</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>898,</v>
+        <v>904,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>884</v>
+        <v>906</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>804</v>
+        <v>828</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>804,</v>
+        <v>828,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>898</v>
+        <v>904</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1363</v>
+        <v>1392</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1363,</v>
+        <v>1392,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>804</v>
+        <v>828</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>575</v>
+        <v>595</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>575,</v>
+        <v>595,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1363</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1047</v>
+        <v>1060</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1047,</v>
+        <v>1060,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>575</v>
+        <v>595</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>592</v>
+        <v>610</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>592,</v>
+        <v>610,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1047</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>637,</v>
+        <v>641,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>592</v>
+        <v>610</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>509</v>
+        <v>541</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>509,</v>
+        <v>541,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>443,</v>
+        <v>448,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>509</v>
+        <v>541</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>852</v>
+        <v>884</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>852,</v>
+        <v>884,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>938</v>
+        <v>943</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>938,</v>
+        <v>943,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>852</v>
+        <v>884</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1427</v>
+        <v>1481</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1427,</v>
+        <v>1481,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>938</v>
+        <v>943</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>130,</v>
+        <v>134,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1427</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>329</v>
+        <v>350</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>329,</v>
+        <v>350,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>218,</v>
+        <v>231,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>329</v>
+        <v>350</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>450,</v>
+        <v>460,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>218</v>
+        <v>231</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>872</v>
+        <v>908</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>872,</v>
+        <v>908,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>450</v>
+        <v>460</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1013,</v>
+        <v>1019,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>872</v>
+        <v>908</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>732</v>
+        <v>748</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>732,</v>
+        <v>748,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1013</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>488</v>
+        <v>518</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>488,</v>
+        <v>518,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>732</v>
+        <v>748</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1030</v>
+        <v>1089</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1030,</v>
+        <v>1089,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>488</v>
+        <v>518</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>582</v>
+        <v>594</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>582,</v>
+        <v>594,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1030</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1515</v>
+        <v>1540</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1515,</v>
+        <v>1540,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>582</v>
+        <v>594</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>223,</v>
+        <v>224,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1515</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>273,</v>
+        <v>278,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>281,</v>
+        <v>284,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>454,</v>
+        <v>460,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>658,</v>
+        <v>667,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>454</v>
+        <v>460</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>297,</v>
+        <v>311,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>658</v>
+        <v>667</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>358,</v>
+        <v>361,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>297</v>
+        <v>311</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>417,</v>
+        <v>434,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>666</v>
+        <v>680</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>666,</v>
+        <v>680,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>417</v>
+        <v>434</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>666</v>
+        <v>680</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>583</v>
+        <v>595</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>583,</v>
+        <v>595,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>940</v>
+        <v>957</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>940,</v>
+        <v>957,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>583</v>
+        <v>595</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>770</v>
+        <v>789</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>770,</v>
+        <v>789,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="2">
-        <v>940</v>
+        <v>957</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2039</v>
+        <v>2093</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2039,</v>
+        <v>2093,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>770</v>
+        <v>789</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>464</v>
+        <v>479</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>464,</v>
+        <v>479,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2039</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>370,</v>
+        <v>376,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>464</v>
+        <v>479</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>544</v>
+        <v>556</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>544,</v>
+        <v>556,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>370</v>
+        <v>376</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>464,</v>
+        <v>482,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>544</v>
+        <v>556</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>339,</v>
+        <v>341,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>464</v>
+        <v>482</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>501</v>
+        <v>538</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>501,</v>
+        <v>538,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>444,</v>
+        <v>454,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>501</v>
+        <v>538</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>290,</v>
+        <v>294,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>444</v>
+        <v>454</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1167</v>
+        <v>1179</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1167,</v>
+        <v>1179,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>614</v>
+        <v>634</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>614,</v>
+        <v>634,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1167</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1650</v>
+        <v>1697</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1650,</v>
+        <v>1697,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>614</v>
+        <v>634</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>796</v>
+        <v>808</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>796,</v>
+        <v>808,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1650</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>334,</v>
+        <v>343,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>796</v>
+        <v>808</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>424</v>
+        <v>459</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>424,</v>
+        <v>459,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>999</v>
+        <v>1027</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>999,</v>
+        <v>1027,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>424</v>
+        <v>459</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1098</v>
+        <v>1138</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1098,</v>
+        <v>1138,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F124" s="2">
-        <v>999</v>
+      <c r="F124" s="3">
+        <v>1027</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2498</v>
+        <v>2530</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2498,</v>
+        <v>2530,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1098</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>656,</v>
+        <v>662,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2498</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>350,</v>
+        <v>361,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>656</v>
+        <v>662</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>444,</v>
+        <v>451,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>244,</v>
+        <v>254,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>444</v>
+        <v>451</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>269,</v>
+        <v>275,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>244</v>
+        <v>254</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>200,</v>
+        <v>202,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>593,</v>
+        <v>597,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>574</v>
+        <v>584</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>574,</v>
+        <v>584,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>494</v>
+        <v>512</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>494,</v>
+        <v>512,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>574</v>
+        <v>584</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>920</v>
+        <v>934</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>920,</v>
+        <v>934,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>494</v>
+        <v>512</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>712,</v>
+        <v>718,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>920</v>
+        <v>934</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>904</v>
+        <v>909</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>904,</v>
+        <v>909,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>712</v>
+        <v>718</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>578</v>
+        <v>594</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>578,</v>
+        <v>594,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>904</v>
+        <v>909</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1116</v>
+        <v>1141</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1116,</v>
+        <v>1141,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>578</v>
+        <v>594</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>312,</v>
+        <v>315,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1116</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1083</v>
+        <v>1100</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1083,</v>
+        <v>1100,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>588,</v>
+        <v>592,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1083</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>615</v>
+        <v>642</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>615,</v>
+        <v>642,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>588</v>
+        <v>592</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>405,</v>
+        <v>415,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>615</v>
+        <v>642</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>240,</v>
+        <v>245,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>405</v>
+        <v>415</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>971</v>
+        <v>990</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>971,</v>
+        <v>990,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4141,7 +4141,7 @@
         <v>144</v>
       </c>
       <c r="F147" s="2">
-        <v>971</v>
+        <v>990</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,11 +4150,11 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>777</v>
+        <v>797</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>777,</v>
+        <v>797,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1081</v>
+        <v>1107</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1081,</v>
+        <v>1107,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>777</v>
+        <v>797</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>258,</v>
+        <v>271,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1081</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>5001</v>
+        <v>5064</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>5001</v>
+        <v>5064</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>258</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 01 May 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDA800D-7667-8B41-BE3D-BED0F8280682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A477F0A-182C-8A44-98EA-4636835BDD7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>450,</v>
+        <v>453,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>10274</v>
+        <v>10512</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>10274,</v>
+        <v>10512,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>6747</v>
+        <v>6879</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1184</v>
+        <v>1193</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1184,</v>
+        <v>1193,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1184</v>
+        <v>1193</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>24297</v>
+        <v>24477</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>24297,</v>
+        <v>24477,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>10274</v>
+        <v>10512</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>622</v>
+        <v>639</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>622,</v>
+        <v>639,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>622</v>
+        <v>639</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>19615</v>
+        <v>20042</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>19615,</v>
+        <v>20042,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>24297</v>
+        <v>24477</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>206,</v>
+        <v>211,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>17562</v>
+        <v>18067</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17562,</v>
+        <v>18067,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>7552</v>
+        <v>7813</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>436,</v>
+        <v>439,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>18523</v>
+        <v>18943</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18523,</v>
+        <v>18943,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>18523</v>
+        <v>18943</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>608,</v>
+        <v>613,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>16831</v>
+        <v>17095</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>16831,</v>
+        <v>17095,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>16831</v>
+        <v>17095</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2801</v>
+        <v>2844</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2801,</v>
+        <v>2844,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2801</v>
+        <v>2844</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>6177</v>
+        <v>6304</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6177,</v>
+        <v>6304,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>6177</v>
+        <v>6304</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>306,</v>
+        <v>309,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>5064</v>
+        <v>5174</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5064,</v>
+        <v>5174,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>12868</v>
+        <v>13163</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>427</v>
+        <v>445</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>427,</v>
+        <v>445,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>427</v>
+        <v>445</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>118343</v>
+        <v>120614</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>118343</v>
+        <v>120614</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>10010</v>
+        <v>10254</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>739</v>
+        <v>763</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>739,</v>
+        <v>763,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>739</v>
+        <v>763</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>404,</v>
+        <v>406,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>209,</v>
+        <v>212,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>849</v>
+        <v>864</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>849,</v>
+        <v>864,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>849</v>
+        <v>864</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>118343</v>
+        <v>120614</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>118343,</v>
+        <v>120614,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>118343</v>
+        <v>120614</v>
       </c>
       <c r="M14" s="3">
-        <v>24110</v>
+        <v>24763</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1338</v>
+        <v>1344</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1338,</v>
+        <v>1344,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1338</v>
+        <v>1344</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>11353</v>
+        <v>11654</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11353,</v>
+        <v>11654,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3536</v>
+        <v>3623</v>
       </c>
       <c r="M15" s="2">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>355,</v>
+        <v>373,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>9812</v>
+        <v>9972</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9812,</v>
+        <v>9972,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>11353</v>
+        <v>11654</v>
       </c>
       <c r="M16" s="3">
-        <v>1415</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>601</v>
+        <v>608</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>601,</v>
+        <v>608,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>601</v>
+        <v>608</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3536</v>
+        <v>3623</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3536</v>
+        <v>3623</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>9812</v>
+        <v>9972</v>
       </c>
       <c r="M17" s="2">
-        <v>908</v>
+        <v>925</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1036,</v>
+        <v>1047,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1036</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>801</v>
+        <v>816</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>801,</v>
+        <v>816,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>801</v>
+        <v>816</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>457</v>
+        <v>483</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>457,</v>
+        <v>483,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>457</v>
+        <v>483</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>238,</v>
+        <v>241,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>687369</v>
+        <v>762279</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>687369,</v>
+        <v>762279,</v>
       </c>
       <c r="K21" s="9">
-        <v>687369</v>
+        <v>762279</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>722</v>
+        <v>753</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>722,</v>
+        <v>753,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>722</v>
+        <v>753</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>516116</v>
+        <v>584825</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>516116,</v>
+        <v>584825,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>569,</v>
+        <v>571,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>171253</v>
+        <v>177454</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>171253,</v>
+        <v>177454,</v>
       </c>
       <c r="K23" s="9">
-        <v>171253</v>
+        <v>177454</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>471</v>
+        <v>497</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>471,</v>
+        <v>497,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>471</v>
+        <v>497</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>26771</v>
+        <v>27510</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>26771,</v>
+        <v>27510,</v>
       </c>
       <c r="K24" s="9">
-        <v>26771</v>
+        <v>27510</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>851</v>
+        <v>869</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>851,</v>
+        <v>869,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>851</v>
+        <v>869</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>777</v>
+        <v>800</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>777,</v>
+        <v>800,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>777</v>
+        <v>800</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>485</v>
+        <v>496</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>485,</v>
+        <v>496,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1340</v>
+        <v>1407</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1340,</v>
+        <v>1407,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>485</v>
+        <v>496</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>654,</v>
+        <v>657,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1340</v>
+        <v>1407</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43952</v>
+        <v>43953</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1358</v>
+        <v>1379</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1358,</v>
+        <v>1379,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 01/05/2020,687369,516116,171253,26771,135</v>
+        <v>9:00 02/05/2020,762279,584825,177454,27510,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1819</v>
+        <v>1888</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1819,</v>
+        <v>1888,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1358</v>
+        <v>1379</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 01/05/2020,118343,11353,9812,3536</v>
+        <v>9:00 02/05/2020,120614,11654,9972,3623</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>269,</v>
+        <v>281,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1819</v>
+        <v>1888</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 01/05/2020,10274,24297,19615,17562,18523,16831,6177,5064,118343</v>
+        <v>9:00 02/05/2020,10512,24477,20042,18067,18943,17095,6304,5174,120614</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>476,</v>
+        <v>490,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 01/05/2020,450,1184,622,206,436,608,2801,306,427,739,404,209,849,1338,355,601,1036,801,457,238,722,569,471,851,777,485,1340,654,1358,1819,269,476,1243,686,440,304,734,1044,567,570,827,2506,800,1181,623,616,312,605,2734,543,903,180,631,298,2243,717,637,107,409,459,3331,428,443,551,532,1124,2736,1367,648,906,904,828,1392,595,1060,610,641,541,448,884,943,1481,134,350,231,460,908,1019,748,518,1089,594,1540,224,278,284,460,667,311,361,434,680,20,595,957,789,2093,479,376,556,482,341,538,454,294,1179,634,1697,808,343,459,1027,1138,2530,662,361,451,254,275,202,597,584,512,934,718,909,594,1141,315,1100,592,642,415,245,990,362,797,1107,271,5064</v>
+        <v>9:00 02/05/2020,453,1193,639,211,439,613,2844,309,445,763,406,212,864,1344,373,608,1047,816,483,241,753,571,497,869,800,496,1407,657,1379,1888,281,490,1272,701,472,308,754,1052,584,580,831,2540,834,1214,627,620,317,608,2781,546,909,192,633,302,2271,722,645,122,410,461,3356,440,444,562,530,1131,2773,1394,664,927,918,834,1403,624,1092,620,650,554,451,900,948,1524,134,351,234,468,932,1036,776,518,1118,622,1552,246,287,285,474,672,317,364,456,706,20,612,1005,800,2132,499,382,569,492,344,565,473,296,1186,645,1730,816,355,471,1046,1164,2559,666,367,453,260,276,202,598,592,521,957,723,917,603,1164,316,1126,596,670,434,251,1002,366,812,1139,282,5174</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1243</v>
+        <v>1272</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1243,</v>
+        <v>1272,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>476</v>
+        <v>490</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>686</v>
+        <v>701</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>686,</v>
+        <v>701,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1243</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>440</v>
+        <v>472</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>440,</v>
+        <v>472,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>686</v>
+        <v>701</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>304,</v>
+        <v>308,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>440</v>
+        <v>472</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>734</v>
+        <v>754</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>734,</v>
+        <v>754,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1044</v>
+        <v>1052</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1044,</v>
+        <v>1052,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>734</v>
+        <v>754</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>567</v>
+        <v>584</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>567,</v>
+        <v>584,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1044</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>570,</v>
+        <v>580,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>567</v>
+        <v>584</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>827,</v>
+        <v>831,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>570</v>
+        <v>580</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2506</v>
+        <v>2540</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2506,</v>
+        <v>2540,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>827</v>
+        <v>831</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>800</v>
+        <v>834</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>800,</v>
+        <v>834,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2506</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1181</v>
+        <v>1214</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1181,</v>
+        <v>1214,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>800</v>
+        <v>834</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>623,</v>
+        <v>627,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1181</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>616,</v>
+        <v>620,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>623</v>
+        <v>627</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>312,</v>
+        <v>317,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>605,</v>
+        <v>608,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2734</v>
+        <v>2781</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2734,</v>
+        <v>2781,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>543,</v>
+        <v>546,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2734</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>903</v>
+        <v>909</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>903,</v>
+        <v>909,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>180,</v>
+        <v>192,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>903</v>
+        <v>909</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>631,</v>
+        <v>633,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>180</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>298,</v>
+        <v>302,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2243</v>
+        <v>2271</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2243,</v>
+        <v>2271,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>717</v>
+        <v>722</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>717,</v>
+        <v>722,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2243</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>637,</v>
+        <v>645,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>717</v>
+        <v>722</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>107,</v>
+        <v>122,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>637</v>
+        <v>645</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>409,</v>
+        <v>410,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>107</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>459,</v>
+        <v>461,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3331</v>
+        <v>3356</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3331,</v>
+        <v>3356,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>428,</v>
+        <v>440,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3331</v>
+        <v>3356</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>443,</v>
+        <v>444,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>428</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>551,</v>
+        <v>562,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>532,</v>
+        <v>530,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>551</v>
+        <v>562</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1124</v>
+        <v>1131</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1124,</v>
+        <v>1131,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2736</v>
+        <v>2773</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2736,</v>
+        <v>2773,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1124</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1367</v>
+        <v>1394</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1367,</v>
+        <v>1394,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2736</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>648</v>
+        <v>664</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>648,</v>
+        <v>664,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1367</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>906</v>
+        <v>927</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>906,</v>
+        <v>927,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>648</v>
+        <v>664</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>904</v>
+        <v>918</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>904,</v>
+        <v>918,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>906</v>
+        <v>927</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>828</v>
+        <v>834</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>828,</v>
+        <v>834,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>904</v>
+        <v>918</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1392</v>
+        <v>1403</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1392,</v>
+        <v>1403,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>828</v>
+        <v>834</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>595</v>
+        <v>624</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>595,</v>
+        <v>624,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1392</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1060</v>
+        <v>1092</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1060,</v>
+        <v>1092,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>595</v>
+        <v>624</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>610,</v>
+        <v>620,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1060</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>641,</v>
+        <v>650,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>610</v>
+        <v>620</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>541</v>
+        <v>554</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>541,</v>
+        <v>554,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>641</v>
+        <v>650</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>448,</v>
+        <v>451,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>541</v>
+        <v>554</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>884</v>
+        <v>900</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>884,</v>
+        <v>900,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>943,</v>
+        <v>948,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>884</v>
+        <v>900</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1481</v>
+        <v>1524</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1481,</v>
+        <v>1524,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>943</v>
+        <v>948</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2944,7 +2944,7 @@
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1481</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,11 +2953,11 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>350,</v>
+        <v>351,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>231,</v>
+        <v>234,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>460,</v>
+        <v>468,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>908</v>
+        <v>932</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>908,</v>
+        <v>932,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>460</v>
+        <v>468</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1019</v>
+        <v>1036</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1019,</v>
+        <v>1036,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>908</v>
+        <v>932</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>748</v>
+        <v>776</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>748,</v>
+        <v>776,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1019</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3077,7 +3077,7 @@
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>748</v>
+        <v>776</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,11 +3086,11 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1089</v>
+        <v>1118</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1089,</v>
+        <v>1118,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>594</v>
+        <v>622</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>594,</v>
+        <v>622,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1089</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1540</v>
+        <v>1552</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1540,</v>
+        <v>1552,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>594</v>
+        <v>622</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>224,</v>
+        <v>246,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1540</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>278,</v>
+        <v>287,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>224</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>284,</v>
+        <v>285,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>460,</v>
+        <v>474,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>667,</v>
+        <v>672,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>460</v>
+        <v>474</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>311,</v>
+        <v>317,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>667</v>
+        <v>672</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>361,</v>
+        <v>364,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>434</v>
+        <v>456</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>434,</v>
+        <v>456,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>680</v>
+        <v>706</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>680,</v>
+        <v>706,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>434</v>
+        <v>456</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>680</v>
+        <v>706</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>595</v>
+        <v>612</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>595,</v>
+        <v>612,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>957</v>
+        <v>1005</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>957,</v>
+        <v>1005,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>595</v>
+        <v>612</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>789</v>
+        <v>800</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>789,</v>
+        <v>800,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F107" s="2">
-        <v>957</v>
+      <c r="F107" s="3">
+        <v>1005</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2093</v>
+        <v>2132</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2093,</v>
+        <v>2132,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>789</v>
+        <v>800</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>479</v>
+        <v>499</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>479,</v>
+        <v>499,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2093</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>376,</v>
+        <v>382,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>479</v>
+        <v>499</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>556,</v>
+        <v>569,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>376</v>
+        <v>382</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>482</v>
+        <v>492</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>482,</v>
+        <v>492,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>556</v>
+        <v>569</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>341,</v>
+        <v>344,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>482</v>
+        <v>492</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>538</v>
+        <v>565</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>538,</v>
+        <v>565,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>454</v>
+        <v>473</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>454,</v>
+        <v>473,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>538</v>
+        <v>565</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>294,</v>
+        <v>296,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>454</v>
+        <v>473</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1179</v>
+        <v>1186</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1179,</v>
+        <v>1186,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>634</v>
+        <v>645</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>634,</v>
+        <v>645,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1179</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1697</v>
+        <v>1730</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1697,</v>
+        <v>1730,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>634</v>
+        <v>645</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>808</v>
+        <v>816</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>808,</v>
+        <v>816,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1697</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>343,</v>
+        <v>355,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>808</v>
+        <v>816</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>459,</v>
+        <v>471,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>343</v>
+        <v>355</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>1027</v>
+        <v>1046</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1027,</v>
+        <v>1046,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>459</v>
+        <v>471</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1138</v>
+        <v>1164</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1138,</v>
+        <v>1164,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="3">
-        <v>1027</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2530</v>
+        <v>2559</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2530,</v>
+        <v>2559,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1138</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>662,</v>
+        <v>666,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2530</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>361,</v>
+        <v>367,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>662</v>
+        <v>666</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>451,</v>
+        <v>453,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>254,</v>
+        <v>260,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>275,</v>
+        <v>276,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3837,7 +3837,7 @@
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,11 +3846,11 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>597,</v>
+        <v>598,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>584,</v>
+        <v>592,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>512,</v>
+        <v>521,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>584</v>
+        <v>592</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>934</v>
+        <v>957</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>934,</v>
+        <v>957,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>512</v>
+        <v>521</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>718</v>
+        <v>723</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>718,</v>
+        <v>723,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>934</v>
+        <v>957</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>909,</v>
+        <v>917,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>718</v>
+        <v>723</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>594,</v>
+        <v>603,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>909</v>
+        <v>917</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1141</v>
+        <v>1164</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1141,</v>
+        <v>1164,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>594</v>
+        <v>603</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>315,</v>
+        <v>316,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1141</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1100</v>
+        <v>1126</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1100,</v>
+        <v>1126,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>592,</v>
+        <v>596,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1100</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>642</v>
+        <v>670</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>642,</v>
+        <v>670,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>415</v>
+        <v>434</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>415,</v>
+        <v>434,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>642</v>
+        <v>670</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>245,</v>
+        <v>251,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>415</v>
+        <v>434</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>990</v>
+        <v>1002</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>990,</v>
+        <v>1002,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>362,</v>
+        <v>366,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F147" s="2">
-        <v>990</v>
+      <c r="F147" s="3">
+        <v>1002</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>797</v>
+        <v>812</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>797,</v>
+        <v>812,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1107</v>
+        <v>1139</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1107,</v>
+        <v>1139,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>797</v>
+        <v>812</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>271,</v>
+        <v>282,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1107</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>5064</v>
+        <v>5174</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>5064</v>
+        <v>5174</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>271</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 02 May 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A477F0A-182C-8A44-98EA-4636835BDD7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13B3E62-1AFD-BD42-838D-B1B905F0D4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1014,8 +1014,8 @@
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="6" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="4"/>
     <col min="8" max="8" width="19.83203125" customWidth="1"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>453,</v>
+        <v>456,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>10512</v>
+        <v>10785</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>10512,</v>
+        <v>10785,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>6879</v>
+        <v>7004</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1193</v>
+        <v>1209</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1193,</v>
+        <v>1209,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1193</v>
+        <v>1209</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>24477</v>
+        <v>24700</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>24477,</v>
+        <v>24700,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>10512</v>
+        <v>10785</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>639</v>
+        <v>665</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>639,</v>
+        <v>665,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>639</v>
+        <v>665</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>20042</v>
+        <v>20406</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20042,</v>
+        <v>20406,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>24477</v>
+        <v>24700</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>211,</v>
+        <v>212,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>18067</v>
+        <v>18539</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18067,</v>
+        <v>18539,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>7813</v>
+        <v>7941</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>439,</v>
+        <v>442,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>18943</v>
+        <v>19435</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18943,</v>
+        <v>19435,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>18943</v>
+        <v>19435</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>613,</v>
+        <v>622,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>17095</v>
+        <v>17324</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17095,</v>
+        <v>17324,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>17095</v>
+        <v>17324</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2844</v>
+        <v>2869</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2844,</v>
+        <v>2869,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2844</v>
+        <v>2869</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>6304</v>
+        <v>6405</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6304,</v>
+        <v>6405,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>6304</v>
+        <v>6405</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>309,</v>
+        <v>321,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>5174</v>
+        <v>5248</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5174,</v>
+        <v>5248,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>13163</v>
+        <v>13402</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>445,</v>
+        <v>452,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>120614</v>
+        <v>122842</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>120614</v>
+        <v>122842</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>10254</v>
+        <v>10598</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>763</v>
+        <v>782</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>763,</v>
+        <v>782,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>763</v>
+        <v>782</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>406,</v>
+        <v>412,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>212,</v>
+        <v>214,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>864</v>
+        <v>915</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>864,</v>
+        <v>915,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>864</v>
+        <v>915</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>120614</v>
+        <v>122842</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>120614,</v>
+        <v>122842,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>120614</v>
+        <v>122842</v>
       </c>
       <c r="M14" s="3">
-        <v>24763</v>
+        <v>25282</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1344</v>
+        <v>1354</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1344,</v>
+        <v>1354,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1344</v>
+        <v>1354</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>11654</v>
+        <v>11927</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11654,</v>
+        <v>11927,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3623</v>
+        <v>3689</v>
       </c>
       <c r="M15" s="2">
-        <v>347</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>373,</v>
+        <v>376,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>9972</v>
+        <v>10155</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>9972,</v>
+        <v>10155,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>11654</v>
+        <v>11927</v>
       </c>
       <c r="M16" s="3">
-        <v>1475</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>608,</v>
+        <v>616,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3623</v>
+        <v>3689</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3623</v>
+        <v>3689</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>9972</v>
+        <v>10155</v>
       </c>
       <c r="M17" s="2">
-        <v>925</v>
+        <v>969</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1047</v>
+        <v>1079</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1047,</v>
+        <v>1079,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1047</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>816</v>
+        <v>836</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>816,</v>
+        <v>836,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>816</v>
+        <v>836</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>483</v>
+        <v>502</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>483,</v>
+        <v>502,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>483</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>241,</v>
+        <v>245,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>762279</v>
+        <v>825946</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>762279,</v>
+        <v>825946,</v>
       </c>
       <c r="K21" s="9">
-        <v>762279</v>
+        <v>825946</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>753</v>
+        <v>768</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>753,</v>
+        <v>768,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>753</v>
+        <v>768</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>584825</v>
+        <v>643686</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>584825,</v>
+        <v>643686,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>571,</v>
+        <v>576,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>177454</v>
+        <v>182260</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>177454,</v>
+        <v>182260,</v>
       </c>
       <c r="K23" s="9">
-        <v>177454</v>
+        <v>182260</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>497,</v>
+        <v>502,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>27510</v>
+        <v>28131</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>27510,</v>
+        <v>28131,</v>
       </c>
       <c r="K24" s="9">
-        <v>27510</v>
+        <v>28131</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>869</v>
+        <v>888</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>869,</v>
+        <v>888,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>869</v>
+        <v>888</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>829</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>800,</v>
+        <v>829,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>800</v>
+        <v>829</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>496</v>
+        <v>505</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>496,</v>
+        <v>505,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1407</v>
+        <v>1447</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1407,</v>
+        <v>1447,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>496</v>
+        <v>505</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,17 +1869,17 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>657</v>
+        <v>665</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>657,</v>
+        <v>665,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1407</v>
+        <v>1447</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1379</v>
+        <v>1384</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1379,</v>
+        <v>1384,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>657</v>
+        <v>665</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 02/05/2020,762279,584825,177454,27510,135</v>
+        <v>9:00 02/05/2020,825946,643686,182260,28131,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1888</v>
+        <v>1914</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1888,</v>
+        <v>1914,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1379</v>
+        <v>1384</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 02/05/2020,120614,11654,9972,3623</v>
+        <v>9:00 02/05/2020,122842,11927,10155,3689</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>281,</v>
+        <v>287,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1888</v>
+        <v>1914</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 02/05/2020,10512,24477,20042,18067,18943,17095,6304,5174,120614</v>
+        <v>9:00 02/05/2020,10785,24700,20406,18539,19435,17324,6405,5248,122842</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>490,</v>
+        <v>496,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 02/05/2020,453,1193,639,211,439,613,2844,309,445,763,406,212,864,1344,373,608,1047,816,483,241,753,571,497,869,800,496,1407,657,1379,1888,281,490,1272,701,472,308,754,1052,584,580,831,2540,834,1214,627,620,317,608,2781,546,909,192,633,302,2271,722,645,122,410,461,3356,440,444,562,530,1131,2773,1394,664,927,918,834,1403,624,1092,620,650,554,451,900,948,1524,134,351,234,468,932,1036,776,518,1118,622,1552,246,287,285,474,672,317,364,456,706,20,612,1005,800,2132,499,382,569,492,344,565,473,296,1186,645,1730,816,355,471,1046,1164,2559,666,367,453,260,276,202,598,592,521,957,723,917,603,1164,316,1126,596,670,434,251,1002,366,812,1139,282,5174</v>
+        <v>9:00 02/05/2020,456,1209,665,212,442,622,2869,321,452,782,412,214,915,1354,376,616,1079,836,502,245,768,576,502,888,829,505,1447,665,1384,1914,287,496,1303,712,493,313,774,1066,612,588,833,2615,837,1228,638,622,325,610,2827,547,936,197,634,303,2319,726,653,123,414,462,3379,462,450,572,554,1139,2824,1434,676,946,925,855,1428,626,1118,630,654,559,469,929,952,1607,135,366,246,478,974,1047,787,527,1134,658,1561,251,293,286,480,678,320,367,476,720,20,642,1023,810,2170,507,384,571,506,349,568,487,298,1201,655,1766,851,362,490,1076,1170,2588,667,369,465,267,281,203,600,603,535,970,724,921,626,1186,319,1154,601,694,441,253,1018,370,850,1161,300,5248</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1272</v>
+        <v>1303</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1272,</v>
+        <v>1303,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>490</v>
+        <v>496</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>701</v>
+        <v>712</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>701,</v>
+        <v>712,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1272</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>472</v>
+        <v>493</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>472,</v>
+        <v>493,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>701</v>
+        <v>712</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>308,</v>
+        <v>313,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>472</v>
+        <v>493</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>754</v>
+        <v>774</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>754,</v>
+        <v>774,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1052</v>
+        <v>1066</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1052,</v>
+        <v>1066,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>754</v>
+        <v>774</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>584</v>
+        <v>612</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>584,</v>
+        <v>612,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1052</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>580,</v>
+        <v>588,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>584</v>
+        <v>612</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>831,</v>
+        <v>833,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>580</v>
+        <v>588</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2540</v>
+        <v>2615</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2540,</v>
+        <v>2615,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>834,</v>
+        <v>837,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2540</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1214</v>
+        <v>1228</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1214,</v>
+        <v>1228,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>834</v>
+        <v>837</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>627</v>
+        <v>638</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>627,</v>
+        <v>638,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1214</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>620,</v>
+        <v>622,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>627</v>
+        <v>638</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>317,</v>
+        <v>325,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>608,</v>
+        <v>610,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2781</v>
+        <v>2827</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2781,</v>
+        <v>2827,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>546,</v>
+        <v>547,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2781</v>
+        <v>2827</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>909</v>
+        <v>936</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>909,</v>
+        <v>936,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>192,</v>
+        <v>197,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>909</v>
+        <v>936</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>633,</v>
+        <v>634,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>302,</v>
+        <v>303,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2271</v>
+        <v>2319</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2271,</v>
+        <v>2319,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>722,</v>
+        <v>726,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2271</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>645,</v>
+        <v>653,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>722</v>
+        <v>726</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>122,</v>
+        <v>123,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>645</v>
+        <v>653</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>410,</v>
+        <v>414,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>461,</v>
+        <v>462,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3356</v>
+        <v>3379</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3356,</v>
+        <v>3379,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>440</v>
+        <v>462</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>440,</v>
+        <v>462,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3356</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>444,</v>
+        <v>450,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>440</v>
+        <v>462</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>562,</v>
+        <v>572,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>444</v>
+        <v>450</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>530</v>
+        <v>554</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>530,</v>
+        <v>554,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>562</v>
+        <v>572</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1131</v>
+        <v>1139</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1131,</v>
+        <v>1139,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>530</v>
+        <v>554</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2773</v>
+        <v>2824</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2773,</v>
+        <v>2824,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1131</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1394</v>
+        <v>1434</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1394,</v>
+        <v>1434,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2773</v>
+        <v>2824</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>664</v>
+        <v>676</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>664,</v>
+        <v>676,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1394</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>927</v>
+        <v>946</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>927,</v>
+        <v>946,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>664</v>
+        <v>676</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>918</v>
+        <v>925</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>918,</v>
+        <v>925,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>927</v>
+        <v>946</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>834</v>
+        <v>855</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>834,</v>
+        <v>855,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>918</v>
+        <v>925</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1403</v>
+        <v>1428</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1403,</v>
+        <v>1428,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>834</v>
+        <v>855</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>624,</v>
+        <v>626,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1403</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1092</v>
+        <v>1118</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1092,</v>
+        <v>1118,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>620,</v>
+        <v>630,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1092</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>650,</v>
+        <v>654,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>620</v>
+        <v>630</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>554,</v>
+        <v>559,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>451</v>
+        <v>469</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>451,</v>
+        <v>469,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>554</v>
+        <v>559</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>929</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>900,</v>
+        <v>929,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>451</v>
+        <v>469</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>948</v>
+        <v>952</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>948,</v>
+        <v>952,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>900</v>
+        <v>929</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1524</v>
+        <v>1607</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1524,</v>
+        <v>1607,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>948</v>
+        <v>952</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>134,</v>
+        <v>135,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1524</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>351,</v>
+        <v>366,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>234,</v>
+        <v>246,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>351</v>
+        <v>366</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>468,</v>
+        <v>478,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>234</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>932</v>
+        <v>974</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>932,</v>
+        <v>974,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>468</v>
+        <v>478</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1036,</v>
+        <v>1047,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>932</v>
+        <v>974</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>776</v>
+        <v>787</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>776,</v>
+        <v>787,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1036</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>518,</v>
+        <v>527,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>776</v>
+        <v>787</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1118</v>
+        <v>1134</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1118,</v>
+        <v>1134,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>518</v>
+        <v>527</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>622</v>
+        <v>658</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>622,</v>
+        <v>658,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1118</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1552</v>
+        <v>1561</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1552,</v>
+        <v>1561,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>622</v>
+        <v>658</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>246,</v>
+        <v>251,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1552</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>287,</v>
+        <v>293,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>285,</v>
+        <v>286,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>474,</v>
+        <v>480,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>672</v>
+        <v>678</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>672,</v>
+        <v>678,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>474</v>
+        <v>480</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>317,</v>
+        <v>320,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>672</v>
+        <v>678</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>364,</v>
+        <v>367,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>456</v>
+        <v>476</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>456,</v>
+        <v>476,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>706</v>
+        <v>720</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>706,</v>
+        <v>720,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>456</v>
+        <v>476</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>706</v>
+        <v>720</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>612</v>
+        <v>642</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>612,</v>
+        <v>642,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>1005</v>
+        <v>1023</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1005,</v>
+        <v>1023,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>612</v>
+        <v>642</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>800</v>
+        <v>810</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>800,</v>
+        <v>810,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="3">
-        <v>1005</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2132</v>
+        <v>2170</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2132,</v>
+        <v>2170,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>800</v>
+        <v>810</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>499,</v>
+        <v>507,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2132</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>382,</v>
+        <v>384,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>569,</v>
+        <v>571,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>492</v>
+        <v>506</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>492,</v>
+        <v>506,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>344,</v>
+        <v>349,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>492</v>
+        <v>506</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>565,</v>
+        <v>568,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>473,</v>
+        <v>487,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>296,</v>
+        <v>298,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>473</v>
+        <v>487</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1186</v>
+        <v>1201</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1186,</v>
+        <v>1201,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>645,</v>
+        <v>655,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1186</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1730</v>
+        <v>1766</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1730,</v>
+        <v>1766,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>645</v>
+        <v>655</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>816</v>
+        <v>851</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>816,</v>
+        <v>851,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1730</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>355,</v>
+        <v>362,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>816</v>
+        <v>851</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>471</v>
+        <v>490</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>471,</v>
+        <v>490,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>1046</v>
+        <v>1076</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1046,</v>
+        <v>1076,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>471</v>
+        <v>490</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1164</v>
+        <v>1170</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1164,</v>
+        <v>1170,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="3">
-        <v>1046</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2559</v>
+        <v>2588</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2559,</v>
+        <v>2588,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1164</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>666,</v>
+        <v>667,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2559</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>367,</v>
+        <v>369,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>453,</v>
+        <v>465,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>260,</v>
+        <v>267,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>453</v>
+        <v>465</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>276,</v>
+        <v>281,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>202,</v>
+        <v>203,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>276</v>
+        <v>281</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>598,</v>
+        <v>600,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>592,</v>
+        <v>603,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>521</v>
+        <v>535</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>521,</v>
+        <v>535,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>592</v>
+        <v>603</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>957</v>
+        <v>970</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>957,</v>
+        <v>970,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>521</v>
+        <v>535</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>723,</v>
+        <v>724,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>957</v>
+        <v>970</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>917,</v>
+        <v>921,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>603</v>
+        <v>626</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>603,</v>
+        <v>626,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>917</v>
+        <v>921</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1164</v>
+        <v>1186</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1164,</v>
+        <v>1186,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>603</v>
+        <v>626</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>316,</v>
+        <v>319,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1164</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1126</v>
+        <v>1154</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1126,</v>
+        <v>1154,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>596,</v>
+        <v>601,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1126</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>670</v>
+        <v>694</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>670,</v>
+        <v>694,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>596</v>
+        <v>601</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>434,</v>
+        <v>441,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>670</v>
+        <v>694</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>251,</v>
+        <v>253,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>434</v>
+        <v>441</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>1002</v>
+        <v>1018</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1002,</v>
+        <v>1018,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>366,</v>
+        <v>370,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="3">
-        <v>1002</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>812</v>
+        <v>850</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>812,</v>
+        <v>850,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1139</v>
+        <v>1161</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1139,</v>
+        <v>1161,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>812</v>
+        <v>850</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>282,</v>
+        <v>300,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1139</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>5174</v>
+        <v>5248</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>5174</v>
+        <v>5248</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>282</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as of 03 May 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13B3E62-1AFD-BD42-838D-B1B905F0D4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C5BBE6-9FBD-4D4F-95B0-9423221D76DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="E1" sqref="E1:F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>456,</v>
+        <v>458,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>10785</v>
+        <v>10943</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>10785,</v>
+        <v>10943,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>7004</v>
+        <v>7075</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1209</v>
+        <v>1214</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1209,</v>
+        <v>1214,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1209</v>
+        <v>1214</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>24700</v>
+        <v>24828</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>24700,</v>
+        <v>24828,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>10785</v>
+        <v>10943</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>665</v>
+        <v>678</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>665,</v>
+        <v>678,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>665</v>
+        <v>678</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>20406</v>
+        <v>20652</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20406,</v>
+        <v>20652,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>24700</v>
+        <v>24828</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1172,17 +1172,17 @@
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>18539</v>
+        <v>18967</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18539,</v>
+        <v>18967,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>7941</v>
+        <v>8164</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>442,</v>
+        <v>452,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>19435</v>
+        <v>20125</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>19435,</v>
+        <v>20125,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>19435</v>
+        <v>20125</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>622</v>
+        <v>634</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>622,</v>
+        <v>634,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>622</v>
+        <v>634</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>17324</v>
+        <v>17537</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17324,</v>
+        <v>17537,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>17324</v>
+        <v>17537</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2869</v>
+        <v>2904</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2869,</v>
+        <v>2904,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2869</v>
+        <v>2904</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>6405</v>
+        <v>6489</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6405,</v>
+        <v>6489,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>6405</v>
+        <v>6489</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>321,</v>
+        <v>331,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>5248</v>
+        <v>5320</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5248,</v>
+        <v>5320,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>13402</v>
+        <v>13577</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>452,</v>
+        <v>465,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>122842</v>
+        <v>124861</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>122842</v>
+        <v>124861</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>10598</v>
+        <v>10803</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>782</v>
+        <v>807</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>782,</v>
+        <v>807,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>782</v>
+        <v>807</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>412,</v>
+        <v>413,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>214,</v>
+        <v>217,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>915</v>
+        <v>947</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>915,</v>
+        <v>947,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>915</v>
+        <v>947</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>122842</v>
+        <v>124861</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>122842,</v>
+        <v>124861,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>122842</v>
+        <v>124861</v>
       </c>
       <c r="M14" s="3">
-        <v>25282</v>
+        <v>25528</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1354,</v>
+        <v>1355,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>11927</v>
+        <v>12097</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11927,</v>
+        <v>12097,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3689</v>
+        <v>3767</v>
       </c>
       <c r="M15" s="2">
-        <v>365</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>376,</v>
+        <v>381,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>10155</v>
+        <v>10329</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10155,</v>
+        <v>10329,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>11927</v>
+        <v>12097</v>
       </c>
       <c r="M16" s="3">
-        <v>1515</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>616,</v>
+        <v>626,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3689</v>
+        <v>3767</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3689</v>
+        <v>3767</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>10155</v>
+        <v>10329</v>
       </c>
       <c r="M17" s="2">
-        <v>969</v>
+        <v>983</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1079</v>
+        <v>1086</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1079,</v>
+        <v>1086,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1079</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>836,</v>
+        <v>838,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>502</v>
+        <v>549</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>502,</v>
+        <v>549,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>502</v>
+        <v>549</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>245,</v>
+        <v>252,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>825946</v>
+        <v>882343</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>825946,</v>
+        <v>882343,</v>
       </c>
       <c r="K21" s="9">
-        <v>825946</v>
+        <v>882343</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>768</v>
+        <v>795</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>768,</v>
+        <v>795,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>768</v>
+        <v>795</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>643686</v>
+        <v>695744</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>643686,</v>
+        <v>695744,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>576,</v>
+        <v>582,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>182260</v>
+        <v>186599</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>182260,</v>
+        <v>186599,</v>
       </c>
       <c r="K23" s="9">
-        <v>182260</v>
+        <v>186599</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>502,</v>
+        <v>509,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>28131</v>
+        <v>28446</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>28131,</v>
+        <v>28446,</v>
       </c>
       <c r="K24" s="9">
-        <v>28131</v>
+        <v>28446</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>888</v>
+        <v>908</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>888,</v>
+        <v>908,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>888</v>
+        <v>908</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>829</v>
+        <v>841</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>829,</v>
+        <v>841,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>829</v>
+        <v>841</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>505,</v>
+        <v>507,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1447</v>
+        <v>1504</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1447,</v>
+        <v>1504,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>665,</v>
+        <v>674,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1447</v>
+        <v>1504</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43953</v>
+        <v>43954</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1384</v>
+        <v>1388</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1384,</v>
+        <v>1388,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 02/05/2020,825946,643686,182260,28131,135</v>
+        <v>9:00 03/05/2020,882343,695744,186599,28446,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1914</v>
+        <v>1954</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1914,</v>
+        <v>1954,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1384</v>
+        <v>1388</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 02/05/2020,122842,11927,10155,3689</v>
+        <v>9:00 03/05/2020,124861,12097,10329,3767</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>287,</v>
+        <v>297,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1914</v>
+        <v>1954</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 02/05/2020,10785,24700,20406,18539,19435,17324,6405,5248,122842</v>
+        <v>9:00 03/05/2020,10943,24828,20652,18967,20125,17537,6489,5320,124861</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>496,</v>
+        <v>500,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 02/05/2020,456,1209,665,212,442,622,2869,321,452,782,412,214,915,1354,376,616,1079,836,502,245,768,576,502,888,829,505,1447,665,1384,1914,287,496,1303,712,493,313,774,1066,612,588,833,2615,837,1228,638,622,325,610,2827,547,936,197,634,303,2319,726,653,123,414,462,3379,462,450,572,554,1139,2824,1434,676,946,925,855,1428,626,1118,630,654,559,469,929,952,1607,135,366,246,478,974,1047,787,527,1134,658,1561,251,293,286,480,678,320,367,476,720,20,642,1023,810,2170,507,384,571,506,349,568,487,298,1201,655,1766,851,362,490,1076,1170,2588,667,369,465,267,281,203,600,603,535,970,724,921,626,1186,319,1154,601,694,441,253,1018,370,850,1161,300,5248</v>
+        <v>9:00 03/05/2020,458,1214,678,212,452,634,2904,331,465,807,413,217,947,1355,381,626,1086,838,549,252,795,582,509,908,841,507,1504,674,1388,1954,297,500,1320,727,494,324,785,1070,616,593,838,2650,875,1231,640,625,329,610,2861,549,939,197,637,307,2341,729,655,127,417,462,3418,469,451,578,566,1143,2878,1463,676,948,927,870,1454,626,1154,635,654,566,475,939,955,1626,135,378,254,489,997,1056,801,537,1148,758,1583,257,297,292,496,683,330,381,527,736,20,714,1026,829,2191,518,389,578,518,352,595,491,300,1209,660,1787,873,365,509,1105,1206,2608,673,372,474,277,282,206,601,622,554,990,730,928,635,1202,328,1172,605,768,450,256,1029,377,856,1164,315,5320</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1303</v>
+        <v>1320</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1303,</v>
+        <v>1320,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>712</v>
+        <v>727</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>712,</v>
+        <v>727,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1303</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>493,</v>
+        <v>494,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>712</v>
+        <v>727</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>313,</v>
+        <v>324,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>774</v>
+        <v>785</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>774,</v>
+        <v>785,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>313</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1066,</v>
+        <v>1070,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>774</v>
+        <v>785</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>612,</v>
+        <v>616,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1066</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>588,</v>
+        <v>593,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>612</v>
+        <v>616</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>833,</v>
+        <v>838,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>588</v>
+        <v>593</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2615</v>
+        <v>2650</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2615,</v>
+        <v>2650,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>833</v>
+        <v>838</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>837</v>
+        <v>875</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>837,</v>
+        <v>875,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2615</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1228,</v>
+        <v>1231,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>837</v>
+        <v>875</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>638,</v>
+        <v>640,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>622,</v>
+        <v>625,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>325,</v>
+        <v>329,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2279,7 +2279,7 @@
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2827</v>
+        <v>2861</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2827,</v>
+        <v>2861,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>547,</v>
+        <v>549,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2827</v>
+        <v>2861</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>936,</v>
+        <v>939,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2355,7 +2355,7 @@
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>936</v>
+        <v>939</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,11 +2364,11 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>634,</v>
+        <v>637,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>303,</v>
+        <v>307,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2319</v>
+        <v>2341</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2319,</v>
+        <v>2341,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>726,</v>
+        <v>729,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2319</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>653,</v>
+        <v>655,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>726</v>
+        <v>729</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>123,</v>
+        <v>127,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>414,</v>
+        <v>417,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2507,7 +2507,7 @@
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,11 +2516,11 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3379</v>
+        <v>3418</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3379,</v>
+        <v>3418,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>462,</v>
+        <v>469,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3379</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>450,</v>
+        <v>451,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>462</v>
+        <v>469</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>572,</v>
+        <v>578,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>554</v>
+        <v>566</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>554,</v>
+        <v>566,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>572</v>
+        <v>578</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1139</v>
+        <v>1143</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1139,</v>
+        <v>1143,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>554</v>
+        <v>566</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2824</v>
+        <v>2878</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2824,</v>
+        <v>2878,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1139</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1434</v>
+        <v>1463</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1434,</v>
+        <v>1463,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2824</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2678,7 +2678,7 @@
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1434</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>946,</v>
+        <v>948,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>925,</v>
+        <v>927,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>855</v>
+        <v>870</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>855,</v>
+        <v>870,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>925</v>
+        <v>927</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1428</v>
+        <v>1454</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1428,</v>
+        <v>1454,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>855</v>
+        <v>870</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2773,7 +2773,7 @@
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1428</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,11 +2782,11 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1118</v>
+        <v>1154</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1118,</v>
+        <v>1154,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>630,</v>
+        <v>635,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1118</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2830,7 +2830,7 @@
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>630</v>
+        <v>635</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,11 +2839,11 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>559,</v>
+        <v>566,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>469,</v>
+        <v>475,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>559</v>
+        <v>566</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>929</v>
+        <v>939</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>929,</v>
+        <v>939,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>952,</v>
+        <v>955,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>929</v>
+        <v>939</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1607</v>
+        <v>1626</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1607,</v>
+        <v>1626,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>952</v>
+        <v>955</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2944,7 +2944,7 @@
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1607</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,11 +2953,11 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>366,</v>
+        <v>378,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>246,</v>
+        <v>254,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>366</v>
+        <v>378</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>478,</v>
+        <v>489,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>974</v>
+        <v>997</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>974,</v>
+        <v>997,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>478</v>
+        <v>489</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1047</v>
+        <v>1056</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1047,</v>
+        <v>1056,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="2">
-        <v>974</v>
+        <v>997</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>787</v>
+        <v>801</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>787,</v>
+        <v>801,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1047</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>527</v>
+        <v>537</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>527,</v>
+        <v>537,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>787</v>
+        <v>801</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1134</v>
+        <v>1148</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1134,</v>
+        <v>1148,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>527</v>
+        <v>537</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>658</v>
+        <v>758</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>658,</v>
+        <v>758,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1134</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1561</v>
+        <v>1583</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1561,</v>
+        <v>1583,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>658</v>
+        <v>758</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>251,</v>
+        <v>257,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1561</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>293,</v>
+        <v>297,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>286,</v>
+        <v>292,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>480,</v>
+        <v>496,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>678,</v>
+        <v>683,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>480</v>
+        <v>496</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>320,</v>
+        <v>330,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>678</v>
+        <v>683</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>367,</v>
+        <v>381,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>320</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>476</v>
+        <v>527</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>476,</v>
+        <v>527,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>367</v>
+        <v>381</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>720</v>
+        <v>736</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>720,</v>
+        <v>736,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>476</v>
+        <v>527</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>720</v>
+        <v>736</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>642</v>
+        <v>714</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>642,</v>
+        <v>714,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1023,</v>
+        <v>1026,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>642</v>
+        <v>714</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>810</v>
+        <v>829</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>810,</v>
+        <v>829,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="3">
-        <v>1023</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2170</v>
+        <v>2191</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2170,</v>
+        <v>2191,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>810</v>
+        <v>829</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>507,</v>
+        <v>518,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2170</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>384,</v>
+        <v>389,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>507</v>
+        <v>518</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>571,</v>
+        <v>578,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>384</v>
+        <v>389</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>506,</v>
+        <v>518,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>571</v>
+        <v>578</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>349,</v>
+        <v>352,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>506</v>
+        <v>518</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>568</v>
+        <v>595</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>568,</v>
+        <v>595,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>487,</v>
+        <v>491,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>568</v>
+        <v>595</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>298,</v>
+        <v>300,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1201</v>
+        <v>1209</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1201,</v>
+        <v>1209,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>655,</v>
+        <v>660,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1201</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1766</v>
+        <v>1787</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1766,</v>
+        <v>1787,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>655</v>
+        <v>660</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>851</v>
+        <v>873</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>851,</v>
+        <v>873,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1766</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>362,</v>
+        <v>365,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>851</v>
+        <v>873</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>490</v>
+        <v>509</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>490,</v>
+        <v>509,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>1076</v>
+        <v>1105</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1076,</v>
+        <v>1105,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>490</v>
+        <v>509</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1170</v>
+        <v>1206</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1170,</v>
+        <v>1206,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="3">
-        <v>1076</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2588</v>
+        <v>2608</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2588,</v>
+        <v>2608,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1170</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>667,</v>
+        <v>673,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2588</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>369,</v>
+        <v>372,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>667</v>
+        <v>673</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>465,</v>
+        <v>474,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>267,</v>
+        <v>277,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>465</v>
+        <v>474</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>281,</v>
+        <v>282,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>203,</v>
+        <v>206,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>600,</v>
+        <v>601,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>603</v>
+        <v>622</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>603,</v>
+        <v>622,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>535</v>
+        <v>554</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>535,</v>
+        <v>554,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>603</v>
+        <v>622</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>970</v>
+        <v>990</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>970,</v>
+        <v>990,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>535</v>
+        <v>554</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>724,</v>
+        <v>730,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>970</v>
+        <v>990</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>921</v>
+        <v>928</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>921,</v>
+        <v>928,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>724</v>
+        <v>730</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>626,</v>
+        <v>635,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>921</v>
+        <v>928</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1186</v>
+        <v>1202</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1186,</v>
+        <v>1202,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>626</v>
+        <v>635</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>319,</v>
+        <v>328,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1186</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1154</v>
+        <v>1172</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1154,</v>
+        <v>1172,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>601,</v>
+        <v>605,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1154</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>694</v>
+        <v>768</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>694,</v>
+        <v>768,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>601</v>
+        <v>605</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>441,</v>
+        <v>450,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>694</v>
+        <v>768</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>253,</v>
+        <v>256,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>441</v>
+        <v>450</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>1018</v>
+        <v>1029</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1018,</v>
+        <v>1029,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>370,</v>
+        <v>377,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="3">
-        <v>1018</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>850</v>
+        <v>856</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>850,</v>
+        <v>856,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1161,</v>
+        <v>1164,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>850</v>
+        <v>856</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>300,</v>
+        <v>315,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1161</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>5248</v>
+        <v>5320</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>5248</v>
+        <v>5320</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>300</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as 04 May 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C5BBE6-9FBD-4D4F-95B0-9423221D76DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7DB767-DA68-844C-A7AC-B56C81962154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F151"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>458,</v>
+        <v>461,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>10943</v>
+        <v>11077</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>10943,</v>
+        <v>11077,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>7075</v>
+        <v>7143</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1214</v>
+        <v>1219</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1214,</v>
+        <v>1219,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1214</v>
+        <v>1219</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>24828</v>
+        <v>24988</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>24828,</v>
+        <v>24988,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>10943</v>
+        <v>11077</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>678</v>
+        <v>688</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>678,</v>
+        <v>688,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>678</v>
+        <v>688</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>20652</v>
+        <v>20931</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20652,</v>
+        <v>20931,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>24828</v>
+        <v>24988</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>212,</v>
+        <v>215,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>18967</v>
+        <v>19233</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>18967,</v>
+        <v>19233,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>8164</v>
+        <v>8251</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>452,</v>
+        <v>456,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>20125</v>
+        <v>20428</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20125,</v>
+        <v>20428,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>20125</v>
+        <v>20428</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>634,</v>
+        <v>638,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>17537</v>
+        <v>17756</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17537,</v>
+        <v>17756,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>17537</v>
+        <v>17756</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2904</v>
+        <v>2928</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2904,</v>
+        <v>2928,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2904</v>
+        <v>2928</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>6489</v>
+        <v>6571</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6489,</v>
+        <v>6571,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>6489</v>
+        <v>6571</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>331,</v>
+        <v>337,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>5320</v>
+        <v>5362</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5320,</v>
+        <v>5362,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>13577</v>
+        <v>13788</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>465,</v>
+        <v>469,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>124861</v>
+        <v>126346</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>124861</v>
+        <v>126346</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>10803</v>
+        <v>10982</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>807</v>
+        <v>819</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>807,</v>
+        <v>819,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>807</v>
+        <v>819</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>413,</v>
+        <v>415,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>217,</v>
+        <v>218,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>947</v>
+        <v>970</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>947,</v>
+        <v>970,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>947</v>
+        <v>970</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>124861</v>
+        <v>126346</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>124861,</v>
+        <v>126346,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>124861</v>
+        <v>126346</v>
       </c>
       <c r="M14" s="3">
-        <v>25528</v>
+        <v>25785</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1355</v>
+        <v>1364</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1355,</v>
+        <v>1364,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1355</v>
+        <v>1364</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>12097</v>
+        <v>12266</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12097,</v>
+        <v>12266,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3767</v>
+        <v>3836</v>
       </c>
       <c r="M15" s="2">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>381,</v>
+        <v>384,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>10329</v>
+        <v>10524</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10329,</v>
+        <v>10524,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>12097</v>
+        <v>12266</v>
       </c>
       <c r="M16" s="3">
-        <v>1559</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>626,</v>
+        <v>634,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3767</v>
+        <v>3836</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3767</v>
+        <v>3836</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>10329</v>
+        <v>10524</v>
       </c>
       <c r="M17" s="2">
-        <v>983</v>
+        <v>997</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1086</v>
+        <v>1092</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1086,</v>
+        <v>1092,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1086</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>838</v>
+        <v>845</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>838,</v>
+        <v>845,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>838</v>
+        <v>845</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>549,</v>
+        <v>553,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>252,</v>
+        <v>255,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>882343</v>
+        <v>945299</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>882343,</v>
+        <v>945299,</v>
       </c>
       <c r="K21" s="9">
-        <v>882343</v>
+        <v>945299</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>795</v>
+        <v>807</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>795,</v>
+        <v>807,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>795</v>
+        <v>807</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>695744</v>
+        <v>754715</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>695744,</v>
+        <v>754715,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>582,</v>
+        <v>585,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>186599</v>
+        <v>190584</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>186599,</v>
+        <v>190584,</v>
       </c>
       <c r="K23" s="9">
-        <v>186599</v>
+        <v>190584</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>509,</v>
+        <v>512,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>28446</v>
+        <v>28734</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>28446,</v>
+        <v>28734,</v>
       </c>
       <c r="K24" s="9">
-        <v>28446</v>
+        <v>28734</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>908</v>
+        <v>925</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>908,</v>
+        <v>925,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>908</v>
+        <v>925</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>841</v>
+        <v>859</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>841,</v>
+        <v>859,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>841</v>
+        <v>859</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>507,</v>
+        <v>512,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1504</v>
+        <v>1532</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1504,</v>
+        <v>1532,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>674</v>
+        <v>684</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>674,</v>
+        <v>684,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1504</v>
+        <v>1532</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1388</v>
+        <v>1394</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1388,</v>
+        <v>1394,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>674</v>
+        <v>684</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 03/05/2020,882343,695744,186599,28446,135</v>
+        <v>9:00 04/05/2020,945299,754715,190584,28734,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1954</v>
+        <v>1988</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1954,</v>
+        <v>1988,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1388</v>
+        <v>1394</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 03/05/2020,124861,12097,10329,3767</v>
+        <v>9:00 04/05/2020,126346,12266,10524,3836</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>297,</v>
+        <v>301,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1954</v>
+        <v>1988</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 03/05/2020,10943,24828,20652,18967,20125,17537,6489,5320,124861</v>
+        <v>9:00 04/05/2020,11077,24988,20931,19233,20428,17756,6571,5362,126346</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>500,</v>
+        <v>504,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 03/05/2020,458,1214,678,212,452,634,2904,331,465,807,413,217,947,1355,381,626,1086,838,549,252,795,582,509,908,841,507,1504,674,1388,1954,297,500,1320,727,494,324,785,1070,616,593,838,2650,875,1231,640,625,329,610,2861,549,939,197,637,307,2341,729,655,127,417,462,3418,469,451,578,566,1143,2878,1463,676,948,927,870,1454,626,1154,635,654,566,475,939,955,1626,135,378,254,489,997,1056,801,537,1148,758,1583,257,297,292,496,683,330,381,527,736,20,714,1026,829,2191,518,389,578,518,352,595,491,300,1209,660,1787,873,365,509,1105,1206,2608,673,372,474,277,282,206,601,622,554,990,730,928,635,1202,328,1172,605,768,450,256,1029,377,856,1164,315,5320</v>
+        <v>9:00 04/05/2020,461,1219,688,215,456,638,2928,337,469,819,415,218,970,1364,384,634,1092,845,553,255,807,585,512,925,859,512,1532,684,1394,1988,301,504,1331,733,498,328,825,1080,619,602,841,2664,878,1243,646,627,333,617,2887,552,945,201,654,320,2379,735,663,143,419,463,3481,475,459,595,578,1151,2920,1479,690,967,933,879,1467,628,1168,645,658,582,478,943,953,1662,136,392,256,493,1024,1060,809,541,1150,776,1601,257,300,294,501,684,330,381,535,747,21,727,1024,835,2220,530,401,583,530,356,603,496,300,1212,679,1822,888,367,524,1125,1212,2626,677,384,480,283,287,208,604,627,565,992,729,936,646,1223,333,1176,616,775,457,259,1044,386,879,1171,319,5362</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1320</v>
+        <v>1331</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1320,</v>
+        <v>1331,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>727</v>
+        <v>733</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>727,</v>
+        <v>733,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1320</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>494,</v>
+        <v>498,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>727</v>
+        <v>733</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>324,</v>
+        <v>328,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>785</v>
+        <v>825</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>785,</v>
+        <v>825,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1070</v>
+        <v>1080</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1070,</v>
+        <v>1080,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>785</v>
+        <v>825</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>616,</v>
+        <v>619,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1070</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>593</v>
+        <v>602</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>593,</v>
+        <v>602,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>838,</v>
+        <v>841,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>593</v>
+        <v>602</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2650</v>
+        <v>2664</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2650,</v>
+        <v>2664,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>838</v>
+        <v>841</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>875,</v>
+        <v>878,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2650</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1231</v>
+        <v>1243</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1231,</v>
+        <v>1243,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>875</v>
+        <v>878</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>640,</v>
+        <v>646,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1231</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>625,</v>
+        <v>627,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>640</v>
+        <v>646</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>329,</v>
+        <v>333,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>610,</v>
+        <v>617,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2861</v>
+        <v>2887</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2861,</v>
+        <v>2887,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>610</v>
+        <v>617</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>549,</v>
+        <v>552,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2861</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>939</v>
+        <v>945</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>939,</v>
+        <v>945,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>197,</v>
+        <v>201,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>939</v>
+        <v>945</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>637</v>
+        <v>654</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>637,</v>
+        <v>654,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>307,</v>
+        <v>320,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>637</v>
+        <v>654</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2341</v>
+        <v>2379</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2341,</v>
+        <v>2379,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>307</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>729</v>
+        <v>735</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>729,</v>
+        <v>735,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2341</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>655</v>
+        <v>663</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>655,</v>
+        <v>663,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>729</v>
+        <v>735</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>127,</v>
+        <v>143,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>655</v>
+        <v>663</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>417,</v>
+        <v>419,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>462,</v>
+        <v>463,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3418</v>
+        <v>3481</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3418,</v>
+        <v>3481,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>469,</v>
+        <v>475,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3418</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>451,</v>
+        <v>459,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>578</v>
+        <v>595</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>578,</v>
+        <v>595,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>566,</v>
+        <v>578,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>578</v>
+        <v>595</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1143</v>
+        <v>1151</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1143,</v>
+        <v>1151,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>566</v>
+        <v>578</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2878</v>
+        <v>2920</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2878,</v>
+        <v>2920,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1143</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1463</v>
+        <v>1479</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1463,</v>
+        <v>1479,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2878</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>676</v>
+        <v>690</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>676,</v>
+        <v>690,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1463</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>948</v>
+        <v>967</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>948,</v>
+        <v>967,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>676</v>
+        <v>690</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>927</v>
+        <v>933</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>927,</v>
+        <v>933,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>948</v>
+        <v>967</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>870</v>
+        <v>879</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>870,</v>
+        <v>879,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>927</v>
+        <v>933</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1454</v>
+        <v>1467</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1454,</v>
+        <v>1467,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>870</v>
+        <v>879</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2763,17 +2763,17 @@
       </c>
       <c r="C75" s="5">
         <f t="shared" si="3"/>
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D75" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>626,</v>
+        <v>628,</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1454</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,17 +2782,17 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1154</v>
+        <v>1168</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1154,</v>
+        <v>1168,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="2">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>635,</v>
+        <v>645,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1154</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>654,</v>
+        <v>658,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>635</v>
+        <v>645</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>566</v>
+        <v>582</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>566,</v>
+        <v>582,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>475,</v>
+        <v>478,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>566</v>
+        <v>582</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>939,</v>
+        <v>943,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>955,</v>
+        <v>953,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>939</v>
+        <v>943</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1626</v>
+        <v>1662</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1626,</v>
+        <v>1662,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>135,</v>
+        <v>136,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1626</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>378,</v>
+        <v>392,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>254,</v>
+        <v>256,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>378</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>489,</v>
+        <v>493,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>997</v>
+        <v>1024</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>997,</v>
+        <v>1024,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1056,</v>
+        <v>1060,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F89" s="2">
-        <v>997</v>
+      <c r="F89" s="3">
+        <v>1024</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>801</v>
+        <v>809</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>801,</v>
+        <v>809,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1056</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>537,</v>
+        <v>541,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>801</v>
+        <v>809</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1148,</v>
+        <v>1150,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>537</v>
+        <v>541</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>758</v>
+        <v>776</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>758,</v>
+        <v>776,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1148</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1583</v>
+        <v>1601</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1583,</v>
+        <v>1601,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>758</v>
+        <v>776</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3153,7 +3153,7 @@
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1583</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,11 +3162,11 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>297,</v>
+        <v>300,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>292,</v>
+        <v>294,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>496,</v>
+        <v>501,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>683,</v>
+        <v>684,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3248,7 +3248,7 @@
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3276,11 +3276,11 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>527,</v>
+        <v>535,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>736</v>
+        <v>747</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>736,</v>
+        <v>747,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C104" s="5">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>20,</v>
+        <v>21,</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>736</v>
+        <v>747</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>714</v>
+        <v>727</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>714,</v>
+        <v>727,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F105" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1026,</v>
+        <v>1024,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>714</v>
+        <v>727</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>829</v>
+        <v>835</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>829,</v>
+        <v>835,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="3">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2191</v>
+        <v>2220</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2191,</v>
+        <v>2220,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>829</v>
+        <v>835</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>518,</v>
+        <v>530,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2191</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>389,</v>
+        <v>401,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>578,</v>
+        <v>583,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>389</v>
+        <v>401</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>518,</v>
+        <v>530,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>578</v>
+        <v>583</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>352,</v>
+        <v>356,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>595,</v>
+        <v>603,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>491,</v>
+        <v>496,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>595</v>
+        <v>603</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3552,7 +3552,7 @@
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>491</v>
+        <v>496</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,11 +3561,11 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1209</v>
+        <v>1212</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1209,</v>
+        <v>1212,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>660</v>
+        <v>679</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>660,</v>
+        <v>679,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1209</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1787</v>
+        <v>1822</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1787,</v>
+        <v>1822,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>660</v>
+        <v>679</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>873</v>
+        <v>888</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>873,</v>
+        <v>888,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1787</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>365,</v>
+        <v>367,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>873</v>
+        <v>888</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>509</v>
+        <v>524</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>509,</v>
+        <v>524,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>1105</v>
+        <v>1125</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1105,</v>
+        <v>1125,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>509</v>
+        <v>524</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1206</v>
+        <v>1212</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1206,</v>
+        <v>1212,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="3">
-        <v>1105</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2608</v>
+        <v>2626</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2608,</v>
+        <v>2626,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1206</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>673,</v>
+        <v>677,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2608</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>372,</v>
+        <v>384,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>673</v>
+        <v>677</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>474,</v>
+        <v>480,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>372</v>
+        <v>384</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>277,</v>
+        <v>283,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>474</v>
+        <v>480</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>282,</v>
+        <v>287,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>206,</v>
+        <v>208,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>282</v>
+        <v>287</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>601,</v>
+        <v>604,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>622,</v>
+        <v>627,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>554</v>
+        <v>565</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>554,</v>
+        <v>565,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>622</v>
+        <v>627</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>990,</v>
+        <v>992,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>554</v>
+        <v>565</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>730,</v>
+        <v>729,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="2">
-        <v>990</v>
+        <v>992</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>928</v>
+        <v>936</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>928,</v>
+        <v>936,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>635</v>
+        <v>646</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>635,</v>
+        <v>646,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>928</v>
+        <v>936</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1202</v>
+        <v>1223</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1202,</v>
+        <v>1223,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>635</v>
+        <v>646</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>328,</v>
+        <v>333,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1202</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1172</v>
+        <v>1176</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1172,</v>
+        <v>1176,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>605</v>
+        <v>616</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>605,</v>
+        <v>616,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1172</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>768</v>
+        <v>775</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>768,</v>
+        <v>775,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>605</v>
+        <v>616</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>450,</v>
+        <v>457,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>768</v>
+        <v>775</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>256,</v>
+        <v>259,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>450</v>
+        <v>457</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>1029</v>
+        <v>1044</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1029,</v>
+        <v>1044,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>377,</v>
+        <v>386,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="3">
-        <v>1029</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>856</v>
+        <v>879</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>856,</v>
+        <v>879,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>377</v>
+        <v>386</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1164</v>
+        <v>1171</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1164,</v>
+        <v>1171,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>856</v>
+        <v>879</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>315,</v>
+        <v>319,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1164</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>5320</v>
+        <v>5362</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>5320</v>
+        <v>5362</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as 05 May 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7DB767-DA68-844C-A7AC-B56C81962154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583BC1B7-0171-C14A-9EE2-14DB70E6B725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="E1" sqref="E1:F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>461,</v>
+        <v>462,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>11077</v>
+        <v>11239</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>11077,</v>
+        <v>11239,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>7143</v>
+        <v>7210</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1219</v>
+        <v>1224</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1219,</v>
+        <v>1224,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1219</v>
+        <v>1224</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>24988</v>
+        <v>25240</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>24988,</v>
+        <v>25240,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>11077</v>
+        <v>11239</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>688</v>
+        <v>705</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>688,</v>
+        <v>705,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>688</v>
+        <v>705</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>20931</v>
+        <v>21226</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20931,</v>
+        <v>21226,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>24988</v>
+        <v>25240</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>215,</v>
+        <v>217,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>19233</v>
+        <v>19629</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>19233,</v>
+        <v>19629,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>8251</v>
+        <v>8331</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>456</v>
+        <v>471</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>456,</v>
+        <v>471,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>456</v>
+        <v>471</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>20428</v>
+        <v>20768</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20428,</v>
+        <v>20768,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>20428</v>
+        <v>20768</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>638,</v>
+        <v>641,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>17756</v>
+        <v>17999</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17756,</v>
+        <v>17999,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>17756</v>
+        <v>17999</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2928</v>
+        <v>2954</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2928,</v>
+        <v>2954,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2928</v>
+        <v>2954</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>6571</v>
+        <v>6657</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6571,</v>
+        <v>6657,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>6571</v>
+        <v>6657</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>337,</v>
+        <v>338,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>5362</v>
+        <v>5430</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5362,</v>
+        <v>5430,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>13788</v>
+        <v>14016</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>469,</v>
+        <v>478,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>126346</v>
+        <v>128188</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>126346</v>
+        <v>128188</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>10982</v>
+        <v>11298</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>819</v>
+        <v>833</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>819,</v>
+        <v>833,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>819</v>
+        <v>833</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>415,</v>
+        <v>420,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>218,</v>
+        <v>222,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>970</v>
+        <v>1001</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>970,</v>
+        <v>1001,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="2">
-        <v>970</v>
+      <c r="F14" s="3">
+        <v>1001</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>126346</v>
+        <v>128188</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>126346,</v>
+        <v>128188,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>126346</v>
+        <v>128188</v>
       </c>
       <c r="M14" s="3">
-        <v>25785</v>
+        <v>26441</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1364</v>
+        <v>1387</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1364,</v>
+        <v>1387,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1364</v>
+        <v>1387</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>12266</v>
+        <v>12437</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12266,</v>
+        <v>12437,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3836</v>
+        <v>3881</v>
       </c>
       <c r="M15" s="2">
-        <v>381</v>
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>384,</v>
+        <v>386,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>10524</v>
+        <v>10669</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10524,</v>
+        <v>10669,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>12266</v>
+        <v>12437</v>
       </c>
       <c r="M16" s="3">
-        <v>1571</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1571,20 +1571,20 @@
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3836</v>
+        <v>3881</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3836</v>
+        <v>3881</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>10524</v>
-      </c>
-      <c r="M17" s="2">
-        <v>997</v>
+        <v>10669</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1023</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1092</v>
+        <v>1108</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1092,</v>
+        <v>1108,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1092</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>845</v>
+        <v>859</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>845,</v>
+        <v>859,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>845</v>
+        <v>859</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>553</v>
+        <v>577</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>553,</v>
+        <v>577,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>553</v>
+        <v>577</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>255,</v>
+        <v>259,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>945299</v>
+        <v>1015138</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>945299,</v>
+        <v>1015138,</v>
       </c>
       <c r="K21" s="9">
-        <v>945299</v>
+        <v>1015138</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>807</v>
+        <v>827</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>807,</v>
+        <v>827,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>807</v>
+        <v>827</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>754715</v>
+        <v>820148</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>754715,</v>
+        <v>820148,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>585,</v>
+        <v>587,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>190584</v>
+        <v>194990</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>190584,</v>
+        <v>194990,</v>
       </c>
       <c r="K23" s="9">
-        <v>190584</v>
+        <v>194990</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>512,</v>
+        <v>513,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>28734</v>
+        <v>29427</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>28734,</v>
+        <v>29427,</v>
       </c>
       <c r="K24" s="9">
-        <v>28734</v>
+        <v>29427</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>925</v>
+        <v>937</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>925,</v>
+        <v>937,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>925</v>
+        <v>937</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>859</v>
+        <v>868</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>859,</v>
+        <v>868,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>859</v>
+        <v>868</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>512</v>
+        <v>522</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>512,</v>
+        <v>522,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1532</v>
+        <v>1551</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1532,</v>
+        <v>1551,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>512</v>
+        <v>522</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>684</v>
+        <v>709</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>684,</v>
+        <v>709,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1532</v>
+        <v>1551</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1394</v>
+        <v>1420</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1394,</v>
+        <v>1420,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>684</v>
+        <v>709</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 04/05/2020,945299,754715,190584,28734,135</v>
+        <v>9:00 05/05/2020,1015138,820148,194990,29427,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>1988</v>
+        <v>2007</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1988,</v>
+        <v>2007,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1394</v>
+        <v>1420</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 04/05/2020,126346,12266,10524,3836</v>
+        <v>9:00 05/05/2020,128188,12437,10669,3881</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>301,</v>
+        <v>303,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>1988</v>
+        <v>2007</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 04/05/2020,11077,24988,20931,19233,20428,17756,6571,5362,126346</v>
+        <v>9:00 05/05/2020,11239,25240,21226,19629,20768,17999,6657,5430,128188</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1961,21 +1961,21 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" si="3"/>
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>504,</v>
+        <v>508,</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 04/05/2020,461,1219,688,215,456,638,2928,337,469,819,415,218,970,1364,384,634,1092,845,553,255,807,585,512,925,859,512,1532,684,1394,1988,301,504,1331,733,498,328,825,1080,619,602,841,2664,878,1243,646,627,333,617,2887,552,945,201,654,320,2379,735,663,143,419,463,3481,475,459,595,578,1151,2920,1479,690,967,933,879,1467,628,1168,645,658,582,478,943,953,1662,136,392,256,493,1024,1060,809,541,1150,776,1601,257,300,294,501,684,330,381,535,747,21,727,1024,835,2220,530,401,583,530,356,603,496,300,1212,679,1822,888,367,524,1125,1212,2626,677,384,480,283,287,208,604,627,565,992,729,936,646,1223,333,1176,616,775,457,259,1044,386,879,1171,319,5362</v>
+        <v>9:00 05/05/2020,462,1224,705,217,471,641,2954,338,478,833,420,222,1001,1387,386,634,1108,859,577,259,827,587,513,937,868,522,1551,709,1420,2007,303,508,1344,750,522,330,843,1102,660,613,844,2699,887,1267,652,630,333,627,2915,555,951,210,659,323,2411,737,676,145,423,472,3544,509,472,621,583,1156,2962,1513,696,984,938,884,1483,628,1192,652,659,588,479,946,958,1697,137,406,257,493,1055,1064,813,543,1165,798,1630,265,305,296,507,696,333,384,557,761,22,758,1050,841,2248,548,417,586,539,358,610,509,300,1218,678,1843,896,374,532,1139,1223,2647,693,384,489,289,289,209,607,637,572,1010,731,942,649,1241,335,1185,629,818,465,261,1056,397,887,1201,329,5430</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1331</v>
+        <v>1344</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1331,</v>
+        <v>1344,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="2">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>733</v>
+        <v>750</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>733,</v>
+        <v>750,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1331</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>498</v>
+        <v>522</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>498,</v>
+        <v>522,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>733</v>
+        <v>750</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>328,</v>
+        <v>330,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>498</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>825</v>
+        <v>843</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>825,</v>
+        <v>843,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1080,</v>
+        <v>1102,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>825</v>
+        <v>843</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>619</v>
+        <v>660</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>619,</v>
+        <v>660,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1080</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>602</v>
+        <v>613</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>602,</v>
+        <v>613,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>619</v>
+        <v>660</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>841,</v>
+        <v>844,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>602</v>
+        <v>613</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2664</v>
+        <v>2699</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2664,</v>
+        <v>2699,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>841</v>
+        <v>844</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>878</v>
+        <v>887</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>878,</v>
+        <v>887,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2664</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1243</v>
+        <v>1267</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1243,</v>
+        <v>1267,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>878</v>
+        <v>887</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>646,</v>
+        <v>652,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1243</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>627,</v>
+        <v>630,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>646</v>
+        <v>652</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2260,7 +2260,7 @@
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,11 +2269,11 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>617,</v>
+        <v>627,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2887</v>
+        <v>2915</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2887,</v>
+        <v>2915,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>617</v>
+        <v>627</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>552,</v>
+        <v>555,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2887</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>945</v>
+        <v>951</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>945,</v>
+        <v>951,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>201,</v>
+        <v>210,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>945</v>
+        <v>951</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>654,</v>
+        <v>659,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>320,</v>
+        <v>323,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>654</v>
+        <v>659</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2379</v>
+        <v>2411</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2379,</v>
+        <v>2411,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>735,</v>
+        <v>737,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2379</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>663</v>
+        <v>676</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>663,</v>
+        <v>676,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>143,</v>
+        <v>145,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>663</v>
+        <v>676</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>419,</v>
+        <v>423,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>463,</v>
+        <v>472,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3481</v>
+        <v>3544</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3481,</v>
+        <v>3544,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>475</v>
+        <v>509</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>475,</v>
+        <v>509,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3481</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>459</v>
+        <v>472</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>459,</v>
+        <v>472,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>475</v>
+        <v>509</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>595</v>
+        <v>621</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>595,</v>
+        <v>621,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>459</v>
+        <v>472</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>578,</v>
+        <v>583,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>595</v>
+        <v>621</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1151</v>
+        <v>1156</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1151,</v>
+        <v>1156,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>578</v>
+        <v>583</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2920</v>
+        <v>2962</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2920,</v>
+        <v>2962,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1151</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1479</v>
+        <v>1513</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1479,</v>
+        <v>1513,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2920</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>690,</v>
+        <v>696,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1479</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>967</v>
+        <v>984</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>967,</v>
+        <v>984,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>690</v>
+        <v>696</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>933</v>
+        <v>938</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>933,</v>
+        <v>938,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>967</v>
+        <v>984</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>879,</v>
+        <v>884,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>933</v>
+        <v>938</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1467</v>
+        <v>1483</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1467,</v>
+        <v>1483,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>879</v>
+        <v>884</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2773,7 +2773,7 @@
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1467</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,11 +2782,11 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1168</v>
+        <v>1192</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1168,</v>
+        <v>1192,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>645</v>
+        <v>652</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>645,</v>
+        <v>652,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1168</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>658,</v>
+        <v>659,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>645</v>
+        <v>652</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>582</v>
+        <v>588</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>582,</v>
+        <v>588,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>478,</v>
+        <v>479,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>582</v>
+        <v>588</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>943</v>
+        <v>946</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>943,</v>
+        <v>946,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>953</v>
+        <v>958</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>953,</v>
+        <v>958,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>943</v>
+        <v>946</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1662</v>
+        <v>1697</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1662,</v>
+        <v>1697,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>953</v>
+        <v>958</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2934,17 +2934,17 @@
       </c>
       <c r="C84" s="5">
         <f t="shared" si="3"/>
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D84" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>136,</v>
+        <v>137,</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1662</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,17 +2953,17 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>392,</v>
+        <v>406,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F85" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>256,</v>
+        <v>257,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>392</v>
+        <v>406</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -3001,7 +3001,7 @@
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,11 +3010,11 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>1024</v>
+        <v>1055</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1024,</v>
+        <v>1055,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1060</v>
+        <v>1064</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1060,</v>
+        <v>1064,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="3">
-        <v>1024</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>809,</v>
+        <v>813,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1060</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>541,</v>
+        <v>543,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>809</v>
+        <v>813</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1150</v>
+        <v>1165</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1150,</v>
+        <v>1165,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>776</v>
+        <v>798</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>776,</v>
+        <v>798,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1150</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1601</v>
+        <v>1630</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1601,</v>
+        <v>1630,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>776</v>
+        <v>798</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>257,</v>
+        <v>265,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1601</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>300,</v>
+        <v>305,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>257</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>294,</v>
+        <v>296,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>501,</v>
+        <v>507,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>684</v>
+        <v>696</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>684,</v>
+        <v>696,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>501</v>
+        <v>507</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>330,</v>
+        <v>333,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>684</v>
+        <v>696</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C101" s="5">
         <f t="shared" si="5"/>
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D101" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>381,</v>
+        <v>384,</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,17 +3276,17 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>535</v>
+        <v>557</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>535,</v>
+        <v>557,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F102" s="2">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>747</v>
+        <v>761</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>747,</v>
+        <v>761,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>535</v>
+        <v>557</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C104" s="5">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>21,</v>
+        <v>22,</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>747</v>
+        <v>761</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>727</v>
+        <v>758</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>727,</v>
+        <v>758,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F105" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>1024</v>
+        <v>1050</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1024,</v>
+        <v>1050,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>727</v>
+        <v>758</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>835</v>
+        <v>841</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>835,</v>
+        <v>841,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="3">
-        <v>1024</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2220</v>
+        <v>2248</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2220,</v>
+        <v>2248,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>835</v>
+        <v>841</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>530</v>
+        <v>548</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>530,</v>
+        <v>548,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2220</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>401</v>
+        <v>417</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>401,</v>
+        <v>417,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>530</v>
+        <v>548</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>583,</v>
+        <v>586,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>401</v>
+        <v>417</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>530</v>
+        <v>539</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>530,</v>
+        <v>539,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>356,</v>
+        <v>358,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>530</v>
+        <v>539</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>603,</v>
+        <v>610,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>496</v>
+        <v>509</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>496,</v>
+        <v>509,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>603</v>
+        <v>610</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3552,7 +3552,7 @@
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>496</v>
+        <v>509</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,11 +3561,11 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1212</v>
+        <v>1218</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1212,</v>
+        <v>1218,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>679,</v>
+        <v>678,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1212</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1822</v>
+        <v>1843</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1822,</v>
+        <v>1843,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>888</v>
+        <v>896</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>888,</v>
+        <v>896,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1822</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>367,</v>
+        <v>374,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>888</v>
+        <v>896</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>524,</v>
+        <v>532,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>367</v>
+        <v>374</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1125,</v>
+        <v>1139,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1212</v>
+        <v>1223</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1212,</v>
+        <v>1223,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="3">
-        <v>1125</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2626</v>
+        <v>2647</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2626,</v>
+        <v>2647,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1212</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>677</v>
+        <v>693</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>677,</v>
+        <v>693,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2626</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3761,7 +3761,7 @@
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>677</v>
+        <v>693</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,11 +3770,11 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>480</v>
+        <v>489</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>480,</v>
+        <v>489,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C129" s="5">
         <f t="shared" si="5"/>
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="D129" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>283,</v>
+        <v>289,</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>480</v>
+        <v>489</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,17 +3808,17 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>287,</v>
+        <v>289,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F130" s="2">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C131" s="5">
         <f t="shared" si="5"/>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D131" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>208,</v>
+        <v>209,</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,17 +3846,17 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>604,</v>
+        <v>607,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F132" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>627,</v>
+        <v>637,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>565,</v>
+        <v>572,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>627</v>
+        <v>637</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>992</v>
+        <v>1010</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>992,</v>
+        <v>1010,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>565</v>
+        <v>572</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>729,</v>
+        <v>731,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F136" s="2">
-        <v>992</v>
+      <c r="F136" s="3">
+        <v>1010</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>936</v>
+        <v>942</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>936,</v>
+        <v>942,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>729</v>
+        <v>731</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>646,</v>
+        <v>649,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>936</v>
+        <v>942</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1223</v>
+        <v>1241</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1223,</v>
+        <v>1241,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -3998,17 +3998,17 @@
       </c>
       <c r="C140" s="5">
         <f t="shared" si="5"/>
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>333,</v>
+        <v>335,</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1223</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1176</v>
+        <v>1185</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1176,</v>
+        <v>1185,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F141" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>616</v>
+        <v>629</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>616,</v>
+        <v>629,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1176</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>775</v>
+        <v>818</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>775,</v>
+        <v>818,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>616</v>
+        <v>629</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>457,</v>
+        <v>465,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>775</v>
+        <v>818</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>259,</v>
+        <v>261,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>457</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>1044</v>
+        <v>1056</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1044,</v>
+        <v>1056,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>386,</v>
+        <v>397,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="3">
-        <v>1044</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>879</v>
+        <v>887</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>879,</v>
+        <v>887,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>386</v>
+        <v>397</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1171</v>
+        <v>1201</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1171,</v>
+        <v>1201,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>879</v>
+        <v>887</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>319,</v>
+        <v>329,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1171</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>5362</v>
+        <v>5430</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>5362</v>
+        <v>5430</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>319</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data as 06 May 2020
</commit_message>
<xml_diff>
--- a/asset/loading-data-helper.xlsx
+++ b/asset/loading-data-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/covid-19-uk/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583BC1B7-0171-C14A-9EE2-14DB70E6B725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37FAAF7-0988-7C47-A26A-6CFF8EDDC660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{956908E7-D61C-DD4E-8DD7-4809B420B199}"/>
   </bookViews>
@@ -1047,34 +1047,34 @@
       </c>
       <c r="C2" s="5">
         <f>F2</f>
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(C2,",")</f>
-        <v>462,</v>
+        <v>465,</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
       </c>
       <c r="I2" s="5">
         <f>L3</f>
-        <v>11239</v>
+        <v>11390</v>
       </c>
       <c r="J2" s="6" t="str">
         <f>_xlfn.CONCAT(I2,",")</f>
-        <v>11239,</v>
+        <v>11390,</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="L2" s="3">
-        <v>7210</v>
+        <v>7292</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1083,34 +1083,34 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C26" si="1">F3</f>
-        <v>1224</v>
+        <v>1233</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1224,</v>
+        <v>1233,</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1224</v>
+        <v>1233</v>
       </c>
       <c r="H3" t="s">
         <v>161</v>
       </c>
       <c r="I3" s="5">
         <f>L4</f>
-        <v>25240</v>
+        <v>25357</v>
       </c>
       <c r="J3" s="6" t="str">
         <f t="shared" ref="J3:J24" si="2">_xlfn.CONCAT(I3,",")</f>
-        <v>25240,</v>
+        <v>25357,</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L3" s="3">
-        <v>11239</v>
+        <v>11390</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1119,34 +1119,34 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>705,</v>
+        <v>710,</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="H4" t="s">
         <v>162</v>
       </c>
       <c r="I4" s="5">
         <f>L2+L9</f>
-        <v>21226</v>
+        <v>21443</v>
       </c>
       <c r="J4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>21226,</v>
+        <v>21443,</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="L4" s="3">
-        <v>25240</v>
+        <v>25357</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -1155,34 +1155,34 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>217,</v>
+        <v>219,</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
         <v>163</v>
       </c>
       <c r="I5" s="5">
         <f>L5+L10</f>
-        <v>19629</v>
+        <v>19872</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>19629,</v>
+        <v>19872,</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>172</v>
       </c>
       <c r="L5" s="3">
-        <v>8331</v>
+        <v>8395</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>471,</v>
+        <v>476,</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="H6" t="s">
         <v>164</v>
       </c>
       <c r="I6" s="5">
         <f>L6</f>
-        <v>20768</v>
+        <v>21000</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>20768,</v>
+        <v>21000,</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>173</v>
       </c>
       <c r="L6" s="3">
-        <v>20768</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>641,</v>
+        <v>646,</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="H7" t="s">
         <v>165</v>
       </c>
       <c r="I7" s="5">
         <f>L7</f>
-        <v>17999</v>
+        <v>18509</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>17999,</v>
+        <v>18509,</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="3">
-        <v>17999</v>
+        <v>18509</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1263,34 +1263,34 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>2954</v>
+        <v>2977</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2954,</v>
+        <v>2977,</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>2954</v>
+        <v>2977</v>
       </c>
       <c r="H8" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="5">
         <f>L8</f>
-        <v>6657</v>
+        <v>6726</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>6657,</v>
+        <v>6726,</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="3">
-        <v>6657</v>
+        <v>6726</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1299,34 +1299,34 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>338,</v>
+        <v>339,</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H9" t="s">
         <v>167</v>
       </c>
       <c r="I9" s="5">
         <f>I14-SUM(I2:I8)</f>
-        <v>5430</v>
+        <v>5502</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>5430,</v>
+        <v>5502,</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="L9" s="3">
-        <v>14016</v>
+        <v>14151</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1335,34 +1335,34 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>478,</v>
+        <v>483,</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="H10" t="s">
         <v>168</v>
       </c>
       <c r="I10" s="5">
         <f>I14</f>
-        <v>128188</v>
+        <v>129799</v>
       </c>
       <c r="J10" s="6" t="str">
         <f>_xlfn.CONCAT(I10)</f>
-        <v>128188</v>
+        <v>129799</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="3">
-        <v>11298</v>
+        <v>11477</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>833</v>
+        <v>842</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>833,</v>
+        <v>842,</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2">
-        <v>833</v>
+        <v>842</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>441</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>420,</v>
+        <v>441,</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="2">
-        <v>420</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1409,17 +1409,17 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>222,</v>
+        <v>225,</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>192</v>
@@ -1437,37 +1437,37 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>1001</v>
+        <v>1022</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1001,</v>
+        <v>1022,</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="3">
-        <v>1001</v>
+        <v>1022</v>
       </c>
       <c r="H14" t="s">
         <v>178</v>
       </c>
       <c r="I14" s="5">
         <f>L14</f>
-        <v>128188</v>
+        <v>129799</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>128188,</v>
+        <v>129799,</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L14" s="3">
-        <v>128188</v>
+        <v>129799</v>
       </c>
       <c r="M14" s="3">
-        <v>26441</v>
+        <v>27008</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1476,37 +1476,37 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="1"/>
-        <v>1387</v>
+        <v>1389</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1387,</v>
+        <v>1389,</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1387</v>
+        <v>1389</v>
       </c>
       <c r="H15" t="s">
         <v>179</v>
       </c>
       <c r="I15" s="5">
         <f>L16</f>
-        <v>12437</v>
+        <v>12709</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>12437,</v>
+        <v>12709,</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>184</v>
       </c>
       <c r="L15" s="3">
-        <v>3881</v>
+        <v>3934</v>
       </c>
       <c r="M15" s="2">
-        <v>387</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1515,37 +1515,37 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" si="1"/>
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>386,</v>
+        <v>390,</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="H16" t="s">
         <v>180</v>
       </c>
       <c r="I16" s="5">
         <f>L17</f>
-        <v>10669</v>
+        <v>10764</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10669,</v>
+        <v>10764,</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="L16" s="3">
-        <v>12437</v>
+        <v>12709</v>
       </c>
       <c r="M16" s="3">
-        <v>1576</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -1554,37 +1554,37 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>634,</v>
+        <v>640,</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F17" s="2">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="H17" t="s">
         <v>181</v>
       </c>
       <c r="I17" s="5">
         <f>L15</f>
-        <v>3881</v>
+        <v>3934</v>
       </c>
       <c r="J17" s="6" t="str">
         <f>_xlfn.CONCAT(I17)</f>
-        <v>3881</v>
+        <v>3934</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
       <c r="L17" s="3">
-        <v>10669</v>
+        <v>10764</v>
       </c>
       <c r="M17" s="3">
-        <v>1023</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>1108</v>
+        <v>1116</v>
       </c>
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1108,</v>
+        <v>1116,</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="3">
-        <v>1108</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" si="1"/>
-        <v>859</v>
+        <v>864</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>859,</v>
+        <v>864,</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="2">
-        <v>859</v>
+        <v>864</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -1631,17 +1631,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>577</v>
+        <v>590</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>577,</v>
+        <v>590,</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>577</v>
+        <v>590</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="18">
@@ -1650,31 +1650,31 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>259,</v>
+        <v>260,</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
       <c r="I21" s="5">
         <f>K21</f>
-        <v>1015138</v>
+        <v>1072144</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>1015138,</v>
+        <v>1072144,</v>
       </c>
       <c r="K21" s="9">
-        <v>1015138</v>
+        <v>1072144</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1683,28 +1683,28 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" si="1"/>
-        <v>827</v>
+        <v>843</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>827,</v>
+        <v>843,</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>827</v>
+        <v>843</v>
       </c>
       <c r="H22" t="s">
         <v>188</v>
       </c>
       <c r="I22" s="5">
         <f>I21-I23</f>
-        <v>820148</v>
+        <v>871043</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>820148,</v>
+        <v>871043,</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="18">
@@ -1713,31 +1713,31 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" si="1"/>
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>587,</v>
+        <v>588,</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="H23" t="s">
         <v>189</v>
       </c>
       <c r="I23" s="5">
         <f>K23</f>
-        <v>194990</v>
+        <v>201101</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>194990,</v>
+        <v>201101,</v>
       </c>
       <c r="K23" s="9">
-        <v>194990</v>
+        <v>201101</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="18">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" si="1"/>
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>513,</v>
+        <v>517,</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="H24" t="s">
         <v>190</v>
       </c>
       <c r="I24" s="5">
         <f>K24</f>
-        <v>29427</v>
+        <v>30076</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>29427,</v>
+        <v>30076,</v>
       </c>
       <c r="K24" s="9">
-        <v>29427</v>
+        <v>30076</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1779,17 +1779,17 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" si="1"/>
-        <v>937</v>
+        <v>953</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>937,</v>
+        <v>953,</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>937</v>
+        <v>953</v>
       </c>
       <c r="H25" t="s">
         <v>191</v>
@@ -1812,17 +1812,17 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" si="1"/>
-        <v>868</v>
+        <v>881</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>868,</v>
+        <v>881,</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>868</v>
+        <v>881</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="C27" s="5">
         <f>F28</f>
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>522,</v>
+        <v>524,</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>155</v>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ref="C28:C91" si="3">F29</f>
-        <v>1551</v>
+        <v>1572</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1551,</v>
+        <v>1572,</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -1869,21 +1869,21 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="3"/>
-        <v>709</v>
+        <v>720</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>709,</v>
+        <v>720,</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="3">
-        <v>1551</v>
+        <v>1572</v>
       </c>
       <c r="H29" s="7">
         <f ca="1">TODAY()</f>
-        <v>43956</v>
+        <v>43957</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -1892,21 +1892,21 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" si="3"/>
-        <v>1420</v>
+        <v>1430</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1420,</v>
+        <v>1430,</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="2">
-        <v>709</v>
+        <v>720</v>
       </c>
       <c r="H30" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J21:J25)</f>
-        <v>9:00 05/05/2020,1015138,820148,194990,29427,135</v>
+        <v>9:00 06/05/2020,1072144,871043,201101,30076,135</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -1915,21 +1915,21 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" si="3"/>
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2007,</v>
+        <v>2012,</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="3">
-        <v>1420</v>
+        <v>1430</v>
       </c>
       <c r="H31" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J14:J17)</f>
-        <v>9:00 05/05/2020,128188,12437,10669,3881</v>
+        <v>9:00 06/05/2020,129799,12709,10764,3934</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -1938,21 +1938,21 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" si="3"/>
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>303,</v>
+        <v>306,</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="3">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="H32" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  J2:J10)</f>
-        <v>9:00 05/05/2020,11239,25240,21226,19629,20768,17999,6657,5430,128188</v>
+        <v>9:00 06/05/2020,11390,25357,21443,19872,21000,18509,6726,5502,129799</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -1971,11 +1971,11 @@
         <v>30</v>
       </c>
       <c r="F33" s="2">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="H33" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("9:00 ",TEXT( TODAY(), "dd/mm/yyyy"), ",",  D2:D151)</f>
-        <v>9:00 05/05/2020,462,1224,705,217,471,641,2954,338,478,833,420,222,1001,1387,386,634,1108,859,577,259,827,587,513,937,868,522,1551,709,1420,2007,303,508,1344,750,522,330,843,1102,660,613,844,2699,887,1267,652,630,333,627,2915,555,951,210,659,323,2411,737,676,145,423,472,3544,509,472,621,583,1156,2962,1513,696,984,938,884,1483,628,1192,652,659,588,479,946,958,1697,137,406,257,493,1055,1064,813,543,1165,798,1630,265,305,296,507,696,333,384,557,761,22,758,1050,841,2248,548,417,586,539,358,610,509,300,1218,678,1843,896,374,532,1139,1223,2647,693,384,489,289,289,209,607,637,572,1010,731,942,649,1241,335,1185,629,818,465,261,1056,397,887,1201,329,5430</v>
+        <v>9:00 06/05/2020,465,1233,710,219,476,646,2977,339,483,842,441,225,1022,1389,390,640,1116,864,590,260,843,588,517,953,881,524,1572,720,1430,2012,306,508,1355,753,540,340,855,1105,682,627,848,2725,888,1268,654,631,335,630,2944,561,958,216,662,329,2434,738,680,146,426,473,3911,534,475,629,584,1160,3010,1534,714,995,944,896,1497,628,1204,654,661,589,484,955,964,1733,137,409,258,495,1073,1072,819,551,1178,808,1633,278,309,297,514,701,337,384,566,768,23,768,1057,846,2250,552,419,591,549,361,611,513,305,1220,681,1865,908,380,540,1159,1227,2677,697,388,504,289,292,209,608,644,581,1021,733,946,650,1255,335,1211,631,828,467,264,1067,401,893,1207,348,5502</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1984,11 +1984,11 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" si="3"/>
-        <v>1344</v>
+        <v>1355</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1344,</v>
+        <v>1355,</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>31</v>
@@ -2003,17 +2003,17 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" si="3"/>
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>750,</v>
+        <v>753,</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="3">
-        <v>1344</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="36" spans="2:8">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" si="3"/>
-        <v>522</v>
+        <v>540</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>522,</v>
+        <v>540,</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="2">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="37" spans="2:8">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>330,</v>
+        <v>340,</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>522</v>
+        <v>540</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -2060,17 +2060,17 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" si="3"/>
-        <v>843</v>
+        <v>855</v>
       </c>
       <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>843,</v>
+        <v>855,</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="2">
-        <v>330</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="2:8">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" si="3"/>
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1102,</v>
+        <v>1105,</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="2">
-        <v>843</v>
+        <v>855</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" si="3"/>
-        <v>660</v>
+        <v>682</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>660,</v>
+        <v>682,</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="3">
-        <v>1102</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -2117,17 +2117,17 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" si="3"/>
-        <v>613</v>
+        <v>627</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>613,</v>
+        <v>627,</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="2">
-        <v>660</v>
+        <v>682</v>
       </c>
     </row>
     <row r="42" spans="2:8">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" si="3"/>
-        <v>844</v>
+        <v>848</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>844,</v>
+        <v>848,</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="2">
-        <v>613</v>
+        <v>627</v>
       </c>
     </row>
     <row r="43" spans="2:8">
@@ -2155,17 +2155,17 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" si="3"/>
-        <v>2699</v>
+        <v>2725</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2699,</v>
+        <v>2725,</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="2">
-        <v>844</v>
+        <v>848</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" si="3"/>
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>887,</v>
+        <v>888,</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="3">
-        <v>2699</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="45" spans="2:8">
@@ -2193,17 +2193,17 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" si="3"/>
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1267,</v>
+        <v>1268,</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="2">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -2212,17 +2212,17 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" si="3"/>
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>652,</v>
+        <v>654,</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="3">
-        <v>1267</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -2231,17 +2231,17 @@
       </c>
       <c r="C47" s="5">
         <f>F48+F27</f>
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>630,</v>
+        <v>631,</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="2">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -2250,17 +2250,17 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" si="3"/>
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>333,</v>
+        <v>335,</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>156</v>
       </c>
       <c r="F48" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2269,17 +2269,17 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" si="3"/>
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>627,</v>
+        <v>630,</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2288,17 +2288,17 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" si="3"/>
-        <v>2915</v>
+        <v>2944</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2915,</v>
+        <v>2944,</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="2">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" si="3"/>
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>555,</v>
+        <v>561,</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="3">
-        <v>2915</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="52" spans="2:6">
@@ -2326,17 +2326,17 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" si="3"/>
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>951,</v>
+        <v>958,</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="2">
-        <v>555</v>
+        <v>561</v>
       </c>
     </row>
     <row r="53" spans="2:6">
@@ -2345,17 +2345,17 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" si="3"/>
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>210,</v>
+        <v>216,</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="2">
-        <v>951</v>
+        <v>958</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2364,17 +2364,17 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" si="3"/>
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>659,</v>
+        <v>662,</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="2">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="2:6">
@@ -2383,17 +2383,17 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" si="3"/>
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>323,</v>
+        <v>329,</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F55" s="2">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2402,17 +2402,17 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" si="3"/>
-        <v>2411</v>
+        <v>2434</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2411,</v>
+        <v>2434,</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>157</v>
       </c>
       <c r="F56" s="2">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" si="3"/>
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>737,</v>
+        <v>738,</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="3">
-        <v>2411</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" si="3"/>
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>676,</v>
+        <v>680,</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F58" s="2">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" si="3"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>145,</v>
+        <v>146,</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F59" s="2">
-        <v>676</v>
+        <v>680</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2478,17 +2478,17 @@
       </c>
       <c r="C60" s="5">
         <f t="shared" si="3"/>
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>423,</v>
+        <v>426,</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="C61" s="5">
         <f t="shared" si="3"/>
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>472,</v>
+        <v>473,</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F61" s="2">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2516,17 +2516,17 @@
       </c>
       <c r="C62" s="5">
         <f t="shared" si="3"/>
-        <v>3544</v>
+        <v>3911</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3544,</v>
+        <v>3911,</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F62" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2535,17 +2535,17 @@
       </c>
       <c r="C63" s="5">
         <f t="shared" si="3"/>
-        <v>509</v>
+        <v>534</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>509,</v>
+        <v>534,</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F63" s="3">
-        <v>3544</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C64" s="5">
         <f t="shared" si="3"/>
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>472,</v>
+        <v>475,</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F64" s="2">
-        <v>509</v>
+        <v>534</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -2573,17 +2573,17 @@
       </c>
       <c r="C65" s="5">
         <f t="shared" si="3"/>
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>621,</v>
+        <v>629,</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="2">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C66" s="5">
         <f t="shared" si="3"/>
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D66" s="6" t="str">
         <f t="shared" ref="D66:D129" si="4">_xlfn.CONCAT(C66,",")</f>
-        <v>583,</v>
+        <v>584,</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="2">
-        <v>621</v>
+        <v>629</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -2611,17 +2611,17 @@
       </c>
       <c r="C67" s="5">
         <f t="shared" si="3"/>
-        <v>1156</v>
+        <v>1160</v>
       </c>
       <c r="D67" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1156,</v>
+        <v>1160,</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="C68" s="5">
         <f t="shared" si="3"/>
-        <v>2962</v>
+        <v>3010</v>
       </c>
       <c r="D68" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2962,</v>
+        <v>3010,</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F68" s="3">
-        <v>1156</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C69" s="5">
         <f t="shared" si="3"/>
-        <v>1513</v>
+        <v>1534</v>
       </c>
       <c r="D69" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1513,</v>
+        <v>1534,</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F69" s="3">
-        <v>2962</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -2668,17 +2668,17 @@
       </c>
       <c r="C70" s="5">
         <f t="shared" si="3"/>
-        <v>696</v>
+        <v>714</v>
       </c>
       <c r="D70" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>696,</v>
+        <v>714,</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F70" s="3">
-        <v>1513</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C71" s="5">
         <f t="shared" si="3"/>
-        <v>984</v>
+        <v>995</v>
       </c>
       <c r="D71" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>984,</v>
+        <v>995,</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F71" s="2">
-        <v>696</v>
+        <v>714</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2706,17 +2706,17 @@
       </c>
       <c r="C72" s="5">
         <f t="shared" si="3"/>
-        <v>938</v>
+        <v>944</v>
       </c>
       <c r="D72" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>938,</v>
+        <v>944,</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F72" s="2">
-        <v>984</v>
+        <v>995</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2725,17 +2725,17 @@
       </c>
       <c r="C73" s="5">
         <f t="shared" si="3"/>
-        <v>884</v>
+        <v>896</v>
       </c>
       <c r="D73" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>884,</v>
+        <v>896,</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F73" s="2">
-        <v>938</v>
+        <v>944</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2744,17 +2744,17 @@
       </c>
       <c r="C74" s="5">
         <f t="shared" si="3"/>
-        <v>1483</v>
+        <v>1497</v>
       </c>
       <c r="D74" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1483,</v>
+        <v>1497,</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F74" s="2">
-        <v>884</v>
+        <v>896</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2773,7 +2773,7 @@
         <v>72</v>
       </c>
       <c r="F75" s="3">
-        <v>1483</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2782,11 +2782,11 @@
       </c>
       <c r="C76" s="5">
         <f t="shared" si="3"/>
-        <v>1192</v>
+        <v>1204</v>
       </c>
       <c r="D76" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1192,</v>
+        <v>1204,</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>73</v>
@@ -2801,17 +2801,17 @@
       </c>
       <c r="C77" s="5">
         <f t="shared" si="3"/>
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D77" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>652,</v>
+        <v>654,</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F77" s="3">
-        <v>1192</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2820,17 +2820,17 @@
       </c>
       <c r="C78" s="5">
         <f t="shared" si="3"/>
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D78" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>659,</v>
+        <v>661,</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F78" s="2">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2839,17 +2839,17 @@
       </c>
       <c r="C79" s="5">
         <f t="shared" si="3"/>
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D79" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>588,</v>
+        <v>589,</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F79" s="2">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="C80" s="5">
         <f t="shared" si="3"/>
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="D80" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>479,</v>
+        <v>484,</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F80" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2877,17 +2877,17 @@
       </c>
       <c r="C81" s="5">
         <f t="shared" si="3"/>
-        <v>946</v>
+        <v>955</v>
       </c>
       <c r="D81" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>946,</v>
+        <v>955,</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F81" s="2">
-        <v>479</v>
+        <v>484</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2896,17 +2896,17 @@
       </c>
       <c r="C82" s="5">
         <f t="shared" si="3"/>
-        <v>958</v>
+        <v>964</v>
       </c>
       <c r="D82" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>958,</v>
+        <v>964,</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F82" s="2">
-        <v>946</v>
+        <v>955</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2915,17 +2915,17 @@
       </c>
       <c r="C83" s="5">
         <f t="shared" si="3"/>
-        <v>1697</v>
+        <v>1733</v>
       </c>
       <c r="D83" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1697,</v>
+        <v>1733,</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F83" s="2">
-        <v>958</v>
+        <v>964</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2944,7 +2944,7 @@
         <v>81</v>
       </c>
       <c r="F84" s="3">
-        <v>1697</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2953,11 +2953,11 @@
       </c>
       <c r="C85" s="5">
         <f t="shared" si="3"/>
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="D85" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>406,</v>
+        <v>409,</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>82</v>
@@ -2972,17 +2972,17 @@
       </c>
       <c r="C86" s="5">
         <f t="shared" si="3"/>
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D86" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>257,</v>
+        <v>258,</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F86" s="2">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="C87" s="5">
         <f t="shared" si="3"/>
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D87" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>493,</v>
+        <v>495,</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F87" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="C88" s="5">
         <f t="shared" si="3"/>
-        <v>1055</v>
+        <v>1073</v>
       </c>
       <c r="D88" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1055,</v>
+        <v>1073,</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F88" s="2">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="89" spans="2:6">
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C89" s="5">
         <f t="shared" si="3"/>
-        <v>1064</v>
+        <v>1072</v>
       </c>
       <c r="D89" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1064,</v>
+        <v>1072,</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F89" s="3">
-        <v>1055</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -3048,17 +3048,17 @@
       </c>
       <c r="C90" s="5">
         <f t="shared" si="3"/>
-        <v>813</v>
+        <v>819</v>
       </c>
       <c r="D90" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>813,</v>
+        <v>819,</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F90" s="3">
-        <v>1064</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="C91" s="5">
         <f t="shared" si="3"/>
-        <v>543</v>
+        <v>551</v>
       </c>
       <c r="D91" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>543,</v>
+        <v>551,</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>813</v>
+        <v>819</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -3086,17 +3086,17 @@
       </c>
       <c r="C92" s="5">
         <f t="shared" ref="C92:C150" si="5">F93</f>
-        <v>1165</v>
+        <v>1178</v>
       </c>
       <c r="D92" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1165,</v>
+        <v>1178,</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F92" s="2">
-        <v>543</v>
+        <v>551</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -3105,17 +3105,17 @@
       </c>
       <c r="C93" s="5">
         <f t="shared" si="5"/>
-        <v>798</v>
+        <v>808</v>
       </c>
       <c r="D93" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>798,</v>
+        <v>808,</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="3">
-        <v>1165</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C94" s="5">
         <f t="shared" si="5"/>
-        <v>1630</v>
+        <v>1633</v>
       </c>
       <c r="D94" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1630,</v>
+        <v>1633,</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F94" s="2">
-        <v>798</v>
+        <v>808</v>
       </c>
     </row>
     <row r="95" spans="2:6">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="C95" s="5">
         <f t="shared" si="5"/>
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="D95" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>265,</v>
+        <v>278,</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="3">
-        <v>1630</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -3162,17 +3162,17 @@
       </c>
       <c r="C96" s="5">
         <f t="shared" si="5"/>
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D96" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>305,</v>
+        <v>309,</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="2">
-        <v>265</v>
+        <v>278</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3181,17 +3181,17 @@
       </c>
       <c r="C97" s="5">
         <f t="shared" si="5"/>
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D97" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>296,</v>
+        <v>297,</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="2">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3200,17 +3200,17 @@
       </c>
       <c r="C98" s="5">
         <f t="shared" si="5"/>
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="D98" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>507,</v>
+        <v>514,</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3219,17 +3219,17 @@
       </c>
       <c r="C99" s="5">
         <f t="shared" si="5"/>
-        <v>696</v>
+        <v>701</v>
       </c>
       <c r="D99" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>696,</v>
+        <v>701,</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F99" s="2">
-        <v>507</v>
+        <v>514</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -3238,17 +3238,17 @@
       </c>
       <c r="C100" s="5">
         <f t="shared" si="5"/>
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="D100" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>333,</v>
+        <v>337,</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F100" s="2">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -3267,7 +3267,7 @@
         <v>98</v>
       </c>
       <c r="F101" s="2">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -3276,11 +3276,11 @@
       </c>
       <c r="C102" s="5">
         <f t="shared" si="5"/>
-        <v>557</v>
+        <v>566</v>
       </c>
       <c r="D102" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>557,</v>
+        <v>566,</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>99</v>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C103" s="5">
         <f t="shared" si="5"/>
-        <v>761</v>
+        <v>768</v>
       </c>
       <c r="D103" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>761,</v>
+        <v>768,</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F103" s="2">
-        <v>557</v>
+        <v>566</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C104" s="5">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D104" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>22,</v>
+        <v>23,</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F104" s="2">
-        <v>761</v>
+        <v>768</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C105" s="5">
         <f t="shared" si="5"/>
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="D105" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>758,</v>
+        <v>768,</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F105" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -3352,17 +3352,17 @@
       </c>
       <c r="C106" s="5">
         <f t="shared" si="5"/>
-        <v>1050</v>
+        <v>1057</v>
       </c>
       <c r="D106" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1050,</v>
+        <v>1057,</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F106" s="2">
-        <v>758</v>
+        <v>768</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -3371,17 +3371,17 @@
       </c>
       <c r="C107" s="5">
         <f t="shared" si="5"/>
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="D107" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>841,</v>
+        <v>846,</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F107" s="3">
-        <v>1050</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3390,17 +3390,17 @@
       </c>
       <c r="C108" s="5">
         <f t="shared" si="5"/>
-        <v>2248</v>
+        <v>2250</v>
       </c>
       <c r="D108" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2248,</v>
+        <v>2250,</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F108" s="2">
-        <v>841</v>
+        <v>846</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3409,17 +3409,17 @@
       </c>
       <c r="C109" s="5">
         <f t="shared" si="5"/>
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="D109" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>548,</v>
+        <v>552,</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F109" s="3">
-        <v>2248</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C110" s="5">
         <f t="shared" si="5"/>
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D110" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>417,</v>
+        <v>419,</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C111" s="5">
         <f t="shared" si="5"/>
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="D111" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>586,</v>
+        <v>591,</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F111" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="C112" s="5">
         <f t="shared" si="5"/>
-        <v>539</v>
+        <v>549</v>
       </c>
       <c r="D112" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>539,</v>
+        <v>549,</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F112" s="2">
-        <v>586</v>
+        <v>591</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C113" s="5">
         <f t="shared" si="5"/>
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="D113" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>358,</v>
+        <v>361,</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>110</v>
       </c>
       <c r="F113" s="2">
-        <v>539</v>
+        <v>549</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -3504,17 +3504,17 @@
       </c>
       <c r="C114" s="5">
         <f t="shared" si="5"/>
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D114" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>610,</v>
+        <v>611,</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F114" s="2">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="115" spans="2:6">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="C115" s="5">
         <f t="shared" si="5"/>
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="D115" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>509,</v>
+        <v>513,</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F115" s="2">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -3542,17 +3542,17 @@
       </c>
       <c r="C116" s="5">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="D116" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>300,</v>
+        <v>305,</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F116" s="2">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -3561,17 +3561,17 @@
       </c>
       <c r="C117" s="5">
         <f t="shared" si="5"/>
-        <v>1218</v>
+        <v>1220</v>
       </c>
       <c r="D117" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1218,</v>
+        <v>1220,</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
       <c r="F117" s="2">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3580,17 +3580,17 @@
       </c>
       <c r="C118" s="5">
         <f t="shared" si="5"/>
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="D118" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>678,</v>
+        <v>681,</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F118" s="3">
-        <v>1218</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C119" s="5">
         <f t="shared" si="5"/>
-        <v>1843</v>
+        <v>1865</v>
       </c>
       <c r="D119" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1843,</v>
+        <v>1865,</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F119" s="2">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3618,17 +3618,17 @@
       </c>
       <c r="C120" s="5">
         <f t="shared" si="5"/>
-        <v>896</v>
+        <v>908</v>
       </c>
       <c r="D120" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>896,</v>
+        <v>908,</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F120" s="3">
-        <v>1843</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -3637,17 +3637,17 @@
       </c>
       <c r="C121" s="5">
         <f t="shared" si="5"/>
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="D121" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>374,</v>
+        <v>380,</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F121" s="2">
-        <v>896</v>
+        <v>908</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="C122" s="5">
         <f t="shared" si="5"/>
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="D122" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>532,</v>
+        <v>540,</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F122" s="2">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3675,17 +3675,17 @@
       </c>
       <c r="C123" s="5">
         <f t="shared" si="5"/>
-        <v>1139</v>
+        <v>1159</v>
       </c>
       <c r="D123" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1139,</v>
+        <v>1159,</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F123" s="2">
-        <v>532</v>
+        <v>540</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="C124" s="5">
         <f t="shared" si="5"/>
-        <v>1223</v>
+        <v>1227</v>
       </c>
       <c r="D124" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1223,</v>
+        <v>1227,</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F124" s="3">
-        <v>1139</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C125" s="5">
         <f t="shared" si="5"/>
-        <v>2647</v>
+        <v>2677</v>
       </c>
       <c r="D125" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>2647,</v>
+        <v>2677,</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F125" s="3">
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -3732,17 +3732,17 @@
       </c>
       <c r="C126" s="5">
         <f t="shared" si="5"/>
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="D126" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>693,</v>
+        <v>697,</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F126" s="3">
-        <v>2647</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -3751,17 +3751,17 @@
       </c>
       <c r="C127" s="5">
         <f t="shared" si="5"/>
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="D127" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>384,</v>
+        <v>388,</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F127" s="2">
-        <v>693</v>
+        <v>697</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -3770,17 +3770,17 @@
       </c>
       <c r="C128" s="5">
         <f t="shared" si="5"/>
-        <v>489</v>
+        <v>504</v>
       </c>
       <c r="D128" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>489,</v>
+        <v>504,</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F128" s="2">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -3799,7 +3799,7 @@
         <v>126</v>
       </c>
       <c r="F129" s="2">
-        <v>489</v>
+        <v>504</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -3808,11 +3808,11 @@
       </c>
       <c r="C130" s="5">
         <f t="shared" si="5"/>
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D130" s="6" t="str">
         <f t="shared" ref="D130:D150" si="6">_xlfn.CONCAT(C130,",")</f>
-        <v>289,</v>
+        <v>292,</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>127</v>
@@ -3837,7 +3837,7 @@
         <v>128</v>
       </c>
       <c r="F131" s="2">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3846,11 +3846,11 @@
       </c>
       <c r="C132" s="5">
         <f t="shared" si="5"/>
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>607,</v>
+        <v>608,</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>129</v>
@@ -3865,17 +3865,17 @@
       </c>
       <c r="C133" s="5">
         <f t="shared" si="5"/>
-        <v>637</v>
+        <v>644</v>
       </c>
       <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>637,</v>
+        <v>644,</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F133" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3884,17 +3884,17 @@
       </c>
       <c r="C134" s="5">
         <f t="shared" si="5"/>
-        <v>572</v>
+        <v>581</v>
       </c>
       <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>572,</v>
+        <v>581,</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F134" s="2">
-        <v>637</v>
+        <v>644</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="C135" s="5">
         <f t="shared" si="5"/>
-        <v>1010</v>
+        <v>1021</v>
       </c>
       <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1010,</v>
+        <v>1021,</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F135" s="2">
-        <v>572</v>
+        <v>581</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -3922,17 +3922,17 @@
       </c>
       <c r="C136" s="5">
         <f t="shared" si="5"/>
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>731,</v>
+        <v>733,</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F136" s="3">
-        <v>1010</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="C137" s="5">
         <f t="shared" si="5"/>
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>942,</v>
+        <v>946,</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F137" s="2">
-        <v>731</v>
+        <v>733</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C138" s="5">
         <f t="shared" si="5"/>
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>649,</v>
+        <v>650,</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F138" s="2">
-        <v>942</v>
+        <v>946</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="C139" s="5">
         <f t="shared" si="5"/>
-        <v>1241</v>
+        <v>1255</v>
       </c>
       <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1241,</v>
+        <v>1255,</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F139" s="2">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -4008,7 +4008,7 @@
         <v>137</v>
       </c>
       <c r="F140" s="3">
-        <v>1241</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -4017,11 +4017,11 @@
       </c>
       <c r="C141" s="5">
         <f t="shared" si="5"/>
-        <v>1185</v>
+        <v>1211</v>
       </c>
       <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1185,</v>
+        <v>1211,</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>138</v>
@@ -4036,17 +4036,17 @@
       </c>
       <c r="C142" s="5">
         <f t="shared" si="5"/>
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>629,</v>
+        <v>631,</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F142" s="3">
-        <v>1185</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -4055,17 +4055,17 @@
       </c>
       <c r="C143" s="5">
         <f t="shared" si="5"/>
-        <v>818</v>
+        <v>828</v>
       </c>
       <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>818,</v>
+        <v>828,</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F143" s="2">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C144" s="5">
         <f t="shared" si="5"/>
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>465,</v>
+        <v>467,</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F144" s="2">
-        <v>818</v>
+        <v>828</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4093,17 +4093,17 @@
       </c>
       <c r="C145" s="5">
         <f t="shared" si="5"/>
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>261,</v>
+        <v>264,</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F145" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -4112,17 +4112,17 @@
       </c>
       <c r="C146" s="5">
         <f t="shared" si="5"/>
-        <v>1056</v>
+        <v>1067</v>
       </c>
       <c r="D146" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1056,</v>
+        <v>1067,</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F146" s="2">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -4131,17 +4131,17 @@
       </c>
       <c r="C147" s="5">
         <f t="shared" si="5"/>
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D147" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>397,</v>
+        <v>401,</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>144</v>
       </c>
       <c r="F147" s="3">
-        <v>1056</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -4150,17 +4150,17 @@
       </c>
       <c r="C148" s="5">
         <f t="shared" si="5"/>
-        <v>887</v>
+        <v>893</v>
       </c>
       <c r="D148" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>887,</v>
+        <v>893,</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F148" s="2">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -4169,17 +4169,17 @@
       </c>
       <c r="C149" s="5">
         <f t="shared" si="5"/>
-        <v>1201</v>
+        <v>1207</v>
       </c>
       <c r="D149" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>1201,</v>
+        <v>1207,</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F149" s="2">
-        <v>887</v>
+        <v>893</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -4188,17 +4188,17 @@
       </c>
       <c r="C150" s="5">
         <f t="shared" si="5"/>
-        <v>329</v>
+        <v>348</v>
       </c>
       <c r="D150" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>329,</v>
+        <v>348,</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F150" s="3">
-        <v>1201</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C151" s="5">
         <f>I9</f>
-        <v>5430</v>
+        <v>5502</v>
       </c>
       <c r="D151" s="6" t="str">
         <f>_xlfn.CONCAT(C151)</f>
-        <v>5430</v>
+        <v>5502</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F151" s="2">
-        <v>329</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>